<commit_message>
[Vinay] Added Water Management feature
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
@@ -5,24 +5,24 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="registeredUserDetails" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="ownerDetails" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="addressDetails" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="assessmentDetails" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="assessmentDetails" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="addressDetails" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="amenities" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="constructionTypeDetails" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="floorDetails" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="approvalDetails" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="propertyHeaderDetails" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="dataEntryPropertyHeader" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="applicantParticulars" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="connectionDetails" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="feeDetails" sheetId="13" state="visible" r:id="rId14"/>
-    <sheet name="searchDetails" sheetId="14" state="visible" r:id="rId15"/>
-    <sheet name="enclosedDocumentsDetails" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="applicantParticulars" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="connectionDetails" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="feeDetails" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="enclosedDocuments" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="vltReport" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="fieldInseptionDetailsForWaterConnection" sheetId="15" state="visible" r:id="rId16"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="170">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -51,9 +51,6 @@
     <t xml:space="preserve">juniorAssistant</t>
   </si>
   <si>
-    <t xml:space="preserve">944177</t>
-  </si>
-  <si>
     <t xml:space="preserve">kurnool_eGov@123</t>
   </si>
   <si>
@@ -81,12 +78,18 @@
     <t xml:space="preserve">0935528</t>
   </si>
   <si>
-    <t xml:space="preserve">Admin</t>
+    <t xml:space="preserve">admin</t>
   </si>
   <si>
     <t xml:space="preserve">egovernments</t>
   </si>
   <si>
+    <t xml:space="preserve">assistantEngineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0954568</t>
+  </si>
+  <si>
     <t xml:space="preserve">mobileNumber</t>
   </si>
   <si>
@@ -123,6 +126,27 @@
     <t xml:space="preserve">Ram</t>
   </si>
   <si>
+    <t xml:space="preserve">reasonForCreation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extentOfSite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">occupancyCertificateNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">registrationDocNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">registrationDocDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assessmentNewProperty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEW PROPERTY</t>
+  </si>
+  <si>
     <t xml:space="preserve">locality</t>
   </si>
   <si>
@@ -159,27 +183,6 @@
     <t xml:space="preserve">12/46</t>
   </si>
   <si>
-    <t xml:space="preserve">reasonForCreation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">extentOfSite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">occupancyCertificateNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">registrationDocNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">registrationDocDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assessmentNewProperty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NEW PROPERTY</t>
-  </si>
-  <si>
     <t xml:space="preserve">lift</t>
   </si>
   <si>
@@ -363,7 +366,13 @@
     <t xml:space="preserve">C.Naresh/ENG_Assistant Engineer_4</t>
   </si>
   <si>
-    <t xml:space="preserve">Forward to engineer</t>
+    <t xml:space="preserve">Forward to Engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">engineer1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A.P.Sreenivasulu/ENG_Assistant Engineer_1</t>
   </si>
   <si>
     <t xml:space="preserve">propertyType</t>
@@ -372,138 +381,181 @@
     <t xml:space="preserve">categoryOfOwnership</t>
   </si>
   <si>
+    <t xml:space="preserve">residentialPrivate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Residential</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Private</t>
+  </si>
+  <si>
     <t xml:space="preserve">assessmentNumber</t>
   </si>
   <si>
-    <t xml:space="preserve">residentialPrivate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Residential</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Private</t>
-  </si>
-  <si>
-    <t xml:space="preserve">karthik</t>
-  </si>
-  <si>
     <t xml:space="preserve">hscNumber</t>
   </si>
   <si>
     <t xml:space="preserve">connectionDate</t>
   </si>
   <si>
-    <t xml:space="preserve">applicantDetails</t>
+    <t xml:space="preserve">applicantInfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">applicantInfo1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/2_12.50</t>
   </si>
   <si>
     <t xml:space="preserve">waterSourceType</t>
   </si>
   <si>
+    <t xml:space="preserve">connectionType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">category</t>
+  </si>
+  <si>
     <t xml:space="preserve">usageType</t>
   </si>
   <si>
-    <t xml:space="preserve">connectionType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hscPipilineSize</t>
+    <t xml:space="preserve">hscPipeSize</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sumpCapacity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">noOfPersons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reasonForAdditionalConn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">connectionInfo</t>
   </si>
   <si>
     <t xml:space="preserve">1016 SURFACE WATER</t>
   </si>
   <si>
+    <t xml:space="preserve">Non-metered</t>
+  </si>
+  <si>
     <t xml:space="preserve">RESIDENTIALS</t>
   </si>
   <si>
-    <t xml:space="preserve">Non-metered</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GENERAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3/4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">monthlyFee</t>
+    <t xml:space="preserve">OYT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">connectionInfo1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Connection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">monthlyFees</t>
   </si>
   <si>
     <t xml:space="preserve">donationCharges</t>
   </si>
   <si>
-    <t xml:space="preserve">feeType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dataId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">searchValue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">searchWithAssessmentNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">searchWithDoorNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">searchWithMobileNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">searchWithZoneAndWardNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zone-1;Revenue Ward No 87</t>
-  </si>
-  <si>
-    <t xml:space="preserve">documentNum1</t>
+    <t xml:space="preserve">meterCost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meterName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meterSINo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">previousReading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lastReadingDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">currentReading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">feeInfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abcd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">documentNo1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">documentNo2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">documentNo3</t>
   </si>
   <si>
     <t xml:space="preserve">documentDate1</t>
   </si>
   <si>
-    <t xml:space="preserve">documentNum2</t>
-  </si>
-  <si>
     <t xml:space="preserve">documentDate2</t>
   </si>
   <si>
-    <t xml:space="preserve">documentNum3</t>
-  </si>
-  <si>
     <t xml:space="preserve">documentDate3</t>
   </si>
   <si>
-    <t xml:space="preserve">enclosedDocuments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">03/12/2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">04/12/2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K78</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05/12/2016</t>
+    <t xml:space="preserve">enclosedInfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03/12/16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fromDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">report1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06/12/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">material</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unitOfMeasurement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">existingDistributionPipeline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pipelineToHomeDistance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estimationCharges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inspectionInfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
-    <numFmt numFmtId="167" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="168" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -595,7 +647,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -616,6 +668,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -628,12 +688,28 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -714,19 +790,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.2666666666667"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.0148148148148"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.6555555555556"/>
-    <col collapsed="false" hidden="false" max="26" min="4" style="0" width="10.9740740740741"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="14.1111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.8740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.3185185185185"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.737037037037"/>
+    <col collapsed="false" hidden="false" max="26" min="4" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="13.8185185185185"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -755,11 +831,11 @@
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="1" t="n">
+        <v>944177</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="D2" s="2" t="n">
         <f aca="false">TRUE()</f>
@@ -776,13 +852,13 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="0" t="n">
         <f aca="false">TRUE()</f>
@@ -791,13 +867,13 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" s="0" t="n">
         <f aca="false">TRUE()</f>
@@ -806,13 +882,13 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="C5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" s="0" t="n">
         <f aca="false">FALSE()</f>
@@ -821,13 +897,13 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="C6" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" s="0" t="n">
         <f aca="false">FALSE()</f>
@@ -836,16 +912,29 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="5" t="b">
         <v>0</v>
       </c>
     </row>
@@ -865,56 +954,69 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.937037037037"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.537037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.4814814814815"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.7925925925926"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.52592592592593"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="16.6407407407407"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.5222222222222"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.1592592592593"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36296296296296"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="16.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>1234567890</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>115</v>
+        <v>1016093139</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>98765</v>
+      </c>
+      <c r="D2" s="10" t="n">
+        <v>42695</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>1016093127</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -924,56 +1026,129 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3666666666667"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.8740740740741"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.5037037037037"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.462962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.52592592592593"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.2333333333333"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.8037037037037"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.6037037037037"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.5888888888889"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.8037037037037"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.4111111111111"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="20.5703703703704"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.36296296296296"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="23.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>1016093139</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>123456</v>
-      </c>
-      <c r="D2" s="8" t="n">
-        <v>42659</v>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -983,75 +1158,90 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.9518518518519"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.2851851851852"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="17.1481481481481"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.9518518518519"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.52592592592593"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="12.1"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.5222222222222"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.8962962962963"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.9259259259259"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.1222222222222"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.5296296296296"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36296296296296"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>110</v>
+        <v>140</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>122</v>
+        <v>142</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="25.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>125</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>114</v>
+        <v>144</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>100</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>129</v>
+        <v>148</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>1234</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>123456</v>
+      </c>
+      <c r="H2" s="10" t="n">
+        <v>42689</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>123465</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -1061,49 +1251,77 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2296296296296"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7555555555556"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.1481481481481"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.52592592592593"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.1111111111111"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.4111111111111"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0074074074074"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6148148148148"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="13" width="15.7296296296296"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="15.1222222222222"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="13" width="14.8222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36296296296296"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>130</v>
+        <v>149</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>150</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>132</v>
+        <v>155</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>500</v>
+        <v>123</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>100</v>
+        <v>456</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>789</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -1113,58 +1331,40 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.5851851851852"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.7"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.3703703703704"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3185185185185"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="13.7111111111111"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="14.0185185185185"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36296296296296"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>134</v>
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="B2" s="9" t="n">
-        <v>1016093139</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>9878976543</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>139</v>
+        <v>159</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -1183,67 +1383,75 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.662962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9333333333333"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6333333333333"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.2296296296296"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.7481481481481"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="16.5407407407407"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36296296296296"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="14" width="12.1"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="14" width="10.6888888888889"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="15" width="8.77407407407407"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="15" width="18.4555555555556"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="15" width="6.85185185185185"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="15" width="22.1851851851852"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="14" width="20.9777777777778"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="15" width="17.7481481481481"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="14" width="8.36296296296296"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>145</v>
+    <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="A2" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>152</v>
+      <c r="C2" s="15" t="n">
+        <v>10</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="E2" s="15" t="n">
+        <v>100</v>
+      </c>
+      <c r="F2" s="15" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2" s="14" t="n">
+        <v>1000</v>
+      </c>
+      <c r="H2" s="15" t="n">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
@@ -1270,13 +1478,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.9740740740741"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.9148148148148"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.7592592592593"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.9740740740741"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.5592592592593"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.7777777777778"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.6222222222222"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.4666666666667"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1703703703704"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3851851851852"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.6814814814815"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1284,45 +1492,45 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>9878976543</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="5" t="s">
         <v>26</v>
       </c>
+      <c r="E2" s="7" t="s">
+        <v>27</v>
+      </c>
       <c r="F2" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1344,21 +1552,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.9740740740741"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.0925925925926"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="12.2481481481481"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.1296296296296"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.2481481481481"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.8518518518519"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.5592592592593"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.562962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.3814814814815"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.9333333333333"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.6814814814815"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1366,45 +1574,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>540037</v>
+      <c r="C2" s="0" t="n">
+        <v>5000</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>111</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>123</v>
+      </c>
+      <c r="F2" s="8" t="n">
+        <v>42350</v>
       </c>
     </row>
   </sheetData>
@@ -1423,21 +1625,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.3444444444444"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.9518518518519"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.8555555555556"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.9666666666667"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.262962962963"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.3259259259259"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.8962962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.9555555555556"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.0518518518519"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.4444444444444"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.737037037037"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.9555555555556"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.6814814814815"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1445,39 +1648,45 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>43</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="0" t="n">
-        <v>5000</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>111</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>123</v>
-      </c>
-      <c r="F2" s="6" t="n">
-        <v>42350</v>
+      <c r="G2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>540037</v>
       </c>
     </row>
   </sheetData>
@@ -1504,9 +1713,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="10.9740740740741"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.7"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.6814814814815"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1514,30 +1721,30 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" s="7" t="s">
         <v>49</v>
       </c>
+      <c r="C1" s="9" t="s">
+        <v>50</v>
+      </c>
       <c r="D1" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B2" s="0" t="n">
         <f aca="false">TRUE()</f>
@@ -1592,8 +1799,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.3444444444444"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.8518518518519"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.6814814814815"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1601,33 +1808,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1649,26 +1856,26 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.9740740740741"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.2481481481481"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.9703703703704"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.9148148148148"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="10.9740740740741"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.1111111111111"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.9740740740741"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.0518518518519"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.462962962963"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.56666666666667"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.74074074074074"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="24.3037037037037"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="21.262962962963"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="22.2444444444444"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.9555555555556"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.4814814814815"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6222222222222"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.8185185185185"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.5814814814815"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.6592592592593"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.37037037037037"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.64444444444445"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="23.7148148148148"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="10.6814814814815"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1676,78 +1883,78 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="6" t="n">
+        <v>25</v>
+      </c>
+      <c r="H2" s="8" t="n">
         <v>42653</v>
       </c>
-      <c r="I2" s="6" t="n">
+      <c r="I2" s="8" t="n">
         <v>42654</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K2" s="0" t="n">
         <v>10</v>
@@ -1756,9 +1963,9 @@
         <v>20</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="N2" s="6" t="n">
+        <v>87</v>
+      </c>
+      <c r="N2" s="8" t="n">
         <v>42358</v>
       </c>
       <c r="O2" s="0" t="n">
@@ -1781,20 +1988,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.0925925925926"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1074074074074"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.0111111111111"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.062962962963"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.1074074074074"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.7962962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.7185185185185"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.6185185185185"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.1814814814815"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.5185185185185"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.6814814814815"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1802,101 +2009,118 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C6" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="C7" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="E6" s="0" t="s">
-        <v>109</v>
+      <c r="D7" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1915,47 +2139,40 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.8925925925926"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.7333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4444444444444"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4037037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.6814814814815"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>1234567890</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Karthik] Modified create challan feature to introduce new steps
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="14"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="registeredUserDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="172">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t xml:space="preserve">0954568</t>
+  </si>
+  <si>
+    <t xml:space="preserve">seniorAssistant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">944186</t>
   </si>
   <si>
     <t xml:space="preserve">mobileNumber</t>
@@ -550,14 +556,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
     <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-    <numFmt numFmtId="168" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="169" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -594,12 +601,6 @@
       <name val="Menlo"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -647,7 +648,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -672,7 +673,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -688,15 +689,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -790,19 +783,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.8740740740741"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.3185185185185"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.737037037037"/>
-    <col collapsed="false" hidden="false" max="26" min="4" style="0" width="10.6814814814815"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="13.8185185185185"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.2666666666667"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.6"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.1296296296296"/>
+    <col collapsed="false" hidden="false" max="26" min="4" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="14.1111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -920,12 +913,13 @@
       <c r="C7" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="5" t="b">
+      <c r="D7" s="5" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -934,7 +928,22 @@
       <c r="C8" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="5" t="b">
+      <c r="D8" s="5" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="6" t="b">
         <v>0</v>
       </c>
     </row>
@@ -962,10 +971,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="16.6407407407407"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.5222222222222"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.1592592592593"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36296296296296"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="16.9518518518519"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.7962962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.52592592592593"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -973,18 +982,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1016093139</v>
@@ -998,7 +1007,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1016093127</v>
@@ -1034,71 +1043,71 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="20.6777777777778"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.2333333333333"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.8037037037037"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.6037037037037"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.5888888888889"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.8037037037037"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.4111111111111"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="20.5703703703704"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.36296296296296"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="21.1666666666667"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.5592592592593"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.2481481481481"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.7185185185185"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.0703703703704"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.52592592592593"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C1" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>125</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>123</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>20</v>
@@ -1112,25 +1121,25 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>135</v>
-      </c>
       <c r="E3" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>25</v>
@@ -1139,7 +1148,7 @@
         <v>4</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -1166,15 +1175,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="12.1"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.5222222222222"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.8962962962963"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.9259259259259"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.1222222222222"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.5296296296296"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36296296296296"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="12.3481481481481"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.7962962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.0518518518519"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.1518518518519"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2481481481481"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.4814814814815"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.8740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.52592592592593"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1182,33 +1191,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1000</v>
@@ -1220,7 +1229,7 @@
         <v>100</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>1234</v>
@@ -1259,14 +1268,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.1111111111111"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.4111111111111"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0074074074074"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6148148148148"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="13" width="15.7296296296296"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="15.1222222222222"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="13" width="14.8222222222222"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36296296296296"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.4259259259259"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7185185185185"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3259259259259"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.9148148148148"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="11" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="15.4814814814815"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="11" width="15.0925925925926"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.52592592592593"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1274,27 +1283,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="F1" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>154</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>123</v>
@@ -1305,14 +1314,14 @@
       <c r="D2" s="0" t="n">
         <v>789</v>
       </c>
-      <c r="E2" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>156</v>
+      <c r="E2" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -1339,32 +1348,32 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3185185185185"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="13.7111111111111"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="14.0185185185185"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36296296296296"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.6"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="11" width="14.0148148148148"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="14.3074074074074"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.52592592592593"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>158</v>
+      <c r="B1" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>160</v>
+        <v>161</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -1385,72 +1394,72 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="14" width="12.1"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="14" width="10.6888888888889"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="15" width="8.77407407407407"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="15" width="18.4555555555556"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="15" width="6.85185185185185"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="15" width="22.1851851851852"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="14" width="20.9777777777778"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="15" width="17.7481481481481"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="14" width="8.36296296296296"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="12" width="12.3481481481481"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="12" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="18.9111111111111"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="13" width="6.95925925925926"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="22.7333333333333"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="12" width="21.4592592592593"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="13" width="18.1296296296296"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="12" width="8.52592592592593"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="D1" s="15" t="s">
+      <c r="B1" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="C1" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="D1" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="E1" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="F1" s="13" t="s">
         <v>167</v>
       </c>
+      <c r="G1" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="C2" s="15" t="n">
+      <c r="A2" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" s="13" t="n">
         <v>10</v>
       </c>
-      <c r="D2" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="E2" s="15" t="n">
+      <c r="D2" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="E2" s="13" t="n">
         <v>100</v>
       </c>
-      <c r="F2" s="15" t="n">
+      <c r="F2" s="13" t="n">
         <v>10</v>
       </c>
-      <c r="G2" s="14" t="n">
+      <c r="G2" s="12" t="n">
         <v>1000</v>
       </c>
-      <c r="H2" s="15" t="n">
+      <c r="H2" s="13" t="n">
         <v>1000</v>
       </c>
     </row>
@@ -1478,13 +1487,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6814814814815"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.6222222222222"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.4666666666667"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.6814814814815"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1703703703704"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3851851851852"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.9148148148148"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.7592592592593"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.5592592592593"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.7777777777778"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.9740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1492,45 +1501,45 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>9878976543</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1560,13 +1569,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.8518518518519"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.5592592592593"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.562962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.3814814814815"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.7740740740741"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.9333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.3444444444444"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.9518518518519"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.8555555555556"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.9666666666667"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.262962962963"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.3259259259259"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.9740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1574,27 +1583,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>5000</v>
@@ -1633,14 +1642,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6814814814815"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.8962962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.9555555555556"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.0518518518519"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.4444444444444"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.737037037037"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.9555555555556"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.0925925925926"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="12.2481481481481"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.1296296296296"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.2481481481481"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.9740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1648,42 +1656,42 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>540037</v>
@@ -1713,7 +1721,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.9740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1721,30 +1729,30 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B2" s="0" t="n">
         <f aca="false">TRUE()</f>
@@ -1799,8 +1807,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.8518518518519"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.3444444444444"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.9740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1808,33 +1816,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1861,21 +1869,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6814814814815"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.9555555555556"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.4814814814815"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6222222222222"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="10.6814814814815"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.8185185185185"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.5814814814815"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.6592592592593"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.37037037037037"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.64444444444445"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="23.7148148148148"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="20.7740740740741"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="21.6555555555556"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.2481481481481"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.9703703703704"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.9148148148148"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.1111111111111"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.9740740740741"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.0518518518519"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.56666666666667"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.74074074074074"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="24.3037037037037"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="21.262962962963"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="22.2444444444444"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="10.9740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1883,69 +1891,69 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H2" s="8" t="n">
         <v>42653</v>
@@ -1954,7 +1962,7 @@
         <v>42654</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="K2" s="0" t="n">
         <v>10</v>
@@ -1963,7 +1971,7 @@
         <v>20</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="N2" s="8" t="n">
         <v>42358</v>
@@ -1996,12 +2004,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.7962962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.7185185185185"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.6185185185185"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.1814814814815"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.5185185185185"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.0925925925926"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1074074074074"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.0111111111111"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.062962962963"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.1074074074074"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.9740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2009,16 +2017,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2026,16 +2034,16 @@
         <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2043,16 +2051,16 @@
         <v>8</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2060,16 +2068,16 @@
         <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2077,50 +2085,50 @@
         <v>12</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D7" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>112</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2147,10 +2155,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4444444444444"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4037037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.8925925925926"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.9740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2158,21 +2166,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated data entry screen
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="registeredUserDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,539 +17,596 @@
     <sheet name="floorDetails" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="approvalDetails" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="propertyHeaderDetails" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="applicantParticulars" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="connectionDetails" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="feeDetails" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="enclosedDocuments" sheetId="13" state="visible" r:id="rId14"/>
-    <sheet name="vltReport" sheetId="14" state="visible" r:id="rId15"/>
-    <sheet name="fieldInseptionDetailsForWaterConnection" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="editAssessmentDetails" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="editFloorDetails" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="applicantParticulars" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="connectionDetails" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="feeDetails" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="enclosedDocuments" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="vltReport" sheetId="16" state="visible" r:id="rId17"/>
+    <sheet name="fieldInseptionDetailsForWaterConnection" sheetId="17" state="visible" r:id="rId18"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="172">
-  <si>
-    <t xml:space="preserve">dataName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hasZone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">juniorAssistant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kurnool_eGov@123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">billCollector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0944206</t>
-  </si>
-  <si>
-    <t xml:space="preserve">revenueInspector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">944210</t>
-  </si>
-  <si>
-    <t xml:space="preserve">revenueOfficer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">946800</t>
-  </si>
-  <si>
-    <t xml:space="preserve">commissioner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0935528</t>
-  </si>
-  <si>
-    <t xml:space="preserve">admin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">egovernments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assistantEngineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0954568</t>
-  </si>
-  <si>
-    <t xml:space="preserve">seniorAssistant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">944186</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mobileNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ownerName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">emailAddress</t>
-  </si>
-  <si>
-    <t xml:space="preserve">guardianRelation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">guardian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bimal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bimal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Male</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bimal@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Father</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ram</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reasonForCreation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">extentOfSite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">occupancyCertificateNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">registrationDocNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">registrationDocDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assessmentNewProperty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NEW PROPERTY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">locality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">zoneNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wardNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">blockNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">electionWard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">doorNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pincode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">addressOne</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4th colony</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zone-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Election Ward No. 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12/46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lift</t>
-  </si>
-  <si>
-    <t xml:space="preserve">toilets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">waterTap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">electricity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">attachedBathroom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">waterHarvesting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cableConnection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">all</t>
-  </si>
-  <si>
-    <t xml:space="preserve">floorType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">roofType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wallType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">woodType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">defaultConstructionType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Black Stones</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Absheet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BAMBOO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allmixing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">floorNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">classificationOfBuilding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">natureOfUsage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">firmName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">occupancy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">occupantName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">constructionDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">effectiveFromDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unstructuredLand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">length</t>
-  </si>
-  <si>
-    <t xml:space="preserve">breadth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">buildingPermissionNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">buildingPermissionDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plinthAreaInBuildingPlan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">firstFloor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1st floor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Huts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Residence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Owner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11/22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">approverDepartment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">approverDesignation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">approver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">approverRemarks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REVENUE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bill Collector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D.Khasim ~ REV_Bill Collector_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forward to bill collector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UD Revenue Inspector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P.Sadiq Hussain ~ UD RI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forward to revenue insoector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revenue Officer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B.Veeraswamy ~ REV_Revenue Officer_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forward to revenue officer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADMINISTRATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Commissioner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S.Ravindra Babu ~ ADM_Commissioner_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forward to commissioner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">engineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENGINEERING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assistant Engineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C.Naresh/ENG_Assistant Engineer_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forward to Engineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">engineer1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A.P.Sreenivasulu/ENG_Assistant Engineer_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">propertyType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">categoryOfOwnership</t>
-  </si>
-  <si>
-    <t xml:space="preserve">residentialPrivate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Residential</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Private</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assessmentNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hscNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">connectionDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">applicantInfo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">applicantInfo1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1/2_12.50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">waterSourceType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">connectionType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">usageType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hscPipeSize</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sumpCapacity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">noOfPersons</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reasonForAdditionalConn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">connectionInfo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1016 SURFACE WATER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-metered</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RESIDENTIALS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OYT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">connectionInfo1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New Connection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">monthlyFees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">donationCharges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">meterCost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">meterName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">meterSINo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">previousReading</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lastReadingDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">currentReading</t>
-  </si>
-  <si>
-    <t xml:space="preserve">feeInfo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abcd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">documentNo1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">documentNo2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">documentNo3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">documentDate1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">documentDate2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">documentDate3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">enclosedInfo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">03/12/16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fromDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">toDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">report1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06/12/2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">material</t>
-  </si>
-  <si>
-    <t xml:space="preserve">quantity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unitOfMeasurement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">existingDistributionPipeline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pipelineToHomeDistance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">estimationCharges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inspectionInfo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">m</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="192">
+  <si>
+    <t>dataName</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>hasZone</t>
+  </si>
+  <si>
+    <t>juniorAssistant</t>
+  </si>
+  <si>
+    <t>kurnool_eGov@123</t>
+  </si>
+  <si>
+    <t>billCollector</t>
+  </si>
+  <si>
+    <t>0944206</t>
+  </si>
+  <si>
+    <t>revenueInspector</t>
+  </si>
+  <si>
+    <t>944210</t>
+  </si>
+  <si>
+    <t>revenueOfficer</t>
+  </si>
+  <si>
+    <t>946800</t>
+  </si>
+  <si>
+    <t>commissioner</t>
+  </si>
+  <si>
+    <t>0935528</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>egovernments</t>
+  </si>
+  <si>
+    <t>assistantEngineer</t>
+  </si>
+  <si>
+    <t>0954568</t>
+  </si>
+  <si>
+    <t>seniorAssistant</t>
+  </si>
+  <si>
+    <t>944186</t>
+  </si>
+  <si>
+    <t>mobileNumber</t>
+  </si>
+  <si>
+    <t>ownerName</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>emailAddress</t>
+  </si>
+  <si>
+    <t>guardianRelation</t>
+  </si>
+  <si>
+    <t>guardian</t>
+  </si>
+  <si>
+    <t>bimal</t>
+  </si>
+  <si>
+    <t>Bimal</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Bimal@gmail.com</t>
+  </si>
+  <si>
+    <t>Father</t>
+  </si>
+  <si>
+    <t>Ram</t>
+  </si>
+  <si>
+    <t>reasonForCreation</t>
+  </si>
+  <si>
+    <t>extentOfSite</t>
+  </si>
+  <si>
+    <t>occupancyCertificateNumber</t>
+  </si>
+  <si>
+    <t>registrationDocNumber</t>
+  </si>
+  <si>
+    <t>registrationDocDate</t>
+  </si>
+  <si>
+    <t>assessmentNewProperty</t>
+  </si>
+  <si>
+    <t>NEW PROPERTY</t>
+  </si>
+  <si>
+    <t>locality</t>
+  </si>
+  <si>
+    <t>zoneNumber</t>
+  </si>
+  <si>
+    <t>wardNumber</t>
+  </si>
+  <si>
+    <t>blockNumber</t>
+  </si>
+  <si>
+    <t>electionWard</t>
+  </si>
+  <si>
+    <t>doorNumber</t>
+  </si>
+  <si>
+    <t>pincode</t>
+  </si>
+  <si>
+    <t>addressOne</t>
+  </si>
+  <si>
+    <t>4th colony</t>
+  </si>
+  <si>
+    <t>Zone-1</t>
+  </si>
+  <si>
+    <t>Election Ward No. 1</t>
+  </si>
+  <si>
+    <t>12/46</t>
+  </si>
+  <si>
+    <t>lift</t>
+  </si>
+  <si>
+    <t>toilets</t>
+  </si>
+  <si>
+    <t>waterTap</t>
+  </si>
+  <si>
+    <t>electricity</t>
+  </si>
+  <si>
+    <t>attachedBathroom</t>
+  </si>
+  <si>
+    <t>waterHarvesting</t>
+  </si>
+  <si>
+    <t>cableConnection</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>floorType</t>
+  </si>
+  <si>
+    <t>roofType</t>
+  </si>
+  <si>
+    <t>wallType</t>
+  </si>
+  <si>
+    <t>woodType</t>
+  </si>
+  <si>
+    <t>defaultConstructionType</t>
+  </si>
+  <si>
+    <t>Black Stones</t>
+  </si>
+  <si>
+    <t>Absheet</t>
+  </si>
+  <si>
+    <t>BAMBOO</t>
+  </si>
+  <si>
+    <t>Allmixing</t>
+  </si>
+  <si>
+    <t>floorNumber</t>
+  </si>
+  <si>
+    <t>classificationOfBuilding</t>
+  </si>
+  <si>
+    <t>natureOfUsage</t>
+  </si>
+  <si>
+    <t>firmName</t>
+  </si>
+  <si>
+    <t>occupancy</t>
+  </si>
+  <si>
+    <t>occupantName</t>
+  </si>
+  <si>
+    <t>constructionDate</t>
+  </si>
+  <si>
+    <t>effectiveFromDate</t>
+  </si>
+  <si>
+    <t>unstructuredLand</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>breadth</t>
+  </si>
+  <si>
+    <t>buildingPermissionNumber</t>
+  </si>
+  <si>
+    <t>buildingPermissionDate</t>
+  </si>
+  <si>
+    <t>plinthAreaInBuildingPlan</t>
+  </si>
+  <si>
+    <t>firstFloor</t>
+  </si>
+  <si>
+    <t>1st floor</t>
+  </si>
+  <si>
+    <t>Huts</t>
+  </si>
+  <si>
+    <t>Residence</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>11/22</t>
+  </si>
+  <si>
+    <t>approverDepartment</t>
+  </si>
+  <si>
+    <t>approverDesignation</t>
+  </si>
+  <si>
+    <t>approver</t>
+  </si>
+  <si>
+    <t>approverRemarks</t>
+  </si>
+  <si>
+    <t>REVENUE</t>
+  </si>
+  <si>
+    <t>Bill Collector</t>
+  </si>
+  <si>
+    <t>D.Khasim ~ REV_Bill Collector_1</t>
+  </si>
+  <si>
+    <t>Forward to bill collector</t>
+  </si>
+  <si>
+    <t>UD Revenue Inspector</t>
+  </si>
+  <si>
+    <t>P.Sadiq Hussain ~ UD RI</t>
+  </si>
+  <si>
+    <t>Forward to revenue insoector</t>
+  </si>
+  <si>
+    <t>Revenue Officer</t>
+  </si>
+  <si>
+    <t>B.Veeraswamy ~ REV_Revenue Officer_3</t>
+  </si>
+  <si>
+    <t>Forward to revenue officer</t>
+  </si>
+  <si>
+    <t>ADMINISTRATION</t>
+  </si>
+  <si>
+    <t>Commissioner</t>
+  </si>
+  <si>
+    <t>S.Ravindra Babu ~ ADM_Commissioner_1</t>
+  </si>
+  <si>
+    <t>Forward to commissioner</t>
+  </si>
+  <si>
+    <t>engineer</t>
+  </si>
+  <si>
+    <t>ENGINEERING</t>
+  </si>
+  <si>
+    <t>Assistant Engineer</t>
+  </si>
+  <si>
+    <t>C.Naresh/ENG_Assistant Engineer_4</t>
+  </si>
+  <si>
+    <t>Forward to Engineer</t>
+  </si>
+  <si>
+    <t>engineer1</t>
+  </si>
+  <si>
+    <t>A.P.Sreenivasulu/ENG_Assistant Engineer_1</t>
+  </si>
+  <si>
+    <t>propertyType</t>
+  </si>
+  <si>
+    <t>categoryOfOwnership</t>
+  </si>
+  <si>
+    <t>residentialPrivate</t>
+  </si>
+  <si>
+    <t>Residential</t>
+  </si>
+  <si>
+    <t>Private</t>
+  </si>
+  <si>
+    <t>assessmentAdditionProperty</t>
+  </si>
+  <si>
+    <t>editfloorNumber</t>
+  </si>
+  <si>
+    <t>editclassificationOfBuilding</t>
+  </si>
+  <si>
+    <t>editnatureOfUsage</t>
+  </si>
+  <si>
+    <t>editfirmName</t>
+  </si>
+  <si>
+    <t>editoccupancy</t>
+  </si>
+  <si>
+    <t>editoccupantName</t>
+  </si>
+  <si>
+    <t>editconstructionDate</t>
+  </si>
+  <si>
+    <t>editeffectiveFromDate</t>
+  </si>
+  <si>
+    <t>editunstructuredLand</t>
+  </si>
+  <si>
+    <t>editlength</t>
+  </si>
+  <si>
+    <t>editbreadth</t>
+  </si>
+  <si>
+    <t>editbuildingPermissionNumber</t>
+  </si>
+  <si>
+    <t>editbuildingPermissionDate</t>
+  </si>
+  <si>
+    <t>editplinthAreaInBuildingPlan</t>
+  </si>
+  <si>
+    <t>firstFloorAdditionaltaration</t>
+  </si>
+  <si>
+    <t>2nd Floor</t>
+  </si>
+  <si>
+    <t>Commercial</t>
+  </si>
+  <si>
+    <t>Sunil</t>
+  </si>
+  <si>
+    <t>33/22</t>
+  </si>
+  <si>
+    <t>assessmentNumber</t>
+  </si>
+  <si>
+    <t>hscNumber</t>
+  </si>
+  <si>
+    <t>connectionDate</t>
+  </si>
+  <si>
+    <t>applicantInfo</t>
+  </si>
+  <si>
+    <t>applicantInfo1</t>
+  </si>
+  <si>
+    <t>1/2_12.50</t>
+  </si>
+  <si>
+    <t>waterSourceType</t>
+  </si>
+  <si>
+    <t>connectionType</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>usageType</t>
+  </si>
+  <si>
+    <t>hscPipeSize</t>
+  </si>
+  <si>
+    <t>sumpCapacity</t>
+  </si>
+  <si>
+    <t>noOfPersons</t>
+  </si>
+  <si>
+    <t>reasonForAdditionalConn</t>
+  </si>
+  <si>
+    <t>connectionInfo</t>
+  </si>
+  <si>
+    <t>1016 SURFACE WATER</t>
+  </si>
+  <si>
+    <t>Non-metered</t>
+  </si>
+  <si>
+    <t>RESIDENTIALS</t>
+  </si>
+  <si>
+    <t>OYT</t>
+  </si>
+  <si>
+    <t>connectionInfo1</t>
+  </si>
+  <si>
+    <t>New Connection</t>
+  </si>
+  <si>
+    <t>monthlyFees</t>
+  </si>
+  <si>
+    <t>donationCharges</t>
+  </si>
+  <si>
+    <t>meterCost</t>
+  </si>
+  <si>
+    <t>meterName</t>
+  </si>
+  <si>
+    <t>meterSINo</t>
+  </si>
+  <si>
+    <t>previousReading</t>
+  </si>
+  <si>
+    <t>lastReadingDate</t>
+  </si>
+  <si>
+    <t>currentReading</t>
+  </si>
+  <si>
+    <t>feeInfo</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>documentNo1</t>
+  </si>
+  <si>
+    <t>documentNo2</t>
+  </si>
+  <si>
+    <t>documentNo3</t>
+  </si>
+  <si>
+    <t>documentDate1</t>
+  </si>
+  <si>
+    <t>documentDate2</t>
+  </si>
+  <si>
+    <t>documentDate3</t>
+  </si>
+  <si>
+    <t>enclosedInfo</t>
+  </si>
+  <si>
+    <t>03/12/16</t>
+  </si>
+  <si>
+    <t>fromDate</t>
+  </si>
+  <si>
+    <t>toDate</t>
+  </si>
+  <si>
+    <t>report1</t>
+  </si>
+  <si>
+    <t>06/12/2016</t>
+  </si>
+  <si>
+    <t>material</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>unitOfMeasurement</t>
+  </si>
+  <si>
+    <t>rate</t>
+  </si>
+  <si>
+    <t>existingDistributionPipeline</t>
+  </si>
+  <si>
+    <t>pipelineToHomeDistance</t>
+  </si>
+  <si>
+    <t>estimationCharges</t>
+  </si>
+  <si>
+    <t>inspectionInfo</t>
+  </si>
+  <si>
+    <t>m</t>
   </si>
 </sst>
 </file>
@@ -557,11 +614,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
     <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-    <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="168" formatCode="0.00"/>
     <numFmt numFmtId="169" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="6">
@@ -569,7 +626,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -592,7 +649,7 @@
       <sz val="12"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
-      <family val="0"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -648,12 +705,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -665,15 +722,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -689,11 +746,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -701,7 +758,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -785,8 +846,8 @@
   </sheetPr>
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -794,7 +855,8 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.2666666666667"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.6"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.1296296296296"/>
-    <col collapsed="false" hidden="false" max="26" min="4" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.0074074074074"/>
+    <col collapsed="false" hidden="false" max="26" min="5" style="0" width="10.9740740740741"/>
     <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="14.1111111111111"/>
   </cols>
   <sheetData>
@@ -824,7 +886,7 @@
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="4" t="n">
         <v>944177</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -834,7 +896,7 @@
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="E2" s="5"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
@@ -847,7 +909,7 @@
       <c r="A3" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -862,7 +924,7 @@
       <c r="A4" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -877,7 +939,7 @@
       <c r="A5" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -892,7 +954,7 @@
       <c r="A6" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -907,13 +969,13 @@
       <c r="A7" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="5" t="n">
+      <c r="D7" s="6" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -922,13 +984,13 @@
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="5" t="n">
+      <c r="D8" s="6" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -937,20 +999,21 @@
       <c r="A9" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="6" t="b">
+      <c r="D9" s="6" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -959,6 +1022,186 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.6111111111111"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1222222222222"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.8259259259259"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36296296296296"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>5000</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.7333333333333"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.1925925925926"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="8.36296296296296"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.6925925925926"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.4074074074074"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="8.36296296296296"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.8222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.36296296296296"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="H2" s="8" t="n">
+        <v>42319</v>
+      </c>
+      <c r="I2" s="8" t="n">
+        <v>42327</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="K2" s="10" t="n">
+        <v>10</v>
+      </c>
+      <c r="L2" s="10" t="n">
+        <v>20</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="N2" s="8" t="n">
+        <v>42358</v>
+      </c>
+      <c r="O2" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -982,18 +1225,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>122</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1016093139</v>
@@ -1001,13 +1244,13 @@
       <c r="C2" s="0" t="n">
         <v>98765</v>
       </c>
-      <c r="D2" s="10" t="n">
+      <c r="D2" s="11" t="n">
         <v>42695</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>124</v>
+        <v>144</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1016093127</v>
@@ -1022,7 +1265,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -1030,7 +1273,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1057,57 +1300,57 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>125</v>
+        <v>145</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>126</v>
+        <v>146</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>127</v>
+        <v>147</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>115</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>131</v>
+        <v>151</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>133</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>134</v>
+        <v>154</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>118</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>125</v>
+        <v>145</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>20</v>
@@ -1121,25 +1364,25 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>139</v>
+        <v>159</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>118</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>125</v>
+        <v>145</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>25</v>
@@ -1148,13 +1391,13 @@
         <v>4</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>140</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -1162,7 +1405,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1191,33 +1434,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>144</v>
+        <v>164</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>145</v>
+        <v>165</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>146</v>
+        <v>166</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>148</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1000</v>
@@ -1229,7 +1472,7 @@
         <v>100</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>150</v>
+        <v>170</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>1234</v>
@@ -1237,7 +1480,7 @@
       <c r="G2" s="0" t="n">
         <v>123456</v>
       </c>
-      <c r="H2" s="10" t="n">
+      <c r="H2" s="11" t="n">
         <v>42689</v>
       </c>
       <c r="I2" s="0" t="n">
@@ -1247,7 +1490,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -1255,7 +1498,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1272,9 +1515,9 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7185185185185"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3259259259259"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.9148148148148"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="11" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="15.4814814814815"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="11" width="15.0925925925926"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.4814814814815"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.0925925925926"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.52592592592593"/>
   </cols>
   <sheetData>
@@ -1283,27 +1526,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>151</v>
+        <v>171</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>152</v>
+        <v>172</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>155</v>
+        <v>173</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>156</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>157</v>
+        <v>177</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>123</v>
@@ -1314,20 +1557,20 @@
       <c r="D2" s="0" t="n">
         <v>789</v>
       </c>
-      <c r="E2" s="11" t="s">
-        <v>158</v>
+      <c r="E2" s="3" t="s">
+        <v>178</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>158</v>
+        <v>178</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>158</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -1335,7 +1578,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1349,8 +1592,8 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.6"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="11" width="14.0148148148148"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="14.3074074074074"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.0148148148148"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.3074074074074"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.52592592592593"/>
   </cols>
   <sheetData>
@@ -1358,28 +1601,28 @@
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>160</v>
+      <c r="B1" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>162</v>
+        <v>181</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -1387,7 +1630,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -1402,71 +1645,71 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="12" width="12.3481481481481"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="12" width="10.9740740740741"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="18.9111111111111"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="13" width="6.95925925925926"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="22.7333333333333"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="12" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="12" width="18.9111111111111"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="12" width="6.95925925925926"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="12" width="22.7333333333333"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="12" width="21.4592592592593"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="13" width="18.1296296296296"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="12" width="18.1296296296296"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="12" width="8.52592592592593"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>164</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>169</v>
+      <c r="B1" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="C2" s="13" t="n">
+      <c r="C2" s="14" t="n">
         <v>10</v>
       </c>
-      <c r="D2" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="E2" s="13" t="n">
+      <c r="D2" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E2" s="14" t="n">
         <v>100</v>
       </c>
-      <c r="F2" s="13" t="n">
+      <c r="F2" s="14" t="n">
         <v>10</v>
       </c>
-      <c r="G2" s="12" t="n">
+      <c r="G2" s="13" t="n">
         <v>1000</v>
       </c>
-      <c r="H2" s="13" t="n">
+      <c r="H2" s="14" t="n">
         <v>1000</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -1548,7 +1791,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1621,7 +1864,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1670,7 +1913,7 @@
       <c r="F1" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>44</v>
       </c>
       <c r="H1" s="0" t="s">
@@ -1690,7 +1933,7 @@
       <c r="F2" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="4" t="s">
         <v>50</v>
       </c>
       <c r="H2" s="0" t="n">
@@ -1700,7 +1943,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1786,7 +2029,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1848,7 +2091,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1864,7 +2107,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
@@ -1880,7 +2123,7 @@
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.462962962963"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.56666666666667"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.74074074074074"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="24.3037037037037"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="4" width="24.3037037037037"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="21.262962962963"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="22.2444444444444"/>
     <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="10.9740740740741"/>
@@ -1923,7 +2166,7 @@
       <c r="L1" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="4" t="s">
         <v>79</v>
       </c>
       <c r="N1" s="0" t="s">
@@ -1970,7 +2213,7 @@
       <c r="L2" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="4" t="s">
         <v>89</v>
       </c>
       <c r="N2" s="8" t="n">
@@ -1983,7 +2226,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2134,7 +2377,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2150,7 +2393,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
@@ -2186,7 +2429,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
[Vinay] Modified the Design & Added the PTReport feature
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="registeredUserDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,588 +25,603 @@
     <sheet name="enclosedDocuments" sheetId="15" state="visible" r:id="rId16"/>
     <sheet name="vltReport" sheetId="16" state="visible" r:id="rId17"/>
     <sheet name="fieldInseptionDetailsForWaterConnection" sheetId="17" state="visible" r:id="rId18"/>
+    <sheet name="ptReport" sheetId="18" state="visible" r:id="rId19"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="192">
-  <si>
-    <t>dataName</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>hasZone</t>
-  </si>
-  <si>
-    <t>juniorAssistant</t>
-  </si>
-  <si>
-    <t>kurnool_eGov@123</t>
-  </si>
-  <si>
-    <t>billCollector</t>
-  </si>
-  <si>
-    <t>0944206</t>
-  </si>
-  <si>
-    <t>revenueInspector</t>
-  </si>
-  <si>
-    <t>944210</t>
-  </si>
-  <si>
-    <t>revenueOfficer</t>
-  </si>
-  <si>
-    <t>946800</t>
-  </si>
-  <si>
-    <t>commissioner</t>
-  </si>
-  <si>
-    <t>0935528</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>egovernments</t>
-  </si>
-  <si>
-    <t>assistantEngineer</t>
-  </si>
-  <si>
-    <t>0954568</t>
-  </si>
-  <si>
-    <t>seniorAssistant</t>
-  </si>
-  <si>
-    <t>944186</t>
-  </si>
-  <si>
-    <t>mobileNumber</t>
-  </si>
-  <si>
-    <t>ownerName</t>
-  </si>
-  <si>
-    <t>gender</t>
-  </si>
-  <si>
-    <t>emailAddress</t>
-  </si>
-  <si>
-    <t>guardianRelation</t>
-  </si>
-  <si>
-    <t>guardian</t>
-  </si>
-  <si>
-    <t>bimal</t>
-  </si>
-  <si>
-    <t>Bimal</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>Bimal@gmail.com</t>
-  </si>
-  <si>
-    <t>Father</t>
-  </si>
-  <si>
-    <t>Ram</t>
-  </si>
-  <si>
-    <t>reasonForCreation</t>
-  </si>
-  <si>
-    <t>extentOfSite</t>
-  </si>
-  <si>
-    <t>occupancyCertificateNumber</t>
-  </si>
-  <si>
-    <t>registrationDocNumber</t>
-  </si>
-  <si>
-    <t>registrationDocDate</t>
-  </si>
-  <si>
-    <t>assessmentNewProperty</t>
-  </si>
-  <si>
-    <t>NEW PROPERTY</t>
-  </si>
-  <si>
-    <t>locality</t>
-  </si>
-  <si>
-    <t>zoneNumber</t>
-  </si>
-  <si>
-    <t>wardNumber</t>
-  </si>
-  <si>
-    <t>blockNumber</t>
-  </si>
-  <si>
-    <t>electionWard</t>
-  </si>
-  <si>
-    <t>doorNumber</t>
-  </si>
-  <si>
-    <t>pincode</t>
-  </si>
-  <si>
-    <t>addressOne</t>
-  </si>
-  <si>
-    <t>4th colony</t>
-  </si>
-  <si>
-    <t>Zone-1</t>
-  </si>
-  <si>
-    <t>Election Ward No. 1</t>
-  </si>
-  <si>
-    <t>12/46</t>
-  </si>
-  <si>
-    <t>lift</t>
-  </si>
-  <si>
-    <t>toilets</t>
-  </si>
-  <si>
-    <t>waterTap</t>
-  </si>
-  <si>
-    <t>electricity</t>
-  </si>
-  <si>
-    <t>attachedBathroom</t>
-  </si>
-  <si>
-    <t>waterHarvesting</t>
-  </si>
-  <si>
-    <t>cableConnection</t>
-  </si>
-  <si>
-    <t>all</t>
-  </si>
-  <si>
-    <t>floorType</t>
-  </si>
-  <si>
-    <t>roofType</t>
-  </si>
-  <si>
-    <t>wallType</t>
-  </si>
-  <si>
-    <t>woodType</t>
-  </si>
-  <si>
-    <t>defaultConstructionType</t>
-  </si>
-  <si>
-    <t>Black Stones</t>
-  </si>
-  <si>
-    <t>Absheet</t>
-  </si>
-  <si>
-    <t>BAMBOO</t>
-  </si>
-  <si>
-    <t>Allmixing</t>
-  </si>
-  <si>
-    <t>floorNumber</t>
-  </si>
-  <si>
-    <t>classificationOfBuilding</t>
-  </si>
-  <si>
-    <t>natureOfUsage</t>
-  </si>
-  <si>
-    <t>firmName</t>
-  </si>
-  <si>
-    <t>occupancy</t>
-  </si>
-  <si>
-    <t>occupantName</t>
-  </si>
-  <si>
-    <t>constructionDate</t>
-  </si>
-  <si>
-    <t>effectiveFromDate</t>
-  </si>
-  <si>
-    <t>unstructuredLand</t>
-  </si>
-  <si>
-    <t>length</t>
-  </si>
-  <si>
-    <t>breadth</t>
-  </si>
-  <si>
-    <t>buildingPermissionNumber</t>
-  </si>
-  <si>
-    <t>buildingPermissionDate</t>
-  </si>
-  <si>
-    <t>plinthAreaInBuildingPlan</t>
-  </si>
-  <si>
-    <t>firstFloor</t>
-  </si>
-  <si>
-    <t>1st floor</t>
-  </si>
-  <si>
-    <t>Huts</t>
-  </si>
-  <si>
-    <t>Residence</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>Owner</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>11/22</t>
-  </si>
-  <si>
-    <t>approverDepartment</t>
-  </si>
-  <si>
-    <t>approverDesignation</t>
-  </si>
-  <si>
-    <t>approver</t>
-  </si>
-  <si>
-    <t>approverRemarks</t>
-  </si>
-  <si>
-    <t>REVENUE</t>
-  </si>
-  <si>
-    <t>Bill Collector</t>
-  </si>
-  <si>
-    <t>D.Khasim ~ REV_Bill Collector_1</t>
-  </si>
-  <si>
-    <t>Forward to bill collector</t>
-  </si>
-  <si>
-    <t>UD Revenue Inspector</t>
-  </si>
-  <si>
-    <t>P.Sadiq Hussain ~ UD RI</t>
-  </si>
-  <si>
-    <t>Forward to revenue insoector</t>
-  </si>
-  <si>
-    <t>Revenue Officer</t>
-  </si>
-  <si>
-    <t>B.Veeraswamy ~ REV_Revenue Officer_3</t>
-  </si>
-  <si>
-    <t>Forward to revenue officer</t>
-  </si>
-  <si>
-    <t>ADMINISTRATION</t>
-  </si>
-  <si>
-    <t>Commissioner</t>
-  </si>
-  <si>
-    <t>S.Ravindra Babu ~ ADM_Commissioner_1</t>
-  </si>
-  <si>
-    <t>Forward to commissioner</t>
-  </si>
-  <si>
-    <t>engineer</t>
-  </si>
-  <si>
-    <t>ENGINEERING</t>
-  </si>
-  <si>
-    <t>Assistant Engineer</t>
-  </si>
-  <si>
-    <t>C.Naresh/ENG_Assistant Engineer_4</t>
-  </si>
-  <si>
-    <t>Forward to Engineer</t>
-  </si>
-  <si>
-    <t>engineer1</t>
-  </si>
-  <si>
-    <t>A.P.Sreenivasulu/ENG_Assistant Engineer_1</t>
-  </si>
-  <si>
-    <t>propertyType</t>
-  </si>
-  <si>
-    <t>categoryOfOwnership</t>
-  </si>
-  <si>
-    <t>residentialPrivate</t>
-  </si>
-  <si>
-    <t>Residential</t>
-  </si>
-  <si>
-    <t>Private</t>
-  </si>
-  <si>
-    <t>assessmentAdditionProperty</t>
-  </si>
-  <si>
-    <t>editfloorNumber</t>
-  </si>
-  <si>
-    <t>editclassificationOfBuilding</t>
-  </si>
-  <si>
-    <t>editnatureOfUsage</t>
-  </si>
-  <si>
-    <t>editfirmName</t>
-  </si>
-  <si>
-    <t>editoccupancy</t>
-  </si>
-  <si>
-    <t>editoccupantName</t>
-  </si>
-  <si>
-    <t>editconstructionDate</t>
-  </si>
-  <si>
-    <t>editeffectiveFromDate</t>
-  </si>
-  <si>
-    <t>editunstructuredLand</t>
-  </si>
-  <si>
-    <t>editlength</t>
-  </si>
-  <si>
-    <t>editbreadth</t>
-  </si>
-  <si>
-    <t>editbuildingPermissionNumber</t>
-  </si>
-  <si>
-    <t>editbuildingPermissionDate</t>
-  </si>
-  <si>
-    <t>editplinthAreaInBuildingPlan</t>
-  </si>
-  <si>
-    <t>firstFloorAdditionaltaration</t>
-  </si>
-  <si>
-    <t>2nd Floor</t>
-  </si>
-  <si>
-    <t>Commercial</t>
-  </si>
-  <si>
-    <t>Sunil</t>
-  </si>
-  <si>
-    <t>33/22</t>
-  </si>
-  <si>
-    <t>assessmentNumber</t>
-  </si>
-  <si>
-    <t>hscNumber</t>
-  </si>
-  <si>
-    <t>connectionDate</t>
-  </si>
-  <si>
-    <t>applicantInfo</t>
-  </si>
-  <si>
-    <t>applicantInfo1</t>
-  </si>
-  <si>
-    <t>1/2_12.50</t>
-  </si>
-  <si>
-    <t>waterSourceType</t>
-  </si>
-  <si>
-    <t>connectionType</t>
-  </si>
-  <si>
-    <t>category</t>
-  </si>
-  <si>
-    <t>usageType</t>
-  </si>
-  <si>
-    <t>hscPipeSize</t>
-  </si>
-  <si>
-    <t>sumpCapacity</t>
-  </si>
-  <si>
-    <t>noOfPersons</t>
-  </si>
-  <si>
-    <t>reasonForAdditionalConn</t>
-  </si>
-  <si>
-    <t>connectionInfo</t>
-  </si>
-  <si>
-    <t>1016 SURFACE WATER</t>
-  </si>
-  <si>
-    <t>Non-metered</t>
-  </si>
-  <si>
-    <t>RESIDENTIALS</t>
-  </si>
-  <si>
-    <t>OYT</t>
-  </si>
-  <si>
-    <t>connectionInfo1</t>
-  </si>
-  <si>
-    <t>New Connection</t>
-  </si>
-  <si>
-    <t>monthlyFees</t>
-  </si>
-  <si>
-    <t>donationCharges</t>
-  </si>
-  <si>
-    <t>meterCost</t>
-  </si>
-  <si>
-    <t>meterName</t>
-  </si>
-  <si>
-    <t>meterSINo</t>
-  </si>
-  <si>
-    <t>previousReading</t>
-  </si>
-  <si>
-    <t>lastReadingDate</t>
-  </si>
-  <si>
-    <t>currentReading</t>
-  </si>
-  <si>
-    <t>feeInfo</t>
-  </si>
-  <si>
-    <t>abcd</t>
-  </si>
-  <si>
-    <t>documentNo1</t>
-  </si>
-  <si>
-    <t>documentNo2</t>
-  </si>
-  <si>
-    <t>documentNo3</t>
-  </si>
-  <si>
-    <t>documentDate1</t>
-  </si>
-  <si>
-    <t>documentDate2</t>
-  </si>
-  <si>
-    <t>documentDate3</t>
-  </si>
-  <si>
-    <t>enclosedInfo</t>
-  </si>
-  <si>
-    <t>03/12/16</t>
-  </si>
-  <si>
-    <t>fromDate</t>
-  </si>
-  <si>
-    <t>toDate</t>
-  </si>
-  <si>
-    <t>report1</t>
-  </si>
-  <si>
-    <t>06/12/2016</t>
-  </si>
-  <si>
-    <t>material</t>
-  </si>
-  <si>
-    <t>quantity</t>
-  </si>
-  <si>
-    <t>unitOfMeasurement</t>
-  </si>
-  <si>
-    <t>rate</t>
-  </si>
-  <si>
-    <t>existingDistributionPipeline</t>
-  </si>
-  <si>
-    <t>pipelineToHomeDistance</t>
-  </si>
-  <si>
-    <t>estimationCharges</t>
-  </si>
-  <si>
-    <t>inspectionInfo</t>
-  </si>
-  <si>
-    <t>m</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="195">
+  <si>
+    <t xml:space="preserve">dataName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hasZone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">juniorAssistant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kurnool_eGov@123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">billCollector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0944206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">revenueInspector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">944210</t>
+  </si>
+  <si>
+    <t xml:space="preserve">revenueOfficer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">946800</t>
+  </si>
+  <si>
+    <t xml:space="preserve">commissioner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0935528</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">egovernments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assistantEngineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0954568</t>
+  </si>
+  <si>
+    <t xml:space="preserve">seniorAssistant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">944186</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mobileNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ownerName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emailAddress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">guardianRelation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">guardian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bimal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bimal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bimal@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Father</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reasonForCreation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extentOfSite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">occupancyCertificateNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">registrationDocNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">registrationDocDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assessmentNewProperty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEW PROPERTY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">locality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zoneNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wardNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blockNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">electionWard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">doorNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pincode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addressOne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4th colony</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zone-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Election Ward No. 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12/46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lift</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toilets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">waterTap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">electricity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">attachedBathroom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">waterHarvesting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cableConnection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">floorType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">roofType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wallType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">woodType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">defaultConstructionType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Black Stones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAMBOO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allmixing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">floorNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">classificationOfBuilding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">natureOfUsage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">firmName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">occupancy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">occupantName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">constructionDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">effectiveFromDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unstructuredLand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">breadth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buildingPermissionNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buildingPermissionDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plinthAreaInBuildingPlan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">firstFloor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1st floor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Residence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Owner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11/22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">approverDepartment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">approverDesignation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">approver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">approverRemarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REVENUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bill Collector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D.Khasim ~ REV_Bill Collector_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forward to bill collector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UD Revenue Inspector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P.Sadiq Hussain ~ UD RI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forward to revenue insoector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revenue Officer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B.Veeraswamy ~ REV_Revenue Officer_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forward to revenue officer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADMINISTRATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commissioner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S.Ravindra Babu ~ ADM_Commissioner_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forward to commissioner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENGINEERING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assistant Engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C.Naresh/ENG_Assistant Engineer_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forward to Engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">engineer1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A.P.Sreenivasulu/ENG_Assistant Engineer_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">propertyType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">categoryOfOwnership</t>
+  </si>
+  <si>
+    <t xml:space="preserve">residentialPrivate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Residential</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Private</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assessmentAdditionProperty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editfloorNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editclassificationOfBuilding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editnatureOfUsage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editfirmName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editoccupancy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editoccupantName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editconstructionDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editeffectiveFromDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editunstructuredLand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editlength</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editbreadth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editbuildingPermissionNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editbuildingPermissionDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editplinthAreaInBuildingPlan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">firstFloorAdditionaltaration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2nd Floor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commercial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sunil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33/22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assessmentNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hscNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">connectionDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">applicantInfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">applicantInfo1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/2_12.50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">waterSourceType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">connectionType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">usageType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hscPipeSize</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sumpCapacity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">noOfPersons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reasonForAdditionalConn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">connectionInfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1016 SURFACE WATER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-metered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESIDENTIALS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OYT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">connectionInfo1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Connection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">monthlyFees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">donationCharges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meterCost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meterName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meterSINo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">previousReading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lastReadingDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">currentReading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">feeInfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abcd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">documentNo1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">documentNo2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">documentNo3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">documentDate1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">documentDate2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">documentDate3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enclosedInfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03/12/16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fromDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">report1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06/12/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">material</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unitOfMeasurement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">existingDistributionPipeline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pipelineToHomeDistance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estimationCharges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inspectionInfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">report2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07/12/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10/12/2016</t>
   </si>
 </sst>
 </file>
@@ -614,7 +629,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
     <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
@@ -705,7 +720,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -764,6 +779,10 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -847,17 +866,17 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.2666666666667"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.6"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.1296296296296"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.0074074074074"/>
-    <col collapsed="false" hidden="false" max="26" min="5" style="0" width="10.9740740740741"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="14.1111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6592592592593"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.5222222222222"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3259259259259"/>
+    <col collapsed="false" hidden="false" max="26" min="5" style="0" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="14.4037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1013,7 +1032,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1034,10 +1053,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.6111111111111"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1222222222222"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.8259259259259"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36296296296296"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.1851851851852"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.4814814814815"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.437037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.52592592592593"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1065,7 +1084,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -1080,20 +1099,20 @@
   </sheetPr>
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.7333333333333"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.1925925925926"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="8.36296296296296"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.6925925925926"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.4074074074074"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="8.36296296296296"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.8222222222222"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.36296296296296"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.4185185185185"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.4666666666667"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="8.52592592592593"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.9555555555556"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="8.52592592592593"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.0925925925926"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.52592592592593"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1193,7 +1212,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -1214,10 +1233,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="16.9518518518519"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.7962962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.6962962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.52592592592593"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.0925925925926"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.1851851851852"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1265,7 +1284,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -1286,16 +1305,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="21.1666666666667"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.5592592592593"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.837037037037"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.7777777777778"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.2481481481481"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.7185185185185"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.0703703703704"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.52592592592593"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.9518518518519"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.4259259259259"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.4444444444444"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.4259259259259"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.0148148148148"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.5592592592593"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1397,7 +1416,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -1418,15 +1437,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="12.3481481481481"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.7962962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.0518518518519"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.1518518518519"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2481481481481"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.4814814814815"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.8740740740741"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.52592592592593"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="12.5444444444444"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.0925925925926"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2481481481481"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.3481481481481"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4444444444444"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.8740740740741"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.2666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1490,7 +1509,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -1511,14 +1530,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.4259259259259"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7185185185185"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3259259259259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.9148148148148"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.4814814814815"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.0925925925926"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.52592592592593"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7185185185185"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.0148148148148"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.6222222222222"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.2074074074074"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.8740740740741"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.4814814814815"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1570,7 +1589,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -1591,10 +1610,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.6"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.0148148148148"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.52592592592593"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3074074074074"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.6"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1622,7 +1641,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -1643,15 +1662,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="12" width="12.3481481481481"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="12" width="10.9740740740741"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="12" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="12" width="18.9111111111111"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="12" width="6.95925925925926"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="12" width="22.7333333333333"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="12" width="21.4592592592593"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="12" width="18.1296296296296"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="12" width="8.52592592592593"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="12" width="12.5444444444444"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="12" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="12" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="12" width="19.3037037037037"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="12" width="7.15185185185185"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="12" width="23.2259259259259"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="12" width="22.0481481481481"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="12" width="18.5222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="12" width="8.62222222222222"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1709,7 +1728,59 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.4962962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="15" width="12.2037037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="15" width="11.1925925925926"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36296296296296"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>194</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -1730,13 +1801,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.9740740740741"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.9148148148148"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.7592592592593"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.9740740740741"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.5592592592593"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.7777777777778"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.2074074074074"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.0518518518519"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.9518518518519"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.1703703703704"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.2703703703704"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1791,7 +1862,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1812,13 +1883,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.3444444444444"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.9518518518519"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.8555555555556"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.9666666666667"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.262962962963"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.3259259259259"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8333333333333"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.1518518518519"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.6555555555556"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.8518518518519"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.7185185185185"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.2703703703704"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1864,7 +1935,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1885,13 +1956,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.9740740740741"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.0925925925926"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="12.2481481481481"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.1296296296296"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.2481481481481"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.2888888888889"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="12.4444444444444"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.5222222222222"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.4444444444444"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.2703703703704"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1943,7 +2014,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1964,7 +2035,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.2703703703704"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2029,7 +2100,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2050,8 +2121,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.3444444444444"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8333333333333"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.2703703703704"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2091,7 +2162,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2112,21 +2183,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.9740740740741"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.2481481481481"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.9703703703704"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.9148148148148"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="10.9740740740741"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.1111111111111"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.9740740740741"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.0518518518519"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.462962962963"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.56666666666667"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.74074074074074"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="4" width="24.3037037037037"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="21.262962962963"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="22.2444444444444"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4444444444444"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.4592592592593"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.2074074074074"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.4037037037037"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.3666666666667"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.3444444444444"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.8555555555556"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.76296296296296"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.84074074074074"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="4" width="24.8888888888889"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="21.8518518518519"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="22.7333333333333"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="11.2703703703704"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2226,7 +2297,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2247,12 +2318,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.0925925925926"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1074074074074"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.0111111111111"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.062962962963"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.1074074074074"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.4814814814815"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.5"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4037037037037"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.9444444444444"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.6962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.2703703703704"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2377,7 +2448,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2398,10 +2469,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.8925925925926"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.3814814814815"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.2703703703704"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2429,7 +2500,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
[Vinay] Completed the additional water connection feature upto 3 transfers
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="17"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="registeredUserDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -865,18 +865,18 @@
   </sheetPr>
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6592592592593"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.8962962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.5222222222222"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3259259259259"/>
-    <col collapsed="false" hidden="false" max="26" min="5" style="0" width="11.2703703703704"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="14.4037037037037"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0518518518519"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.9111111111111"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6222222222222"/>
+    <col collapsed="false" hidden="false" max="26" min="5" style="0" width="11.562962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="14.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1053,10 +1053,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.1851851851852"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.4814814814815"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.437037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.52592592592593"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.7740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.8740740740741"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.0259259259259"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1105,14 +1105,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.4185185185185"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.4666666666667"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="8.52592592592593"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.9555555555556"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="8.52592592592593"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.0925925925926"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.52592592592593"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.1037037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.7592592592593"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.2481481481481"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.4814814814815"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1227,16 +1227,16 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.0925925925926"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.4814814814815"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.81851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1272,7 +1272,7 @@
         <v>144</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>1016093127</v>
+        <v>1016093140</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>0</v>
@@ -1305,16 +1305,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="21.6555555555556"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.9518518518519"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.4259259259259"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.0740740740741"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.4444444444444"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.4259259259259"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.0148148148148"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.5592592592593"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="22.2444444444444"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7185185185185"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.4259259259259"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.3666666666667"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.7185185185185"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.3074074074074"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.1481481481481"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.81851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1437,15 +1437,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="12.5444444444444"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.0925925925926"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.2481481481481"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.3481481481481"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4444444444444"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.8740740740741"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.2666666666667"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="12.7407407407407"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.4814814814815"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4444444444444"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.5444444444444"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.2666666666667"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.6592592592593"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.81851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1530,14 +1530,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7185185185185"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.0148148148148"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.6222222222222"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.2074074074074"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.462962962963"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.8740740740741"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.4814814814815"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0148148148148"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3074074074074"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.9148148148148"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5037037037037"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.8555555555556"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.2666666666667"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.8740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.81851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1610,10 +1610,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8962962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.6"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.6"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.81851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1662,15 +1662,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="12" width="12.5444444444444"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="12" width="11.2703703703704"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="12" width="9.21111111111111"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="12" width="19.3037037037037"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="12" width="7.15185185185185"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="12" width="23.2259259259259"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="12" width="22.0481481481481"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="12" width="18.5222222222222"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="12" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="12" width="12.7407407407407"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="12" width="11.562962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="12" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="12" width="19.7962962962963"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="12" width="7.25185185185185"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="12" width="23.7148148148148"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="12" width="22.537037037037"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="12" width="18.9111111111111"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="12" width="8.81851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1743,16 +1743,16 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.4962962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="15" width="12.2037037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="15" width="11.1925925925926"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36296296296296"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.7592592592593"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="15" width="12.4444444444444"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="15" width="11.4666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.52592592592593"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1801,13 +1801,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.2703703703704"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.2074074074074"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.0518518518519"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.2703703703704"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.9518518518519"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.1703703703704"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.562962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.5037037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.2481481481481"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.562962962963"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.5592592592593"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.562962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1883,13 +1883,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8333333333333"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.1518518518519"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.6555555555556"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.8518518518519"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.7185185185185"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.3222222222222"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.3481481481481"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.3407407407407"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.3444444444444"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.1074074074074"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.562962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1956,13 +1956,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.2703703703704"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.2888888888889"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="12.4444444444444"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.837037037037"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.5222222222222"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.4444444444444"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.562962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.4851851851852"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.9111111111111"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.562962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2035,7 +2035,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.562962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2121,8 +2121,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.3222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.562962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2183,21 +2183,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.2703703703704"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4444444444444"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.4592592592593"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.2074074074074"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="11.2703703703704"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.4037037037037"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.3666666666667"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.3444444444444"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.8555555555556"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.76296296296296"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.84074074074074"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="4" width="24.8888888888889"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="21.8518518518519"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="22.7333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.562962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.0481481481481"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5037037037037"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="11.562962962963"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.7"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.7555555555556"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.737037037037"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.95925925925926"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="7.93703703703704"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="4" width="25.4777777777778"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="22.3444444444444"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.2259259259259"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="11.562962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2318,12 +2318,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.4814814814815"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.5"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4037037037037"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.9444444444444"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.6962962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.8740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.9925925925926"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.8925925925926"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.8259259259259"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.2814814814815"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.562962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2469,10 +2469,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.462962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.837037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.3814814814815"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.8555555555556"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.8740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.562962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[Vinay] Completed the DailyCollectionReport Feature
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="registeredUserDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,6 +25,7 @@
     <sheet name="enclosedDocuments" sheetId="15" state="visible" r:id="rId16"/>
     <sheet name="vltReport" sheetId="16" state="visible" r:id="rId17"/>
     <sheet name="fieldInseptionDetailsForWaterConnection" sheetId="17" state="visible" r:id="rId18"/>
+    <sheet name="ptReport" sheetId="18" state="visible" r:id="rId19"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="195">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -98,9 +99,6 @@
     <t xml:space="preserve">944186</t>
   </si>
   <si>
-    <t xml:space="preserve">adm_manager</t>
-  </si>
-  <si>
     <t xml:space="preserve">mobileNumber</t>
   </si>
   <si>
@@ -615,6 +613,15 @@
   </si>
   <si>
     <t xml:space="preserve">m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">report2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07/12/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10/12/2016</t>
   </si>
 </sst>
 </file>
@@ -713,7 +720,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -772,6 +779,10 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -852,10 +863,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L65536"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1018,26 +1029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="1" t="n">
-        <v>944168</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="6" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C10" r:id="rId1" display="kurnool_eGov@123"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1072,15 +1064,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>34</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>5000</v>
@@ -1107,7 +1099,7 @@
   </sheetPr>
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -1128,69 +1120,69 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="J1" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="K1" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="L1" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="M1" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="O1" s="0" t="s">
         <v>134</v>
-      </c>
-      <c r="O1" s="0" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>138</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>139</v>
       </c>
       <c r="H2" s="8" t="n">
         <v>42319</v>
@@ -1199,7 +1191,7 @@
         <v>42327</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K2" s="10" t="n">
         <v>10</v>
@@ -1208,7 +1200,7 @@
         <v>20</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N2" s="8" t="n">
         <v>42358</v>
@@ -1236,7 +1228,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1252,18 +1244,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>141</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>142</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1016093139</v>
@@ -1277,10 +1269,10 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>1016093127</v>
+        <v>1016093140</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>0</v>
@@ -1327,57 +1319,57 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C1" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="D1" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="J1" s="0" t="s">
         <v>153</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>155</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>159</v>
-      </c>
       <c r="F2" s="0" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>20</v>
@@ -1391,25 +1383,25 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>159</v>
-      </c>
       <c r="F3" s="0" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>25</v>
@@ -1418,7 +1410,7 @@
         <v>4</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -1461,33 +1453,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>163</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>164</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>167</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>168</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1000</v>
@@ -1499,7 +1491,7 @@
         <v>100</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>1234</v>
@@ -1553,27 +1545,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>172</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>173</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>176</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>123</v>
@@ -1585,13 +1577,13 @@
         <v>789</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -1629,21 +1621,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>180</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>183</v>
-      </c>
       <c r="C2" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -1686,39 +1678,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="D1" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="E1" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="F1" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="G1" s="14" t="s">
         <v>188</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="H1" s="14" t="s">
         <v>189</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="13" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C2" s="14" t="n">
         <v>10</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E2" s="14" t="n">
         <v>100</v>
@@ -1731,6 +1723,58 @@
       </c>
       <c r="H2" s="14" t="n">
         <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.7592592592593"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="15" width="12.4444444444444"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="15" width="11.4666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.52592592592593"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -1771,45 +1815,45 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>9878976543</v>
       </c>
       <c r="C2" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>31</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1853,27 +1897,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>36</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>38</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>39</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>5000</v>
@@ -1926,42 +1970,42 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="0" t="s">
         <v>45</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>51</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>540037</v>
@@ -1999,30 +2043,30 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>57</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="0" t="n">
         <f aca="false">TRUE()</f>
@@ -2086,33 +2130,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>62</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>67</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -2161,69 +2205,69 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="J1" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="K1" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="L1" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="M1" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="O1" s="0" t="s">
         <v>81</v>
-      </c>
-      <c r="O1" s="0" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="F2" s="0" t="s">
-        <v>88</v>
-      </c>
       <c r="G2" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H2" s="8" t="n">
         <v>42653</v>
@@ -2232,7 +2276,7 @@
         <v>42654</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K2" s="0" t="n">
         <v>10</v>
@@ -2241,7 +2285,7 @@
         <v>20</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N2" s="8" t="n">
         <v>42358</v>
@@ -2287,16 +2331,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>93</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2304,16 +2348,16 @@
         <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>97</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2321,16 +2365,16 @@
         <v>8</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>100</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2338,16 +2382,16 @@
         <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="E4" s="0" t="s">
         <v>103</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2355,50 +2399,50 @@
         <v>12</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="D5" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="E5" s="0" t="s">
         <v>107</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="C6" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="D6" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="E6" s="0" t="s">
         <v>112</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>115</v>
-      </c>
       <c r="E7" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2436,21 +2480,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>116</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>119</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Vinay] Modified the tags
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="17"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="registeredUserDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="196">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t xml:space="preserve">944186</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adm_manager</t>
   </si>
   <si>
     <t xml:space="preserve">mobileNumber</t>
@@ -628,13 +631,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
     <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-    <numFmt numFmtId="168" formatCode="0.00"/>
-    <numFmt numFmtId="169" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="169" formatCode="0.00"/>
+    <numFmt numFmtId="170" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -720,7 +724,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -749,6 +753,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -761,11 +769,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -863,10 +871,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1026,6 +1034,20 @@
       </c>
       <c r="D9" s="6" t="n">
         <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>944168</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="7" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1064,15 +1086,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>5000</v>
@@ -1120,89 +1142,89 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="H2" s="8" t="n">
+        <v>139</v>
+      </c>
+      <c r="H2" s="9" t="n">
         <v>42319</v>
       </c>
-      <c r="I2" s="8" t="n">
+      <c r="I2" s="9" t="n">
         <v>42327</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="K2" s="10" t="n">
+        <v>89</v>
+      </c>
+      <c r="K2" s="11" t="n">
         <v>10</v>
       </c>
-      <c r="L2" s="10" t="n">
+      <c r="L2" s="11" t="n">
         <v>20</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="N2" s="8" t="n">
+        <v>140</v>
+      </c>
+      <c r="N2" s="9" t="n">
         <v>42358</v>
       </c>
       <c r="O2" s="0" t="n">
@@ -1244,18 +1266,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1016093139</v>
@@ -1263,13 +1285,13 @@
       <c r="C2" s="0" t="n">
         <v>98765</v>
       </c>
-      <c r="D2" s="11" t="n">
+      <c r="D2" s="12" t="n">
         <v>42695</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1016093140</v>
@@ -1319,57 +1341,57 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>20</v>
@@ -1383,25 +1405,25 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>158</v>
-      </c>
       <c r="F3" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>25</v>
@@ -1410,7 +1432,7 @@
         <v>4</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -1453,33 +1475,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1000</v>
@@ -1491,7 +1513,7 @@
         <v>100</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>1234</v>
@@ -1499,7 +1521,7 @@
       <c r="G2" s="0" t="n">
         <v>123456</v>
       </c>
-      <c r="H2" s="11" t="n">
+      <c r="H2" s="12" t="n">
         <v>42689</v>
       </c>
       <c r="I2" s="0" t="n">
@@ -1545,27 +1567,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>123</v>
@@ -1577,13 +1599,13 @@
         <v>789</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -1621,21 +1643,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -1662,66 +1684,66 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="12" width="12.7407407407407"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="12" width="11.562962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="12" width="9.40740740740741"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="12" width="19.7962962962963"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="12" width="7.25185185185185"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="12" width="23.7148148148148"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="12" width="22.537037037037"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="12" width="18.9111111111111"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="12" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="12.7407407407407"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="11.562962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="19.7962962962963"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="13" width="7.25185185185185"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="23.7148148148148"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="13" width="22.537037037037"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="13" width="18.9111111111111"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="13" width="8.81851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>183</v>
-      </c>
-      <c r="C1" s="14" t="s">
+      <c r="B1" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="C1" s="15" t="s">
         <v>185</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="D1" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="E1" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="F1" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="G1" s="15" t="s">
         <v>189</v>
       </c>
+      <c r="H1" s="15" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="C2" s="14" t="n">
+      <c r="A2" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="C2" s="15" t="n">
         <v>10</v>
       </c>
-      <c r="D2" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="E2" s="14" t="n">
+      <c r="D2" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="E2" s="15" t="n">
         <v>100</v>
       </c>
-      <c r="F2" s="14" t="n">
+      <c r="F2" s="15" t="n">
         <v>10</v>
       </c>
-      <c r="G2" s="13" t="n">
+      <c r="G2" s="14" t="n">
         <v>1000</v>
       </c>
-      <c r="H2" s="14" t="n">
+      <c r="H2" s="15" t="n">
         <v>1000</v>
       </c>
     </row>
@@ -1743,15 +1765,15 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.7592592592593"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="15" width="12.4444444444444"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="15" width="11.4666666666667"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="16" width="12.4444444444444"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="16" width="11.4666666666667"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.52592592592593"/>
   </cols>
   <sheetData>
@@ -1759,22 +1781,22 @@
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
-        <v>179</v>
-      </c>
-      <c r="C1" s="15" t="s">
+      <c r="B1" s="16" t="s">
         <v>180</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="B2" s="15" t="s">
         <v>193</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="B2" s="16" t="s">
         <v>194</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -1815,45 +1837,45 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>9878976543</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="7" t="s">
         <v>29</v>
       </c>
+      <c r="E2" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="F2" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1897,27 +1919,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>5000</v>
@@ -1928,7 +1950,7 @@
       <c r="E2" s="0" t="n">
         <v>123</v>
       </c>
-      <c r="F2" s="8" t="n">
+      <c r="F2" s="9" t="n">
         <v>42350</v>
       </c>
     </row>
@@ -1970,42 +1992,42 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>540037</v>
@@ -2043,30 +2065,30 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" s="9" t="s">
         <v>52</v>
       </c>
+      <c r="C1" s="10" t="s">
+        <v>53</v>
+      </c>
       <c r="D1" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B2" s="0" t="n">
         <f aca="false">TRUE()</f>
@@ -2130,33 +2152,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -2205,78 +2227,78 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="8" t="n">
+        <v>28</v>
+      </c>
+      <c r="H2" s="9" t="n">
         <v>42653</v>
       </c>
-      <c r="I2" s="8" t="n">
+      <c r="I2" s="9" t="n">
         <v>42654</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K2" s="0" t="n">
         <v>10</v>
@@ -2285,9 +2307,9 @@
         <v>20</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="N2" s="8" t="n">
+        <v>90</v>
+      </c>
+      <c r="N2" s="9" t="n">
         <v>42358</v>
       </c>
       <c r="O2" s="0" t="n">
@@ -2331,16 +2353,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2348,16 +2370,16 @@
         <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2365,16 +2387,16 @@
         <v>8</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2382,16 +2404,16 @@
         <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2399,50 +2421,50 @@
         <v>12</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>113</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2480,21 +2502,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Vinay] Added a new feature Closure for Conneciton
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="registeredUserDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -792,18 +792,18 @@
   </sheetPr>
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.3444444444444"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.3037037037037"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.9148148148148"/>
-    <col collapsed="false" hidden="false" max="26" min="5" style="0" width="11.8555555555556"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="14.9925925925926"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.737037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.7962962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.2074074074074"/>
+    <col collapsed="false" hidden="false" max="26" min="5" style="0" width="12.1518518518519"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="15.3851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -995,10 +995,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.4592592592593"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.2666666666667"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.7111111111111"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.1444444444444"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.6592592592593"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.4"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1047,14 +1047,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.7888888888889"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.0518518518519"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="8.81851851851852"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.4444444444444"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="8.81851851851852"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.8740740740741"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.5740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.2481481481481"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.4259259259259"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.2666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1175,10 +1175,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.8740740740741"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.1666666666667"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="18.4222222222222"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.2666666666667"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1247,16 +1247,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="22.7333333333333"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.0148148148148"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.7185185185185"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.662962962963"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.837037037037"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.0148148148148"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.6"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.637037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="23.2259259259259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.3074074074074"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.0148148148148"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.9555555555556"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.3074074074074"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.1259259259259"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1379,15 +1379,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="12.937037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.8740740740741"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.7407407407407"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.837037037037"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.462962962963"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.6592592592593"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.0518518518519"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="13.2296296296296"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.2666666666667"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.937037037037"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.8555555555556"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.0518518518519"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.3444444444444"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1472,14 +1472,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.6"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.2074074074074"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.7962962962963"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.6592592592593"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.2666666666667"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.6"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.5037037037037"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.0925925925926"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.0518518518519"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.6592592592593"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1552,10 +1552,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8962962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1604,15 +1604,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="12" width="12.937037037037"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="12" width="11.8555555555556"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="12" width="9.6037037037037"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="12" width="20.2851851851852"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="12" width="7.34814814814815"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="12" width="24.3037037037037"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="12" width="23.0296296296296"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="12" width="19.3037037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="12" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="12" width="13.2296296296296"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="12" width="12.1518518518519"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="12" width="9.8"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="12" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="12" width="7.44814814814815"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="12" width="24.8888888888889"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="12" width="23.5185185185185"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="12" width="19.7962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="12" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1691,10 +1691,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.0518518518519"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="11.7592592592593"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.2481481481481"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="12.0518518518519"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.81851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1737,16 +1737,19 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.7962962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.4444444444444"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="16.9518518518519"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.9518518518519"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.0925925925926"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1822,12 +1825,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.8111111111111"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5444444444444"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.9296296296296"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.8333333333333"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.5"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.4"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4222222222222"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.7407407407407"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.6148148148148"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.3222222222222"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.9925925925926"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1894,11 +1898,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.6814814814815"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="12.837037037037"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.4259259259259"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.3037037037037"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.9740740740741"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.7185185185185"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.7962962962963"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1970,6 +1976,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.62222222222222"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -2054,7 +2063,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.8111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.4"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2115,18 +2125,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.837037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.537037037037"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.7962962962963"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.9925925925926"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.1481481481481"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.1296296296296"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.15185185185185"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.03703703703704"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="4" width="26.0666666666667"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="22.8333333333333"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.7148148148148"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.0296296296296"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.0925925925926"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.3851851851852"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.5407407407407"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.5222222222222"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.25185185185185"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.13333333333333"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="4" width="26.7518518518519"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="23.3222222222222"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="24.3037037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2247,11 +2260,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.2666666666667"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.4814814814815"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.3814814814815"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="38.7074074074074"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.8703703703704"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6592592592593"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.9703703703704"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.8740740740741"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.6888888888889"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.5555555555556"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2397,9 +2411,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.4259259259259"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.362962962963"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7185185185185"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.9518518518519"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[karthik] Modified LineEstimate Feature
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
@@ -801,12 +801,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.1296296296296"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.462962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.2851851851852"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5037037037037"/>
-    <col collapsed="false" hidden="false" max="26" min="5" style="0" width="12.3481481481481"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="15.7777777777778"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.5222222222222"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.8555555555556"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.7962962962963"/>
+    <col collapsed="false" hidden="false" max="26" min="5" style="0" width="12.5444444444444"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="16.1703703703704"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1016,10 +1016,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.7333333333333"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0518518518519"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.0851851851852"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.4185185185185"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.3444444444444"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.8666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1068,14 +1068,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.3592592592593"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4444444444444"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="9.21111111111111"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.837037037037"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.7185185185185"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="9.21111111111111"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.6592592592593"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.1407407407407"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.0148148148148"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.0518518518519"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1196,10 +1196,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="18.8148148148148"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.6592592592593"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.2444444444444"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="19.2074074074074"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.0518518518519"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.7333333333333"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1268,16 +1268,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="23.7148148148148"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.6"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2481481481481"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.4259259259259"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.6"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.6148148148148"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="24.3037037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8148148148148"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.6"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4444444444444"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.7185185185185"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="24.2037037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1400,15 +1400,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="13.5222222222222"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.6592592592593"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.2296296296296"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.4259259259259"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.3444444444444"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.737037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="13.8185185185185"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.0518518518519"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.4259259259259"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.5222222222222"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.7185185185185"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.737037037037"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.1296296296296"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1493,14 +1493,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8962962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.7962962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.4814814814815"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.3444444444444"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.0518518518519"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.0925925925926"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.8740740740741"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.4222222222222"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.737037037037"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.3444444444444"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1573,10 +1573,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.462962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.8555555555556"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1625,15 +1625,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="12" width="13.5222222222222"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="12" width="12.3481481481481"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="12" width="9.9962962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="12" width="21.262962962963"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="12" width="7.54444444444444"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="12" width="25.4777777777778"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="12" width="24.1074074074074"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="12" width="20.2851851851852"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="12" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="12" width="13.8185185185185"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="12" width="12.5444444444444"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="12" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="12" width="21.8518518518519"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="12" width="7.64444444444445"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="12" width="26.0666666666667"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="12" width="24.6962962962963"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="12" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="12" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1712,10 +1712,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.4444444444444"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="12.2481481481481"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="13.4259259259259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="12.4444444444444"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.21111111111111"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1764,13 +1764,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.81851851851852"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.4814814814815"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.837037037037"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.81851851851852"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.8740740740741"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1846,13 +1846,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.9888888888889"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8148148148148"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.937037037037"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.3"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.8111111111111"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.4814814814815"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.5777777777778"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.2074074074074"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.2296296296296"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.9851851851852"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.4"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.9703703703704"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1919,13 +1919,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.81851851851852"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.2703703703704"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="13.4259259259259"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.0148148148148"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.2851851851852"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.4259259259259"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.562962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="13.7185185185185"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.3074074074074"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.7185185185185"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1998,7 +1998,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2084,8 +2084,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.9888888888889"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.5777777777778"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2146,21 +2146,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.81851851851852"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.4259259259259"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.5185185185185"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.4814814814815"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="8.81851851851852"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.7777777777778"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.9333333333333"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.9111111111111"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.34814814814815"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.23333333333333"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="4" width="27.3407407407407"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="23.8111111111111"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="24.8888888888889"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7185185185185"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.1074074074074"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.8740740740741"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.1703703703704"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.3259259259259"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.3037037037037"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.8148148148148"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.44814814814815"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.32962962962963"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="4" width="27.9296296296296"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="24.4"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="25.4777777777778"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2281,12 +2281,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0518518518519"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.4592592592593"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.362962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.6666666666667"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.2407407407407"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.3444444444444"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.0481481481481"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.9518518518519"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.7444444444445"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.8296296296296"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2432,10 +2432,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.0148148148148"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.4407407407407"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4222222222222"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3074074074074"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.9296296296296"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[Vinay] Added Financial Feature
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="registeredUserDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="202">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -105,6 +105,9 @@
     <t xml:space="preserve">assis_Engineer</t>
   </si>
   <si>
+    <t xml:space="preserve">accountsOfficer</t>
+  </si>
+  <si>
     <t xml:space="preserve">mobileNumber</t>
   </si>
   <si>
@@ -388,6 +391,18 @@
   </si>
   <si>
     <t xml:space="preserve">A.P.Sreenivasulu/ENG_Assistant Engineer_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accountOfficer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACCOUNTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assistant Examiner of Accounts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hanuman Prasad ~ ACC_AEOA_1</t>
   </si>
   <si>
     <t xml:space="preserve">propertyType</t>
@@ -642,7 +657,7 @@
     <numFmt numFmtId="168" formatCode="0.00"/>
     <numFmt numFmtId="169" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -671,6 +686,11 @@
       <name val="Menlo"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="DejaVu Sans Mono"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -715,7 +735,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -756,6 +776,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -793,20 +817,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.5222222222222"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.8555555555556"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.7740740740741"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.7962962962963"/>
-    <col collapsed="false" hidden="false" max="26" min="5" style="0" width="12.5444444444444"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="16.1703703703704"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3037037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.8518518518519"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.4814814814815"/>
+    <col collapsed="false" hidden="false" max="26" min="5" style="0" width="12.937037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -985,6 +1008,20 @@
         <v>5</v>
       </c>
       <c r="D11" s="6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>944162</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="6" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -992,6 +1029,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C11" r:id="rId1" display="kurnool_eGov@123"/>
+    <hyperlink ref="C12" r:id="rId2" display="kurnool_eGov@123"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1016,10 +1054,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.4185185185185"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.3444444444444"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.8666666666667"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.7888888888889"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.1296296296296"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.337037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1027,15 +1065,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>5000</v>
@@ -1068,14 +1106,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.1407407407407"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="9.40740740740741"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.0148148148148"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="9.40740740740741"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.0518518518519"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.7111111111111"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.7185185185185"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.6"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.737037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="9.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1083,69 +1121,69 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="H2" s="8" t="n">
         <v>42319</v>
@@ -1154,16 +1192,16 @@
         <v>42327</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="K2" s="10" t="n">
+        <v>91</v>
+      </c>
+      <c r="K2" s="11" t="n">
         <v>10</v>
       </c>
-      <c r="L2" s="10" t="n">
+      <c r="L2" s="11" t="n">
         <v>20</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="N2" s="8" t="n">
         <v>42358</v>
@@ -1196,10 +1234,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="19.2074074074074"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.0518518518519"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.7333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="20.1851851851852"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.737037037037"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.7148148148148"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1207,18 +1245,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1016093139</v>
@@ -1226,13 +1264,13 @@
       <c r="C2" s="0" t="n">
         <v>98765</v>
       </c>
-      <c r="D2" s="11" t="n">
+      <c r="D2" s="12" t="n">
         <v>42695</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1016093140</v>
@@ -1268,71 +1306,71 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="24.3037037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8148148148148"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.8962962962963"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.6"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4444444444444"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.7185185185185"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.8962962962963"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="24.2037037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="25.4777777777778"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.3074074074074"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.3814814814815"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>20</v>
@@ -1346,25 +1384,25 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>25</v>
@@ -1373,7 +1411,7 @@
         <v>4</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -1400,15 +1438,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="13.8185185185185"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.0518518518519"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.4259259259259"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.5222222222222"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.7185185185185"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.737037037037"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.1296296296296"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="14.4037037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.737037037037"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.0148148148148"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.1111111111111"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.3074074074074"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.4222222222222"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.5222222222222"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.9111111111111"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1416,33 +1454,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1000</v>
@@ -1454,7 +1492,7 @@
         <v>100</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>1234</v>
@@ -1462,7 +1500,7 @@
       <c r="G2" s="0" t="n">
         <v>123456</v>
       </c>
-      <c r="H2" s="11" t="n">
+      <c r="H2" s="12" t="n">
         <v>42689</v>
       </c>
       <c r="I2" s="0" t="n">
@@ -1493,14 +1531,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.0925925925926"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.8740740740741"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.737037037037"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.3444444444444"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.8740740740741"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.6592592592593"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.2074074074074"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.5222222222222"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.1296296296296"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1508,27 +1546,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>123</v>
@@ -1540,13 +1578,13 @@
         <v>789</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -1573,10 +1611,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.8555555555556"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.462962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.8555555555556"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1584,21 +1622,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -1625,66 +1663,66 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="12" width="13.8185185185185"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="12" width="12.5444444444444"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="12" width="10.1925925925926"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="12" width="21.8518518518519"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="12" width="7.64444444444445"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="12" width="26.0666666666667"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="12" width="24.6962962962963"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="12" width="20.7740740740741"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="12" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="14.4037037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="12.937037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="10.5851851851852"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="22.8333333333333"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="13" width="7.84074074074074"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="27.3407407407407"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="13" width="25.8703703703704"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="13" width="21.8518518518519"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="13" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>186</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>187</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>188</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>189</v>
-      </c>
-      <c r="G1" s="14" t="s">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="C1" s="15" t="s">
         <v>191</v>
       </c>
+      <c r="D1" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>172</v>
-      </c>
-      <c r="C2" s="14" t="n">
+      <c r="A2" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="C2" s="15" t="n">
         <v>10</v>
       </c>
-      <c r="D2" s="14" t="s">
-        <v>193</v>
-      </c>
-      <c r="E2" s="14" t="n">
+      <c r="D2" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="E2" s="15" t="n">
         <v>100</v>
       </c>
-      <c r="F2" s="14" t="n">
+      <c r="F2" s="15" t="n">
         <v>10</v>
       </c>
-      <c r="G2" s="13" t="n">
+      <c r="G2" s="14" t="n">
         <v>1000</v>
       </c>
-      <c r="H2" s="14" t="n">
+      <c r="H2" s="15" t="n">
         <v>1000</v>
       </c>
     </row>
@@ -1712,10 +1750,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="13.4259259259259"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="12.4444444444444"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="14.0148148148148"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1723,21 +1761,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -1764,13 +1802,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.8740740740741"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.6592592592593"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.7185185185185"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="18.8148148148148"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.8148148148148"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1778,45 +1816,45 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>9878976543</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1846,13 +1884,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.5777777777778"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.2074074074074"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.2296296296296"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.9851851851852"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.4"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.9703703703704"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.9481481481481"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.1851851851852"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.8185185185185"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.5555555555556"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.5777777777778"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.0481481481481"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1860,27 +1898,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>5000</v>
@@ -1919,13 +1957,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.562962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="13.7185185185185"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.7740740740741"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="13.7185185185185"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.1518518518519"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="14.3074074074074"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.8518518518519"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="14.3074074074074"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1933,42 +1971,42 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>540037</v>
@@ -1998,7 +2036,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2006,30 +2044,30 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B2" s="0" t="n">
         <f aca="false">TRUE()</f>
@@ -2084,8 +2122,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.5777777777778"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.9481481481481"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2093,33 +2131,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2146,21 +2184,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7185185185185"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.1074074074074"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.8740740740741"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.1703703703704"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.3259259259259"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.3037037037037"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.8148148148148"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.44814814814815"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.32962962962963"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="4" width="27.9296296296296"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="24.4"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="25.4777777777778"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3074074074074"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.2814814814815"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.6592592592593"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.9518518518519"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.1074074074074"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.2851851851852"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.64444444444445"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.52592592592593"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="4" width="29.3"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="25.5777777777778"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="26.7518518518519"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2168,69 +2206,69 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H2" s="8" t="n">
         <v>42653</v>
@@ -2239,7 +2277,7 @@
         <v>42654</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K2" s="0" t="n">
         <v>10</v>
@@ -2248,7 +2286,7 @@
         <v>20</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="N2" s="8" t="n">
         <v>42358</v>
@@ -2273,20 +2311,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.3444444444444"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.0481481481481"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.9518518518519"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.7444444444445"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.8296296296296"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.1296296296296"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.0296296296296"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.3407407407407"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.8037037037037"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.2037037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2294,16 +2332,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2311,16 +2349,16 @@
         <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2328,16 +2366,16 @@
         <v>8</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2345,16 +2383,16 @@
         <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2362,50 +2400,64 @@
         <v>12</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>114</v>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -2432,10 +2484,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.9296296296296"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.2074074074074"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.9111111111111"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2443,21 +2495,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[karthik] Done some changes for jenkins
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="registeredUserDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -649,13 +649,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
     <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-    <numFmt numFmtId="168" formatCode="0.00"/>
-    <numFmt numFmtId="169" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="169" formatCode="0.00"/>
+    <numFmt numFmtId="170" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -691,6 +692,7 @@
       <sz val="12"/>
       <name val="DejaVu Sans Mono"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -735,7 +737,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -764,6 +766,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -780,11 +786,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -819,17 +825,18 @@
   </sheetPr>
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3037037037037"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.8518518518519"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.4814814814815"/>
-    <col collapsed="false" hidden="false" max="26" min="5" style="0" width="12.937037037037"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7962962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.3444444444444"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.8740740740741"/>
+    <col collapsed="false" hidden="false" max="26" min="5" style="0" width="13.2296296296296"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="8.62222222222222"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -962,7 +969,7 @@
       <c r="C8" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="6" t="n">
+      <c r="D8" s="7" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1007,7 +1014,7 @@
       <c r="C11" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="6" t="n">
+      <c r="D11" s="7" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1054,10 +1061,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.7888888888889"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.1296296296296"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.337037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.5740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.5222222222222"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.1222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1106,14 +1113,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.7111111111111"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="9.8"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.7185185185185"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.6"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="9.8"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.737037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.4925925925926"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.4259259259259"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.0148148148148"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="18.1296296296296"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1185,25 +1192,25 @@
       <c r="G2" s="0" t="s">
         <v>145</v>
       </c>
-      <c r="H2" s="8" t="n">
+      <c r="H2" s="9" t="n">
         <v>42319</v>
       </c>
-      <c r="I2" s="8" t="n">
+      <c r="I2" s="9" t="n">
         <v>42327</v>
       </c>
       <c r="J2" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="K2" s="11" t="n">
+      <c r="K2" s="12" t="n">
         <v>10</v>
       </c>
-      <c r="L2" s="11" t="n">
+      <c r="L2" s="12" t="n">
         <v>20</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="N2" s="8" t="n">
+      <c r="N2" s="9" t="n">
         <v>42358</v>
       </c>
       <c r="O2" s="0" t="n">
@@ -1234,10 +1241,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.737037037037"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.7148148148148"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.1296296296296"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.3037037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.1925925925926"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1264,7 +1271,7 @@
       <c r="C2" s="0" t="n">
         <v>98765</v>
       </c>
-      <c r="D2" s="12" t="n">
+      <c r="D2" s="13" t="n">
         <v>42695</v>
       </c>
     </row>
@@ -1306,16 +1313,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="25.4777777777778"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.6962962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.837037037037"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.462962962963"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.3814814814815"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="26.0666666666667"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.1851851851852"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.6"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.8555555555556"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="25.9666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="10.1925925925926"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1438,15 +1445,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="14.4037037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.737037037037"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.0148148148148"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.1111111111111"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.5222222222222"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.9111111111111"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="14.7"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.1296296296296"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.3074074074074"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.4037037037037"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.6"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.8148148148148"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.9111111111111"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.3037037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.1925925925926"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1500,7 +1507,7 @@
       <c r="G2" s="0" t="n">
         <v>123456</v>
       </c>
-      <c r="H2" s="12" t="n">
+      <c r="H2" s="13" t="n">
         <v>42689</v>
       </c>
       <c r="I2" s="0" t="n">
@@ -1531,14 +1538,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.462962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.8740740740741"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.6592592592593"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.2074074074074"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.5222222222222"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.1296296296296"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.8555555555556"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.2666666666667"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.0518518518519"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.9111111111111"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.5222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.1925925925926"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1611,10 +1618,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.8555555555556"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.1925925925926"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1663,66 +1670,66 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="14.4037037037037"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="12.937037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="10.5851851851852"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="22.8333333333333"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="13" width="7.84074074074074"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="27.3407407407407"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="13" width="25.8703703703704"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="13" width="21.8518518518519"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="13" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="14" width="14.7"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="14" width="13.2296296296296"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="14" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="14" width="23.3222222222222"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="14" width="7.93703703703704"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="14" width="27.9296296296296"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="14" width="26.5555555555556"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="14" width="22.3444444444444"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="14" width="10.1925925925926"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="14" t="s">
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="16" t="s">
         <v>192</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="16" t="s">
         <v>194</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="16" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="C2" s="15" t="n">
+      <c r="C2" s="16" t="n">
         <v>10</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="16" t="s">
         <v>198</v>
       </c>
-      <c r="E2" s="15" t="n">
+      <c r="E2" s="16" t="n">
         <v>100</v>
       </c>
-      <c r="F2" s="15" t="n">
+      <c r="F2" s="16" t="n">
         <v>10</v>
       </c>
-      <c r="G2" s="14" t="n">
+      <c r="G2" s="15" t="n">
         <v>1000</v>
       </c>
-      <c r="H2" s="15" t="n">
+      <c r="H2" s="16" t="n">
         <v>1000</v>
       </c>
     </row>
@@ -1750,20 +1757,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="14.0148148148148"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="12.837037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.4259259259259"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="14.3074074074074"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>187</v>
       </c>
     </row>
@@ -1771,10 +1778,10 @@
       <c r="A2" s="0" t="s">
         <v>199</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>201</v>
       </c>
     </row>
@@ -1802,13 +1809,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.40740740740741"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.6592592592593"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.7185185185185"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.40740740740741"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="18.8148148148148"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.8148148148148"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0518518518519"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.0148148148148"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="8" width="19.2074074074074"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.2074074074074"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1824,7 +1831,7 @@
       <c r="D1" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="8" t="s">
         <v>26</v>
       </c>
       <c r="F1" s="0" t="s">
@@ -1884,13 +1891,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.9481481481481"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.8185185185185"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.5555555555556"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.5777777777778"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.0481481481481"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.537037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.1111111111111"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.337037037037"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.262962962963"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.537037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1929,7 +1936,7 @@
       <c r="E2" s="0" t="n">
         <v>123</v>
       </c>
-      <c r="F2" s="8" t="n">
+      <c r="F2" s="9" t="n">
         <v>42350</v>
       </c>
     </row>
@@ -1957,13 +1964,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.40740740740741"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.1518518518519"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.8962962962963"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.8518518518519"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.3481481481481"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="14.6"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.3444444444444"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="14.6"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2036,7 +2043,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2046,7 +2053,7 @@
       <c r="B1" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>55</v>
       </c>
       <c r="D1" s="0" t="s">
@@ -2122,8 +2129,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.9481481481481"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.537037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2184,21 +2191,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.40740740740741"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.2814814814815"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.6592592592593"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="9.40740740740741"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.9518518518519"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.1074074074074"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.2851851851852"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.6962962962963"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.64444444444445"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.52592592592593"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="4" width="29.3"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="25.5777777777778"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="26.7518518518519"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.6"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.8703703703704"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.0518518518519"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.5"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="20.1851851851852"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.74074074074074"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="4" width="29.9851851851852"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="26.262962962963"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="27.3407407407407"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2270,10 +2277,10 @@
       <c r="G2" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="8" t="n">
+      <c r="H2" s="9" t="n">
         <v>42653</v>
       </c>
-      <c r="I2" s="8" t="n">
+      <c r="I2" s="9" t="n">
         <v>42654</v>
       </c>
       <c r="J2" s="0" t="s">
@@ -2288,7 +2295,7 @@
       <c r="M2" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="N2" s="8" t="n">
+      <c r="N2" s="9" t="n">
         <v>42358</v>
       </c>
       <c r="O2" s="0" t="n">
@@ -2313,18 +2320,18 @@
   </sheetPr>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.1296296296296"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.0296296296296"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.3407407407407"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.8037037037037"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.2037037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.5222222222222"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.5185185185185"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.0074074074074"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.8814814814815"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.8888888888889"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2450,7 +2457,7 @@
       <c r="A8" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="11" t="s">
         <v>119</v>
       </c>
       <c r="C8" s="0" t="s">
@@ -2484,10 +2491,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.2074074074074"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8962962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.9111111111111"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.5"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[Vinay] Completed the financialTransactions Fetaure
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="ownerDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="187">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -338,7 +338,7 @@
     <t xml:space="preserve">A.P.Sreenivasulu/ENG_Assistant Engineer_1</t>
   </si>
   <si>
-    <t xml:space="preserve">accountOfficer</t>
+    <t xml:space="preserve">accountOfficer1</t>
   </si>
   <si>
     <t xml:space="preserve">ACCOUNTS</t>
@@ -348,6 +348,15 @@
   </si>
   <si>
     <t xml:space="preserve">Hanuman Prasad ~ ACC_AEOA_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accountOfficer2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Examiner of Accounts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D Ramachandra Reddy ~ ACC_EOA_1</t>
   </si>
   <si>
     <t xml:space="preserve">propertyType</t>
@@ -601,7 +610,7 @@
     <numFmt numFmtId="167" formatCode="0.00"/>
     <numFmt numFmtId="168" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -636,6 +645,11 @@
       <name val="DejaVu Sans Mono"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="DejaVu Sans Mono"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -680,7 +694,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -706,6 +720,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -756,19 +774,19 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.8"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.3444444444444"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.8"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.6962962962963"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.6962962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.737037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.6"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="20.1851851851852"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.1851851851852"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -844,14 +862,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.3740740740741"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7185185185185"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="10.1925925925926"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="10.1925925925926"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="18.5222222222222"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.2592592592593"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.0148148148148"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.6"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="18.9111111111111"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="10.3888888888889"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -859,54 +877,54 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>125</v>
+        <v>127</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>128</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>65</v>
@@ -918,10 +936,10 @@
         <v>67</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="H2" s="3" t="n">
         <v>42319</v>
@@ -932,14 +950,14 @@
       <c r="J2" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="K2" s="9" t="n">
+      <c r="K2" s="10" t="n">
         <v>10</v>
       </c>
-      <c r="L2" s="9" t="n">
+      <c r="L2" s="10" t="n">
         <v>20</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="N2" s="3" t="n">
         <v>42358</v>
@@ -972,10 +990,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="21.1666666666667"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.5222222222222"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.8888888888889"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.9111111111111"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.4777777777778"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.5851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -983,18 +1001,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1016093139</v>
@@ -1002,13 +1020,13 @@
       <c r="C2" s="0" t="n">
         <v>98765</v>
       </c>
-      <c r="D2" s="10" t="n">
+      <c r="D2" s="11" t="n">
         <v>42695</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1016093140</v>
@@ -1044,71 +1062,71 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="26.7518518518519"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.6777777777778"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.462962962963"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.4259259259259"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.8962962962963"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.462962962963"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="26.6555555555556"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="27.3407407407407"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.1666666666667"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.8555555555556"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.7185185185185"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.8555555555556"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.3407407407407"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="10.5851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E1" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>137</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>134</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>20</v>
@@ -1122,25 +1140,25 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>145</v>
-      </c>
       <c r="D3" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>25</v>
@@ -1149,7 +1167,7 @@
         <v>4</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -1176,15 +1194,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="14.9925925925926"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.5222222222222"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.6"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.7"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.8962962962963"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.2074074074074"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.3037037037037"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.7962962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="15.3851851851852"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.9111111111111"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.9925925925926"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.7962962962963"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.2851851851852"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.5851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1192,33 +1210,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
-        <v>158</v>
+      <c r="A2" s="8" t="s">
+        <v>161</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1000</v>
@@ -1230,7 +1248,7 @@
         <v>100</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>1234</v>
@@ -1238,7 +1256,7 @@
       <c r="G2" s="0" t="n">
         <v>123456</v>
       </c>
-      <c r="H2" s="10" t="n">
+      <c r="H2" s="11" t="n">
         <v>42689</v>
       </c>
       <c r="I2" s="0" t="n">
@@ -1269,14 +1287,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.8555555555556"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.6592592592593"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.3444444444444"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.3037037037037"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.9111111111111"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.0518518518519"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.737037037037"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.7962962962963"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.3037037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.5851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1284,27 +1302,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="G1" s="8" t="s">
         <v>165</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>123</v>
@@ -1315,14 +1333,14 @@
       <c r="D2" s="0" t="n">
         <v>789</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>167</v>
+      <c r="E2" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -1349,32 +1367,32 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8148148148148"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.4222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.5851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>169</v>
+      <c r="B1" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>171</v>
+        <v>173</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -1401,66 +1419,66 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="11" width="14.9925925925926"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="11" width="13.5222222222222"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="11.0740740740741"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="11" width="23.8111111111111"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="11" width="8.03703703703704"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="28.6148148148148"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="11" width="27.2407407407407"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="11" width="22.8333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="11" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="12" width="15.3851851851852"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="12" width="13.8185185185185"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="12" width="11.3666666666667"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="12" width="24.4"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="12" width="8.13333333333333"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="12" width="29.3"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="12" width="27.8296296296296"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="12" width="23.3222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="12" width="10.5851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>174</v>
-      </c>
-      <c r="E1" s="13" t="s">
+      <c r="B1" s="13" t="s">
         <v>175</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="C1" s="14" t="s">
         <v>176</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="D1" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="E1" s="14" t="s">
         <v>178</v>
       </c>
+      <c r="F1" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
-        <v>179</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="C2" s="13" t="n">
+      <c r="A2" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" s="14" t="n">
         <v>10</v>
       </c>
-      <c r="D2" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="E2" s="13" t="n">
+      <c r="D2" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="E2" s="14" t="n">
         <v>100</v>
       </c>
-      <c r="F2" s="13" t="n">
+      <c r="F2" s="14" t="n">
         <v>10</v>
       </c>
-      <c r="G2" s="12" t="n">
+      <c r="G2" s="13" t="n">
         <v>1000</v>
       </c>
-      <c r="H2" s="13" t="n">
+      <c r="H2" s="14" t="n">
         <v>1000</v>
       </c>
     </row>
@@ -1488,10 +1506,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7185185185185"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.6"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.4259259259259"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0148148148148"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.7185185185185"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.1925925925926"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1499,21 +1517,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -1540,13 +1558,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.1259259259259"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1666666666667"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.4037037037037"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.1222222222222"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.9481481481481"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.0296296296296"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.8111111111111"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.7"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.9074074074074"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.537037037037"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.5185185185185"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1613,13 +1631,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.8"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5444444444444"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="14.8962962962963"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.8333333333333"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="4" width="14.8962962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.7407407407407"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.3222222222222"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="4" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1692,7 +1710,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1778,8 +1796,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.1259259259259"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.8111111111111"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1840,21 +1858,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.8"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8962962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.5555555555556"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.3444444444444"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="9.8"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.9925925925926"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.262962962963"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="20.6777777777778"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.84074074074074"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.81851851851852"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="30.7703703703704"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="26.9481481481481"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="27.9296296296296"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.2407407407407"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.737037037037"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.4814814814815"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.8518518518519"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.1666666666667"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.93703703703704"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="31.5555555555556"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="27.537037037037"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="28.6148148148148"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1967,20 +1985,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.9111111111111"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.1074074074074"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.6925925925926"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="46.0555555555556"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.6703703703704"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3037037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.6962962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.3777777777778"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.2333333333333"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.4555555555556"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2114,6 +2132,20 @@
       </c>
       <c r="D8" s="0" t="s">
         <v>103</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -2140,10 +2172,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.0851851851852"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.6740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2151,21 +2183,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -2192,17 +2224,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.3592592592593"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.9111111111111"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.9074074074074"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.1407407407407"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3037037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.6888888888889"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.3888888888889"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="0" t="s">
@@ -2211,7 +2243,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>5000</v>

</xml_diff>

<commit_message>
[PHOENIX-5868] Completed the creation of  new expense bill
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="191">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -357,6 +357,18 @@
   </si>
   <si>
     <t xml:space="preserve">D Ramachandra Reddy ~ ACC_EOA_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accountOfficer3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D Ramachandra Reddy/ACC_EOA_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">commissioner1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S.Ravindra Babu/ADM_Commissioner_1</t>
   </si>
   <si>
     <t xml:space="preserve">propertyType</t>
@@ -610,7 +622,7 @@
     <numFmt numFmtId="167" formatCode="0.00"/>
     <numFmt numFmtId="168" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -645,11 +657,6 @@
       <name val="DejaVu Sans Mono"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="DejaVu Sans Mono"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -723,7 +730,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -780,13 +787,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.9962962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.737037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.6"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.9962962962963"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.1296296296296"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.1925925925926"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -862,14 +869,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.2592592592593"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.0148148148148"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="10.3888888888889"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.6"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="10.3888888888889"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="18.9111111111111"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.237037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3074074074074"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="10.5851851851852"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="10.5851851851852"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="19.3037037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="10.5851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -877,54 +884,54 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>65</v>
@@ -936,10 +943,10 @@
         <v>67</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="H2" s="3" t="n">
         <v>42319</v>
@@ -957,7 +964,7 @@
         <v>20</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="N2" s="3" t="n">
         <v>42358</v>
@@ -990,10 +997,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="21.6555555555556"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.9111111111111"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.4777777777778"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.5851851851852"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="22.2444444444444"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.3037037037037"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.0666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.7777777777778"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1001,18 +1008,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1016093139</v>
@@ -1026,7 +1033,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1016093140</v>
@@ -1062,71 +1069,71 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="27.3407407407407"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.1666666666667"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.8555555555556"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.462962962963"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.7185185185185"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.8555555555556"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.3407407407407"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="10.5851851851852"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="27.9296296296296"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.8555555555556"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.0148148148148"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.9296296296296"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="10.7777777777778"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>20</v>
@@ -1140,25 +1147,25 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>147</v>
-      </c>
       <c r="C3" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>25</v>
@@ -1167,7 +1174,7 @@
         <v>4</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -1194,15 +1201,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="15.3851851851852"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.9111111111111"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.8962962962963"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.9925925925926"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.6962962962963"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.7962962962963"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.2851851851852"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.5851851851852"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="15.7777777777778"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.3037037037037"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.3851851851852"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.1851851851852"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.2851851851852"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.7777777777778"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1210,33 +1217,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1000</v>
@@ -1248,7 +1255,7 @@
         <v>100</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>1234</v>
@@ -1287,14 +1294,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.0518518518519"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.737037037037"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.6777777777778"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.7962962962963"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.3037037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.5851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.3444444444444"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.1296296296296"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.1666666666667"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.2851851851852"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.7962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.7777777777778"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1302,27 +1309,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>123</v>
@@ -1334,13 +1341,13 @@
         <v>789</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -1367,10 +1374,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8148148148148"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.5851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.2074074074074"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4222222222222"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8148148148148"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.7777777777778"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1378,21 +1385,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -1419,15 +1426,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="12" width="15.3851851851852"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="12" width="13.8185185185185"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="12" width="11.3666666666667"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="12" width="24.4"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="12" width="8.13333333333333"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="12" width="29.3"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="12" width="27.8296296296296"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="12" width="23.3222222222222"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="12" width="10.5851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="12" width="15.7777777777778"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="12" width="14.1111111111111"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="12" width="11.662962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="12" width="24.9888888888889"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="12" width="8.23333333333333"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="12" width="29.9851851851852"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="12" width="28.5148148148148"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="12" width="23.8111111111111"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="12" width="10.7777777777778"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1435,39 +1442,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="13" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="C2" s="14" t="n">
         <v>10</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="E2" s="14" t="n">
         <v>100</v>
@@ -1506,10 +1513,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0148148148148"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.8962962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.7185185185185"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3074074074074"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.0148148148148"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.3888888888889"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1517,21 +1524,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -1558,13 +1565,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.8111111111111"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.6555555555556"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.7"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.9074074074074"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.537037037037"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.5185185185185"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.4962962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.2444444444444"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.9925925925926"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.6888888888889"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.1259259259259"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.1074074074074"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.1925925925926"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1631,13 +1638,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.9962962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.7407407407407"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.3222222222222"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="4" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.937037037037"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.8111111111111"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="4" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.1925925925926"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1710,7 +1717,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.1925925925926"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1796,8 +1803,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.8111111111111"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.4962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.1925925925926"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1858,21 +1865,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.9962962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.2407407407407"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.737037037037"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="9.9962962962963"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.4814814814815"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.8518518518519"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.1666666666667"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="7.93703703703704"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="31.5555555555556"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="27.537037037037"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="28.6148148148148"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.8296296296296"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.1296296296296"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.4222222222222"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.9703703703704"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.3444444444444"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.03703703703704"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.21111111111111"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="32.337037037037"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="28.1259259259259"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="29.3"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="10.1925925925926"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1985,20 +1992,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3037037037037"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.6962962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.3777777777778"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.2333333333333"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.4555555555556"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7962962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.2814814814815"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.162962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.4074074074074"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.2407407407407"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.1925925925926"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2146,6 +2153,51 @@
       </c>
       <c r="D9" s="0" t="s">
         <v>106</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -2172,10 +2224,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6777777777778"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.6740740740741"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1666666666667"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.3592592592593"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.1925925925926"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2183,21 +2235,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2224,10 +2276,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.1407407407407"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3037037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.6888888888889"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.9259259259259"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.7962962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.5703703703704"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.5851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2243,7 +2295,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>5000</v>

</xml_diff>

<commit_message>
[PHOENIX-5878] Compelted the create new & additional water connection
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="ownerDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -787,13 +787,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1925925925926"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.1296296296296"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.8962962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.1925925925926"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="20.6777777777778"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.6777777777778"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.5222222222222"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.1666666666667"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.1666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.3888888888889"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -869,14 +869,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.237037037037"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="10.5851851851852"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.8962962962963"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="10.5851851851852"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="19.3037037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="10.5851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.1185185185185"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.6"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="19.7962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="10.7777777777778"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -991,16 +991,16 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="22.2444444444444"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.3037037037037"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.0666666666667"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="22.7333333333333"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.7962962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.7518518518519"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.0740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1036,7 +1036,7 @@
         <v>140</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>1016093140</v>
+        <v>1016039520</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>0</v>
@@ -1063,22 +1063,22 @@
   </sheetPr>
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="27.9296296296296"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.6555555555556"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.8555555555556"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.0148148148148"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.9296296296296"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="28.6148148148148"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.2444444444444"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.3074074074074"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.4222222222222"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="28.6148148148148"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.0740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1201,15 +1201,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="15.7777777777778"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.3037037037037"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.3851851851852"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.2851851851852"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.7740740740741"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="16.1703703703704"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.7962962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.7777777777778"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.262962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.0740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1294,14 +1294,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.3444444444444"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.1296296296296"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.1666666666667"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.2851851851852"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.7962962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4222222222222"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.737037037037"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.5222222222222"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.2851851851852"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.0740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1374,10 +1374,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.2074074074074"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8148148148148"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8148148148148"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.2074074074074"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.0740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1426,15 +1426,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="12" width="15.7777777777778"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="12" width="14.1111111111111"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="12" width="11.662962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="12" width="24.9888888888889"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="12" width="8.23333333333333"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="12" width="29.9851851851852"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="12" width="28.5148148148148"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="12" width="23.8111111111111"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="12" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="12" width="16.1703703703704"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="12" width="14.4037037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="12" width="11.9555555555556"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="12" width="25.5777777777778"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="12" width="8.32962962962963"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="12" width="30.7703703703704"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="12" width="29.2037037037037"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="12" width="24.4"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="12" width="11.0740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1513,10 +1513,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.0148148148148"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.6"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.3074074074074"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.5851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1565,13 +1565,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.4962962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.2444444444444"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.9925925925926"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.6888888888889"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.1259259259259"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.1074074074074"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.1814814814815"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.7333333333333"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3851851851852"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.5703703703704"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.8111111111111"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.6962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.3888888888889"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1638,13 +1638,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1925925925926"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.937037037037"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.462962962963"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.8111111111111"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="4" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2296296296296"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.8555555555556"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.4"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="4" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.3888888888889"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1717,7 +1717,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.3888888888889"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1803,8 +1803,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.4962962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.1814814814815"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.3888888888889"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1865,21 +1865,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1925925925926"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.8296296296296"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.1296296296296"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="10.1925925925926"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.9703703703704"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.3444444444444"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.6555555555556"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.03703703703704"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.21111111111111"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="32.337037037037"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="28.1259259259259"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="29.3"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.5148148148148"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.5222222222222"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.8148148148148"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.4592592592593"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.8333333333333"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.2444444444444"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.13333333333333"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="33.1222222222222"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="28.8111111111111"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="29.9851851851852"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="10.3888888888889"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1994,18 +1994,18 @@
   </sheetPr>
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7962962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.2814814814815"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.162962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.4074074074074"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.2407407407407"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.2851851851852"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.8703703703704"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.9444444444444"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.5851851851852"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.0222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.3888888888889"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2224,10 +2224,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1666666666667"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.462962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.3592592592593"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.8555555555556"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.0481481481481"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.3888888888889"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2276,10 +2276,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.9259259259259"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.7962962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.5703703703704"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.5851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.7111111111111"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.2851851851852"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.4555555555556"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.7777777777778"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[PHOENIX-5897] Comeplted the change of use water connection scenario
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="ownerDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="194">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -507,6 +507,15 @@
   </si>
   <si>
     <t xml:space="preserve">New Connection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">changeOfUse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NON-RESIDENTIALS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change Of Use</t>
   </si>
   <si>
     <t xml:space="preserve">monthlyFees</t>
@@ -787,13 +796,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3888888888889"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.5222222222222"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3888888888889"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.1666666666667"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.1666666666667"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.5851851851852"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.9111111111111"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.5851851851852"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.5851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -869,14 +878,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.1185185185185"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.6"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="10.7777777777778"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.462962962963"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="10.7777777777778"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="19.7962962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.8555555555556"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="20.2851851851852"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.0740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -991,16 +1000,16 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="22.7333333333333"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.7962962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.7518518518519"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="23.2259259259259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.2851851851852"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.3407407407407"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3666666666667"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1061,24 +1070,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="28.6148148148148"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.2444444444444"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="28.6148148148148"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="29.3"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.7333333333333"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.6"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.8148148148148"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="29.3"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.3666666666667"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1175,6 +1184,29 @@
       </c>
       <c r="J3" s="0" t="s">
         <v>156</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -1201,15 +1233,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="16.1703703703704"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.7962962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.7777777777778"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.6777777777778"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.7740740740741"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.262962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="16.5592592592593"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.2851851851852"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1703703703704"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.1666666666667"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.262962962963"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.8518518518519"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.3666666666667"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1217,33 +1249,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1000</v>
@@ -1255,7 +1287,7 @@
         <v>100</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>1234</v>
@@ -1294,14 +1326,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.737037037037"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.5222222222222"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.6555555555556"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.7740740740741"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.2851851851852"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4222222222222"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8148148148148"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.1296296296296"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.9111111111111"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.2444444444444"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.262962962963"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.3666666666667"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1309,27 +1341,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>123</v>
@@ -1341,13 +1373,13 @@
         <v>789</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -1374,10 +1406,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.6962962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8148148148148"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.2074074074074"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.1851851851852"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.2074074074074"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3666666666667"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1385,21 +1417,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -1426,15 +1458,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="12" width="16.1703703703704"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="12" width="14.4037037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="12" width="11.9555555555556"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="12" width="25.5777777777778"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="12" width="8.32962962962963"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="12" width="30.7703703703704"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="12" width="29.2037037037037"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="12" width="24.4"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="12" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="12" width="16.5592592592593"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="12" width="14.7"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="12" width="12.2481481481481"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="12" width="26.262962962963"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="12" width="8.42592592592593"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="12" width="31.5555555555556"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="12" width="29.8888888888889"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="12" width="24.9888888888889"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="12" width="11.3666666666667"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1442,39 +1474,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="13" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C2" s="14" t="n">
         <v>10</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="E2" s="14" t="n">
         <v>100</v>
@@ -1513,10 +1545,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.6"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.3074074074074"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.5851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.6"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.7777777777778"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1524,21 +1556,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -1565,13 +1597,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.1814814814815"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.7333333333333"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3851851851852"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.5703703703704"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.8111111111111"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.6962962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.9666666666667"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.2259259259259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.7777777777778"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.4555555555556"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.4962962962963"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.2814814814815"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.5851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1638,13 +1670,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3888888888889"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2296296296296"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.8555555555556"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.4"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="4" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.5851851851852"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.5222222222222"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.9888888888889"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="4" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.5851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1717,7 +1749,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.5851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1803,8 +1835,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.1814814814815"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.9666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.5851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1865,21 +1897,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3888888888889"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.5148148148148"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.5222222222222"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="10.3888888888889"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.8148148148148"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.4592592592593"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.8333333333333"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.2444444444444"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.13333333333333"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.40740740740741"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="33.1222222222222"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="28.8111111111111"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="29.9851851851852"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.5851851851852"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.2037037037037"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.9111111111111"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="10.5851851851852"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.2074074074074"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.0481481481481"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.3222222222222"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.7333333333333"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.23333333333333"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="33.9074074074074"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="29.4962962962963"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="30.7703703703704"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="10.5851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2000,12 +2032,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.2851851851852"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.8703703703704"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.9444444444444"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.5851851851852"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.0222222222222"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.5555555555556"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.6333333333333"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.8592592592593"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.8074074074074"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.5851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2224,10 +2256,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.6555555555556"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.8555555555556"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.0481481481481"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2444444444444"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.6333333333333"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.5851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2276,10 +2308,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.7111111111111"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.2851851851852"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.4555555555556"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.4925925925926"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.4333333333333"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.0740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[PHOENIX-5899] Created a data entry screen scenario for water
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="ownerDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="196">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -461,6 +461,9 @@
     <t xml:space="preserve">applicantInfo1</t>
   </si>
   <si>
+    <t xml:space="preserve">dataEntryInfo</t>
+  </si>
+  <si>
     <t xml:space="preserve">1/2_12.50</t>
   </si>
   <si>
@@ -516,6 +519,9 @@
   </si>
   <si>
     <t xml:space="preserve">Change Of Use</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DataEntryScreen</t>
   </si>
   <si>
     <t xml:space="preserve">monthlyFees</t>
@@ -624,12 +630,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
     <numFmt numFmtId="167" formatCode="0.00"/>
     <numFmt numFmtId="168" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="169" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -710,7 +717,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -759,6 +766,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -796,13 +807,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.5851851851852"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.9111111111111"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.5851851851852"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.6555555555556"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.6555555555556"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.5851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3037037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.2444444444444"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.2444444444444"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.7777777777778"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -878,14 +889,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8962962962963"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="11.0740740740741"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.8555555555556"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="11.0740740740741"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="20.2851851851852"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.9814814814815"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="11.3666666666667"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="11.3666666666667"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.3666666666667"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -998,18 +1009,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="23.2259259259259"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.2851851851852"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.3407407407407"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3666666666667"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="23.7148148148148"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.9296296296296"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.662962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1052,6 +1063,20 @@
       </c>
       <c r="D3" s="0" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>1016093135</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>98765</v>
+      </c>
+      <c r="D4" s="12" t="n">
+        <v>42741</v>
       </c>
     </row>
   </sheetData>
@@ -1070,79 +1095,79 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="29.3"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.7333333333333"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.6"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.462962962963"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.8148148148148"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="29.3"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.3666666666667"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="29.9851851851852"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2259259259259"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.4222222222222"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.8555555555556"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.4222222222222"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.2074074074074"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="29.9851851851852"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.662962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>111</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>114</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>20</v>
@@ -1156,25 +1181,25 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>155</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>154</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>114</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>25</v>
@@ -1183,21 +1208,21 @@
         <v>4</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>114</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>19</v>
@@ -1206,7 +1231,39 @@
         <v>2</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -1233,15 +1290,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="16.5592592592593"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.2851851851852"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1703703703704"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.462962962963"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.1666666666667"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.262962962963"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.8518518518519"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.3666666666667"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="16.9518518518519"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.5592592592593"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.8555555555556"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.8518518518519"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.3444444444444"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.662962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1249,33 +1306,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1000</v>
@@ -1287,7 +1344,7 @@
         <v>100</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>1234</v>
@@ -1326,14 +1383,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8148148148148"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.1296296296296"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.9111111111111"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.2444444444444"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.262962962963"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.7740740740741"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.3666666666667"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8148148148148"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.2074074074074"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.5222222222222"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.3037037037037"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.7333333333333"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.8518518518519"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.262962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.662962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1341,27 +1398,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>123</v>
@@ -1373,13 +1430,13 @@
         <v>789</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -1406,10 +1463,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.2074074074074"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.6962962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3666666666667"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.1851851851852"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.662962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1417,21 +1474,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -1458,66 +1515,66 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="12" width="16.5592592592593"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="12" width="14.7"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="12" width="12.2481481481481"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="12" width="26.262962962963"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="12" width="8.42592592592593"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="12" width="31.5555555555556"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="12" width="29.8888888888889"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="12" width="24.9888888888889"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="12" width="11.3666666666667"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="16.9518518518519"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="14.9925925925926"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="12.4444444444444"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="26.9481481481481"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="13" width="8.52592592592593"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="32.337037037037"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="13" width="30.6703703703704"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="13" width="25.5777777777778"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="13" width="11.662962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="D1" s="14" t="s">
+      <c r="B1" s="14" t="s">
         <v>184</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="C1" s="15" t="s">
         <v>185</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="D1" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="E1" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="F1" s="15" t="s">
         <v>188</v>
       </c>
+      <c r="G1" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
-        <v>189</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="C2" s="14" t="n">
+      <c r="A2" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="C2" s="15" t="n">
         <v>10</v>
       </c>
-      <c r="D2" s="14" t="s">
-        <v>190</v>
-      </c>
-      <c r="E2" s="14" t="n">
+      <c r="D2" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="E2" s="15" t="n">
         <v>100</v>
       </c>
-      <c r="F2" s="14" t="n">
+      <c r="F2" s="15" t="n">
         <v>10</v>
       </c>
-      <c r="G2" s="13" t="n">
+      <c r="G2" s="14" t="n">
         <v>1000</v>
       </c>
-      <c r="H2" s="14" t="n">
+      <c r="H2" s="15" t="n">
         <v>1000</v>
       </c>
     </row>
@@ -1545,10 +1602,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8962962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.6"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.0740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1556,21 +1613,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -1597,13 +1654,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.9666666666667"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.2259259259259"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.7777777777778"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.4555555555556"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.4962962962963"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.2814814814815"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.5851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.7518518518519"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.7148148148148"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1703703703704"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.4333333333333"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.1814814814815"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.8703703703704"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.7777777777778"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1670,13 +1727,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.5851851851852"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.5222222222222"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="16.462962962963"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.9888888888889"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="4" width="16.462962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.5851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.8185185185185"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="16.8555555555556"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.5777777777778"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="4" width="16.8555555555556"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.7777777777778"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1749,7 +1806,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.5851851851852"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.7777777777778"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1835,8 +1892,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.9666666666667"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.5851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.7518518518519"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.7777777777778"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1897,21 +1954,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.5851851851852"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.462962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.2037037037037"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.9111111111111"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="10.5851851851852"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.2074074074074"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.0481481481481"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.3222222222222"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="22.7333333333333"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.23333333333333"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.6037037037037"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="33.9074074074074"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="29.4962962962963"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="30.7703703703704"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="10.5851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.8555555555556"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.8888888888889"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.3037037037037"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.537037037037"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.8111111111111"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.2259259259259"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.32962962962963"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="34.6888888888889"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="30.1814814814815"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="31.5555555555556"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="10.7777777777778"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2032,12 +2089,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7740740740741"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.5555555555556"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.6333333333333"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.8592592592593"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.8074074074074"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.5851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.262962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.2407407407407"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.4148148148148"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="52.1333333333333"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.5925925925926"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.7777777777778"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2256,10 +2313,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2444444444444"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.6333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.5851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.7333333333333"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.2222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.7777777777778"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2308,10 +2365,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.4925925925926"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.7740740740741"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.4333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.3740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.262962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.3148148148148"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3666666666667"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[PHOENIX-5899] Written the scenario for water management data entry screen
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="199">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -458,12 +458,18 @@
     <t xml:space="preserve">applicantInfo</t>
   </si>
   <si>
+    <t xml:space="preserve">21/11/2016</t>
+  </si>
+  <si>
     <t xml:space="preserve">applicantInfo1</t>
   </si>
   <si>
     <t xml:space="preserve">dataEntryInfo</t>
   </si>
   <si>
+    <t xml:space="preserve">07/01/2017</t>
+  </si>
+  <si>
     <t xml:space="preserve">1/2_12.50</t>
   </si>
   <si>
@@ -519,6 +525,9 @@
   </si>
   <si>
     <t xml:space="preserve">Change Of Use</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GENERAL</t>
   </si>
   <si>
     <t xml:space="preserve">DataEntryScreen</t>
@@ -630,15 +639,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
     <numFmt numFmtId="167" formatCode="0.00"/>
     <numFmt numFmtId="168" formatCode="DD/MM/YY"/>
-    <numFmt numFmtId="169" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -673,6 +681,12 @@
       <name val="DejaVu Sans Mono"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -762,11 +776,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1012,14 +1026,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="23.7148148148148"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.7740740740741"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.9296296296296"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="27.9296296296296"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.662962962963"/>
   </cols>
   <sheetData>
@@ -1033,7 +1047,7 @@
       <c r="C1" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>138</v>
       </c>
     </row>
@@ -1047,13 +1061,13 @@
       <c r="C2" s="0" t="n">
         <v>98765</v>
       </c>
-      <c r="D2" s="11" t="n">
-        <v>42695</v>
+      <c r="D2" s="11" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1016039599</v>
@@ -1061,22 +1075,22 @@
       <c r="C3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>1016093135</v>
+        <v>1016093176</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>98765</v>
-      </c>
-      <c r="D4" s="12" t="n">
-        <v>42741</v>
+        <v>5626</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1097,8 +1111,8 @@
   </sheetPr>
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1117,57 +1131,57 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>111</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>114</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>20</v>
@@ -1181,25 +1195,25 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>154</v>
-      </c>
       <c r="E3" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>114</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>25</v>
@@ -1208,21 +1222,21 @@
         <v>4</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>114</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>19</v>
@@ -1231,30 +1245,30 @@
         <v>2</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>114</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>25</v>
@@ -1263,7 +1277,7 @@
         <v>4</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -1306,33 +1320,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1000</v>
@@ -1344,7 +1358,7 @@
         <v>100</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>1234</v>
@@ -1352,7 +1366,7 @@
       <c r="G2" s="0" t="n">
         <v>123456</v>
       </c>
-      <c r="H2" s="11" t="n">
+      <c r="H2" s="12" t="n">
         <v>42689</v>
       </c>
       <c r="I2" s="0" t="n">
@@ -1398,27 +1412,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>123</v>
@@ -1430,13 +1444,13 @@
         <v>789</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -1474,21 +1488,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -1531,39 +1545,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C2" s="15" t="n">
         <v>10</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="E2" s="15" t="n">
         <v>100</v>
@@ -1613,21 +1627,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[PHOENIX-5899] Completed the Creation of new property feature
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="ownerDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="201">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -369,6 +369,12 @@
   </si>
   <si>
     <t xml:space="preserve">S.Ravindra Babu/ADM_Commissioner_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deputyExecutiveEngineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deputy Executive Engineer</t>
   </si>
   <si>
     <t xml:space="preserve">propertyType</t>
@@ -764,6 +770,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -773,10 +783,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -821,13 +827,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.7777777777778"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3037037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.7777777777778"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.2444444444444"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.2444444444444"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.7962962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.7333333333333"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.7333333333333"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.0740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -903,14 +909,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.9814814814815"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="11.3666666666667"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="11.3666666666667"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="20.7740740740741"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.3666666666667"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.962962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="11.662962962963"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="11.662962962963"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="21.262962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.662962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -918,54 +924,54 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>132</v>
+        <v>133</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>134</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>65</v>
@@ -977,10 +983,10 @@
         <v>67</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="H2" s="3" t="n">
         <v>42319</v>
@@ -991,14 +997,14 @@
       <c r="J2" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="K2" s="10" t="n">
+      <c r="K2" s="11" t="n">
         <v>10</v>
       </c>
-      <c r="L2" s="10" t="n">
+      <c r="L2" s="11" t="n">
         <v>20</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="N2" s="3" t="n">
         <v>42358</v>
@@ -1025,16 +1031,15 @@
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="23.7148148148148"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.7740740740741"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="27.9296296296296"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.662962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="24.3037037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.262962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="28.6148148148148"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1042,18 +1047,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1016093139</v>
@@ -1061,13 +1066,13 @@
       <c r="C2" s="0" t="n">
         <v>98765</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>140</v>
+      <c r="D2" s="10" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1016039599</v>
@@ -1081,7 +1086,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1016093176</v>
@@ -1089,8 +1094,8 @@
       <c r="C4" s="0" t="n">
         <v>5626</v>
       </c>
-      <c r="D4" s="11" t="s">
-        <v>143</v>
+      <c r="D4" s="10" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1117,71 +1122,70 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="29.9851851851852"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2259259259259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.8962962962963"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.8555555555556"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.2074074074074"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="29.9851851851852"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.662962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="30.7703703703704"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.7148148148148"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8148148148148"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.4222222222222"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.8148148148148"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="30.7703703703704"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C1" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="G2" s="10" t="s">
         <v>146</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>144</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>20</v>
@@ -1195,25 +1199,25 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>154</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>156</v>
-      </c>
       <c r="E3" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>25</v>
@@ -1222,21 +1226,21 @@
         <v>4</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>19</v>
@@ -1245,30 +1249,30 @@
         <v>2</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>25</v>
@@ -1277,7 +1281,7 @@
         <v>4</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -1304,15 +1308,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="16.9518518518519"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.7740740740741"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.462962962963"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.5592592592593"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.8555555555556"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.6555555555556"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.8518518518519"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.3444444444444"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.662962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.262962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.8555555555556"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.9518518518519"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.2444444444444"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.3444444444444"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.8333333333333"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1320,33 +1323,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
-        <v>173</v>
+      <c r="A2" s="9" t="s">
+        <v>175</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1000</v>
@@ -1358,7 +1361,7 @@
         <v>100</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>1234</v>
@@ -1397,14 +1400,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8148148148148"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.2074074074074"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.5222222222222"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.3037037037037"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.7333333333333"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.8518518518519"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.262962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.662962962963"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.2074074074074"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.9111111111111"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7962962962963"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.2259259259259"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.3444444444444"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.8518518518519"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1412,27 +1414,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>177</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="F1" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="E1" s="10" t="s">
         <v>180</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>123</v>
@@ -1443,14 +1445,14 @@
       <c r="D2" s="0" t="n">
         <v>789</v>
       </c>
-      <c r="E2" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>182</v>
+      <c r="E2" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -1477,32 +1479,31 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6777777777778"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.6962962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.662962962963"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1666666666667"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.1851851851852"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.6777777777778"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>184</v>
+      <c r="B1" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>186</v>
+        <v>187</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -1529,15 +1530,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="16.9518518518519"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="14.9925925925926"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="12.4444444444444"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="26.9481481481481"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="13" width="8.52592592592593"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="32.337037037037"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="13" width="30.6703703703704"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="13" width="25.5777777777778"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="13" width="11.662962962963"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="15.3851851851852"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="27.537037037037"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="13" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="33.1222222222222"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="13" width="31.4555555555556"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="13" width="26.262962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="13" width="11.9555555555556"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1545,39 +1546,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C2" s="15" t="n">
         <v>10</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="E2" s="15" t="n">
         <v>100</v>
@@ -1616,10 +1617,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.462962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="14.8962962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.8555555555556"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3666666666667"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1627,21 +1628,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -1668,13 +1669,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.7518518518519"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.7148148148148"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1703703703704"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.4333333333333"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.1814814814815"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.8703703703704"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.437037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.3037037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.5592592592593"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="38.3148148148148"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.9666666666667"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.5555555555556"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.0740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1741,13 +1742,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.7777777777778"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.8185185185185"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="16.8555555555556"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.5777777777778"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="4" width="16.8555555555556"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.1111111111111"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.262962962963"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="4" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.0740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1820,7 +1821,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.0740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1906,8 +1907,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.7518518518519"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.437037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.0740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1968,21 +1969,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.7777777777778"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.8555555555556"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.8888888888889"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.3037037037037"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="10.7777777777778"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.6962962962963"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.537037037037"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.8111111111111"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.2259259259259"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.32962962962963"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.8"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="34.6888888888889"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="30.1814814814815"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="31.5555555555556"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.6703703703704"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7962962962963"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="11.0740740740741"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.1851851851852"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.0296296296296"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.4"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.7148148148148"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.42592592592593"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="35.5703703703704"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="30.9666666666667"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="32.337037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="11.0740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2095,20 +2096,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.262962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.2407407407407"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.4148148148148"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="52.1333333333333"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.5925925925926"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.8518518518519"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8296296296296"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.2"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.4074074074074"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.4740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.0740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2301,6 +2302,17 @@
       </c>
       <c r="E12" s="0" t="s">
         <v>92</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2327,10 +2339,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.7333333333333"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.2222222222222"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.7777777777778"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.2259259259259"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0296296296296"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.9074074074074"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.0740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2338,21 +2350,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -2379,17 +2391,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.3740740740741"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.262962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.3148148148148"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3666666666667"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.2592592592593"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.8518518518519"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.2962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.662962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="0" t="s">
@@ -2398,7 +2410,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>5000</v>

</xml_diff>

<commit_message>
[PHOENIX-5876] Completed the creation of the new water connection
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="202">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -317,6 +317,12 @@
     <t xml:space="preserve">Forward to commissioner</t>
   </si>
   <si>
+    <t xml:space="preserve">commissioner1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S.Ravindra Babu/ADM_Commissioner_1</t>
+  </si>
+  <si>
     <t xml:space="preserve">engineer</t>
   </si>
   <si>
@@ -365,16 +371,13 @@
     <t xml:space="preserve">D Ramachandra Reddy/ACC_EOA_1</t>
   </si>
   <si>
-    <t xml:space="preserve">commissioner1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S.Ravindra Babu/ADM_Commissioner_1</t>
-  </si>
-  <si>
     <t xml:space="preserve">deputyExecutiveEngineer</t>
   </si>
   <si>
     <t xml:space="preserve">Deputy Executive Engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S.Nayab Rasool/ENG_Dy. Executive Engineer_1</t>
   </si>
   <si>
     <t xml:space="preserve">propertyType</t>
@@ -924,54 +927,54 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>65</v>
@@ -983,10 +986,10 @@
         <v>67</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H2" s="3" t="n">
         <v>42319</v>
@@ -1004,7 +1007,7 @@
         <v>20</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="N2" s="3" t="n">
         <v>42358</v>
@@ -1047,18 +1050,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1016093139</v>
@@ -1067,12 +1070,12 @@
         <v>98765</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1016039599</v>
@@ -1086,7 +1089,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1016093176</v>
@@ -1095,7 +1098,7 @@
         <v>5626</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -1135,57 +1138,57 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>20</v>
@@ -1199,25 +1202,25 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>156</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>159</v>
-      </c>
       <c r="F3" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>25</v>
@@ -1226,21 +1229,21 @@
         <v>4</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>19</v>
@@ -1249,30 +1252,30 @@
         <v>2</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>25</v>
@@ -1281,7 +1284,7 @@
         <v>4</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -1323,33 +1326,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1000</v>
@@ -1361,7 +1364,7 @@
         <v>100</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>1234</v>
@@ -1414,27 +1417,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>123</v>
@@ -1446,13 +1449,13 @@
         <v>789</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -1489,21 +1492,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -1546,39 +1549,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C2" s="15" t="n">
         <v>10</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E2" s="15" t="n">
         <v>100</v>
@@ -1628,21 +1631,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -2096,10 +2099,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
@@ -2197,77 +2200,80 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>93</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="E6" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="B7" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="C7" s="0" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="D7" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="D7" s="0" t="s">
+      <c r="E7" s="0" t="s">
         <v>99</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>103</v>
+      <c r="E8" s="0" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C9" s="0" t="s">
+      <c r="D9" s="0" t="s">
         <v>105</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C10" s="0" t="s">
         <v>107</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>105</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>108</v>
@@ -2275,44 +2281,61 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C11" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>105</v>
-      </c>
       <c r="D11" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="B12" s="0" t="s">
-        <v>89</v>
+      <c r="B12" s="7" t="s">
+        <v>103</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="E12" s="0" t="s">
-        <v>92</v>
-      </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="B13" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="C13" s="8" t="s">
+      <c r="B14" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>112</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -2350,21 +2373,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2410,7 +2433,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>5000</v>

</xml_diff>

<commit_message>
[PHOENIX-5876] working on the water charge management charges
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="ownerDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,6 +25,7 @@
     <sheet name="vltReport" sheetId="15" state="visible" r:id="rId16"/>
     <sheet name="fieldInseptionDetailsForWaterConnection" sheetId="16" state="visible" r:id="rId17"/>
     <sheet name="ptReport" sheetId="17" state="visible" r:id="rId18"/>
+    <sheet name="dataFromWeb" sheetId="18" state="visible" r:id="rId19"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="215">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -467,6 +468,9 @@
     <t xml:space="preserve">applicantInfo</t>
   </si>
   <si>
+    <t xml:space="preserve">1016093856</t>
+  </si>
+  <si>
     <t xml:space="preserve">21/11/2016</t>
   </si>
   <si>
@@ -479,6 +483,15 @@
     <t xml:space="preserve">07/01/2017</t>
   </si>
   <si>
+    <t xml:space="preserve">additionalConnection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1016047933</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
     <t xml:space="preserve">1/2_12.50</t>
   </si>
   <si>
@@ -642,6 +655,33 @@
   </si>
   <si>
     <t xml:space="preserve">10/12/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">message1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">actualMessage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">message</t>
+  </si>
+  <si>
+    <t>1016093858</t>
+  </si>
+  <si>
+    <t>1016093859</t>
+  </si>
+  <si>
+    <t>1016093860</t>
+  </si>
+  <si>
+    <t>1016093861</t>
+  </si>
+  <si>
+    <t>1016093862</t>
+  </si>
+  <si>
+    <t>1016093863</t>
   </si>
 </sst>
 </file>
@@ -655,7 +695,7 @@
     <numFmt numFmtId="167" formatCode="0.00"/>
     <numFmt numFmtId="168" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -690,12 +730,6 @@
       <name val="DejaVu Sans Mono"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -740,7 +774,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -770,10 +804,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -830,13 +860,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.0740740740741"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.7962962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.462962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.0740740740741"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.7333333333333"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.7333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.0740740740741"/>
+    <col min="1" max="1" hidden="false" style="0" width="9.6037037037037" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="24.4" collapsed="true"/>
+    <col min="3" max="3" hidden="false" style="0" width="20.1851851851852" collapsed="true"/>
+    <col min="4" max="4" hidden="false" style="0" width="9.6037037037037" collapsed="true"/>
+    <col min="5" max="5" hidden="false" style="1" width="27.9296296296296" collapsed="true"/>
+    <col min="6" max="6" hidden="false" style="0" width="27.9296296296296" collapsed="true"/>
+    <col min="7" max="1025" hidden="false" style="0" width="9.6037037037037" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -912,14 +942,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.962962962963"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="11.662962962963"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.462962962963"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="11.662962962963"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="21.262962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.662962962963"/>
+    <col min="1" max="1" hidden="false" style="0" width="51.0555555555556" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="19.2074074074074" collapsed="true"/>
+    <col min="3" max="7" hidden="false" style="0" width="9.9962962962963" collapsed="true"/>
+    <col min="8" max="8" hidden="false" style="0" width="20.1851851851852" collapsed="true"/>
+    <col min="9" max="9" hidden="false" style="0" width="21.6555555555556" collapsed="true"/>
+    <col min="10" max="13" hidden="false" style="0" width="9.9962962962963" collapsed="true"/>
+    <col min="14" max="14" hidden="false" style="0" width="26.262962962963" collapsed="true"/>
+    <col min="15" max="1025" hidden="false" style="0" width="9.9962962962963" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -973,7 +1003,7 @@
       <c r="A2" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>135</v>
       </c>
       <c r="C2" s="0" t="s">
@@ -1000,10 +1030,10 @@
       <c r="J2" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="K2" s="11" t="n">
+      <c r="K2" s="10" t="n">
         <v>10</v>
       </c>
-      <c r="L2" s="11" t="n">
+      <c r="L2" s="10" t="n">
         <v>20</v>
       </c>
       <c r="M2" s="2" t="s">
@@ -1032,27 +1062,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="24.3037037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.262962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="28.6148148148148"/>
+    <col min="1" max="1" hidden="false" style="0" width="29.9851851851852" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="1" width="29.9851851851852" collapsed="true"/>
+    <col min="3" max="3" hidden="false" style="1" width="26.262962962963" collapsed="true"/>
+    <col min="4" max="4" hidden="false" style="1" width="35.5703703703704" collapsed="true"/>
+    <col min="5" max="1025" hidden="false" style="0" width="10.1925925925926" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>140</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -1063,24 +1095,24 @@
       <c r="A2" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="B2" s="0" t="n">
-        <v>1016093139</v>
-      </c>
-      <c r="C2" s="0" t="n">
+      <c r="B2" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C2" s="1" t="n">
         <v>98765</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>143</v>
+      <c r="D2" s="9" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="B3" s="0" t="n">
+        <v>145</v>
+      </c>
+      <c r="B3" s="1" t="n">
         <v>1016039599</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>0</v>
       </c>
       <c r="D3" s="1" t="n">
@@ -1089,16 +1121,30 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="B4" s="0" t="n">
+        <v>146</v>
+      </c>
+      <c r="B4" s="1" t="n">
         <v>1016093176</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>5626</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>146</v>
+      <c r="D4" s="9" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -1125,70 +1171,71 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="30.7703703703704"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.7148148148148"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8148148148148"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.4222222222222"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.8148148148148"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.6962962962963"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="30.7703703703704"/>
+    <col min="1" max="2" hidden="false" style="0" width="38.3148148148148" collapsed="true"/>
+    <col min="3" max="3" hidden="false" style="0" width="29.3" collapsed="true"/>
+    <col min="4" max="4" hidden="false" style="0" width="23.2259259259259" collapsed="true"/>
+    <col min="5" max="5" hidden="false" style="0" width="22.7333333333333" collapsed="true"/>
+    <col min="6" max="6" hidden="false" style="0" width="18.8148148148148" collapsed="true"/>
+    <col min="7" max="7" hidden="false" style="0" width="21.1666666666667" collapsed="true"/>
+    <col min="8" max="8" hidden="false" style="0" width="23.2259259259259" collapsed="true"/>
+    <col min="9" max="9" hidden="false" style="0" width="24.3037037037037" collapsed="true"/>
+    <col min="10" max="10" hidden="false" style="0" width="38.3148148148148" collapsed="true"/>
+    <col min="11" max="1025" hidden="false" style="0" width="10.1925925925926" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>114</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
-        <v>156</v>
+      <c r="A2" s="8" t="s">
+        <v>160</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>158</v>
+        <v>161</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>162</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>147</v>
+      <c r="G2" s="9" t="s">
+        <v>151</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>20</v>
@@ -1202,25 +1249,25 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>157</v>
-      </c>
       <c r="C3" s="0" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>117</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>25</v>
@@ -1229,21 +1276,21 @@
         <v>4</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>117</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>19</v>
@@ -1252,30 +1299,30 @@
         <v>2</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>117</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>25</v>
@@ -1284,7 +1331,7 @@
         <v>4</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -1311,14 +1358,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.262962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.8555555555556"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.9518518518519"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.2444444444444"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.3444444444444"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.8333333333333"/>
+    <col min="1" max="2" hidden="false" style="0" width="21.1666666666667" collapsed="true"/>
+    <col min="3" max="3" hidden="false" style="0" width="26.262962962963" collapsed="true"/>
+    <col min="4" max="5" hidden="false" style="0" width="20.6777777777778" collapsed="true"/>
+    <col min="6" max="6" hidden="false" style="0" width="21.1666666666667" collapsed="true"/>
+    <col min="7" max="7" hidden="false" style="0" width="27.3407407407407" collapsed="true"/>
+    <col min="8" max="8" hidden="false" style="0" width="27.537037037037" collapsed="true"/>
+    <col min="9" max="9" hidden="false" style="0" width="28.1259259259259" collapsed="true"/>
+    <col min="10" max="1025" hidden="false" style="0" width="10.1925925925926" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1326,33 +1373,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
-        <v>176</v>
+      <c r="A2" s="8" t="s">
+        <v>180</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1000</v>
@@ -1364,7 +1411,7 @@
         <v>100</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>1234</v>
@@ -1372,7 +1419,7 @@
       <c r="G2" s="0" t="n">
         <v>123456</v>
       </c>
-      <c r="H2" s="12" t="n">
+      <c r="H2" s="11" t="n">
         <v>42689</v>
       </c>
       <c r="I2" s="0" t="n">
@@ -1403,13 +1450,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.2074074074074"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.6962962962963"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.9111111111111"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7962962962963"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.2259259259259"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.3444444444444"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.8518518518519"/>
+    <col min="1" max="1" hidden="false" style="0" width="23.7148148148148" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="24.3037037037037" collapsed="true"/>
+    <col min="3" max="3" hidden="false" style="0" width="23.3222222222222" collapsed="true"/>
+    <col min="4" max="4" hidden="false" style="0" width="24.4" collapsed="true"/>
+    <col min="5" max="5" hidden="false" style="0" width="28.6148148148148" collapsed="true"/>
+    <col min="6" max="6" hidden="false" style="0" width="27.537037037037" collapsed="true"/>
+    <col min="7" max="7" hidden="false" style="0" width="26.9481481481481" collapsed="true"/>
+    <col min="8" max="1025" hidden="false" style="0" width="10.1925925925926" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1417,27 +1465,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>183</v>
+        <v>184</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>123</v>
@@ -1448,14 +1496,14 @@
       <c r="D2" s="0" t="n">
         <v>789</v>
       </c>
-      <c r="E2" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>185</v>
+      <c r="E2" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -1482,31 +1530,32 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1666666666667"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.6777777777778"/>
+    <col min="1" max="1" hidden="false" style="0" width="26.0666666666667" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="24.8888888888889" collapsed="true"/>
+    <col min="3" max="3" hidden="false" style="0" width="25.4777777777778" collapsed="true"/>
+    <col min="4" max="1025" hidden="false" style="0" width="10.1925925925926" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>187</v>
+      <c r="B1" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>189</v>
+        <v>192</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -1533,66 +1582,66 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="15.3851851851852"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="27.537037037037"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="13" width="8.62222222222222"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="33.1222222222222"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="13" width="31.4555555555556"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="13" width="26.262962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="13" width="11.9555555555556"/>
+    <col min="1" max="1" hidden="false" style="12" width="21.1666666666667" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="12" width="18.8148148148148" collapsed="true"/>
+    <col min="3" max="3" hidden="false" style="12" width="15.2888888888889" collapsed="true"/>
+    <col min="4" max="4" hidden="false" style="12" width="34.0037037037037" collapsed="true"/>
+    <col min="5" max="5" hidden="false" style="12" width="10.3888888888889" collapsed="true"/>
+    <col min="6" max="6" hidden="false" style="12" width="41.2555555555556" collapsed="true"/>
+    <col min="7" max="7" hidden="false" style="12" width="39.1" collapsed="true"/>
+    <col min="8" max="8" hidden="false" style="12" width="32.437037037037" collapsed="true"/>
+    <col min="9" max="1025" hidden="false" style="12" width="14.3074074074074" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
-        <v>190</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="F1" s="15" t="s">
+      <c r="B1" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="D1" s="14" t="s">
         <v>196</v>
       </c>
+      <c r="E1" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="C2" s="15" t="n">
+      <c r="A2" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="C2" s="14" t="n">
         <v>10</v>
       </c>
-      <c r="D2" s="15" t="s">
-        <v>198</v>
-      </c>
-      <c r="E2" s="15" t="n">
+      <c r="D2" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="E2" s="14" t="n">
         <v>100</v>
       </c>
-      <c r="F2" s="15" t="n">
+      <c r="F2" s="14" t="n">
         <v>10</v>
       </c>
-      <c r="G2" s="14" t="n">
+      <c r="G2" s="13" t="n">
         <v>1000</v>
       </c>
-      <c r="H2" s="15" t="n">
+      <c r="H2" s="14" t="n">
         <v>1000</v>
       </c>
     </row>
@@ -1620,10 +1669,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.8555555555556"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3666666666667"/>
+    <col min="1" max="1" hidden="false" style="0" width="19.2074074074074" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="1" width="20.6777777777778" collapsed="true"/>
+    <col min="3" max="3" hidden="false" style="1" width="18.8148148148148" collapsed="true"/>
+    <col min="4" max="1025" hidden="false" style="0" width="9.8" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1631,21 +1680,66 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>201</v>
+        <v>205</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col min="1" max="1" hidden="false" style="0" width="16.5592592592593" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="17.2481481481481" collapsed="true"/>
+    <col min="3" max="1025" hidden="false" style="0" width="9.9962962962963" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -1672,13 +1766,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.437037037037"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.3037037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.5592592592593"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="38.3148148148148"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.9666666666667"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.5555555555556"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.0740740740741"/>
+    <col min="1" max="1" hidden="false" style="0" width="40.2740740740741" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="29.9851851851852" collapsed="true"/>
+    <col min="3" max="3" hidden="false" style="0" width="20.1851851851852" collapsed="true"/>
+    <col min="4" max="4" hidden="false" style="0" width="47.7222222222222" collapsed="true"/>
+    <col min="5" max="5" hidden="false" style="0" width="38.3148148148148" collapsed="true"/>
+    <col min="6" max="6" hidden="false" style="0" width="33.0222222222222" collapsed="true"/>
+    <col min="7" max="1025" hidden="false" style="0" width="9.6037037037037" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1745,13 +1839,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.0740740740741"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.1111111111111"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.262962962963"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="4" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.0740740740741"/>
+    <col min="1" max="1" hidden="false" style="0" width="9.6037037037037" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="17.2481481481481" collapsed="true"/>
+    <col min="3" max="4" hidden="false" style="0" width="21.1666666666667" collapsed="true"/>
+    <col min="5" max="5" hidden="false" style="0" width="22.2444444444444" collapsed="true"/>
+    <col min="6" max="6" hidden="false" style="0" width="32.437037037037" collapsed="true"/>
+    <col min="7" max="7" hidden="false" style="4" width="21.1666666666667" collapsed="true"/>
+    <col min="8" max="1025" hidden="false" style="0" width="9.6037037037037" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1824,7 +1918,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.0740740740741"/>
+    <col min="1" max="1025" hidden="false" style="0" width="9.6037037037037" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1910,8 +2004,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.437037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.0740740740741"/>
+    <col min="1" max="1" hidden="false" style="0" width="40.2740740740741" collapsed="true"/>
+    <col min="2" max="1025" hidden="false" style="0" width="9.6037037037037" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1972,21 +2066,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.0740740740741"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.6703703703704"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7962962962963"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="11.0740740740741"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.0296296296296"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.4"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.7148148148148"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.42592592592593"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.9962962962963"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="35.5703703703704"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="30.9666666666667"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="32.337037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="11.0740740740741"/>
+    <col min="1" max="1" hidden="false" style="0" width="9.6037037037037" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="21.1666666666667" collapsed="true"/>
+    <col min="3" max="3" hidden="false" style="0" width="38.2185185185185" collapsed="true"/>
+    <col min="4" max="4" hidden="false" style="0" width="24.4" collapsed="true"/>
+    <col min="5" max="6" hidden="false" style="0" width="9.6037037037037" collapsed="true"/>
+    <col min="7" max="7" hidden="false" style="0" width="24.8888888888889" collapsed="true"/>
+    <col min="8" max="8" hidden="false" style="0" width="28.5148148148148" collapsed="true"/>
+    <col min="9" max="9" hidden="false" style="0" width="30.1814814814815" collapsed="true"/>
+    <col min="10" max="10" hidden="false" style="0" width="29.3" collapsed="true"/>
+    <col min="11" max="11" hidden="false" style="0" width="9.9962962962963" collapsed="true"/>
+    <col min="12" max="12" hidden="false" style="0" width="12.2481481481481" collapsed="true"/>
+    <col min="13" max="13" hidden="false" style="2" width="44.3925925925926" collapsed="true"/>
+    <col min="14" max="14" hidden="false" style="0" width="38.3148148148148" collapsed="true"/>
+    <col min="15" max="15" hidden="false" style="0" width="40.2740740740741" collapsed="true"/>
+    <col min="16" max="1025" hidden="false" style="0" width="9.6037037037037" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2101,18 +2195,18 @@
   </sheetPr>
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.8518518518519"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8296296296296"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.2"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.4074074074074"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.4740740740741"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.0740740740741"/>
+    <col min="1" max="1" hidden="false" style="0" width="26.9481481481481" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="34.5925925925926" collapsed="true"/>
+    <col min="3" max="3" hidden="false" style="0" width="42.6259259259259" collapsed="true"/>
+    <col min="4" max="4" hidden="false" style="0" width="66.8333333333333" collapsed="true"/>
+    <col min="5" max="5" hidden="false" style="0" width="44.1962962962963" collapsed="true"/>
+    <col min="6" max="1025" hidden="false" style="0" width="9.6037037037037" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2362,10 +2456,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.2259259259259"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0296296296296"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.9074074074074"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.0740740740741"/>
+    <col min="1" max="1" hidden="false" style="0" width="28.6148148148148" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="22.2444444444444" collapsed="true"/>
+    <col min="3" max="3" hidden="false" style="0" width="35.8666666666667" collapsed="true"/>
+    <col min="4" max="1025" hidden="false" style="0" width="9.6037037037037" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2414,17 +2508,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.2592592592593"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.8518518518519"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.2962962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.662962962963"/>
+    <col min="1" max="1" hidden="false" style="0" width="45.1740740740741" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="26.9481481481481" collapsed="true"/>
+    <col min="3" max="3" hidden="false" style="0" width="48.9" collapsed="true"/>
+    <col min="4" max="1025" hidden="false" style="0" width="9.9962962962963" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="0" t="s">

</xml_diff>

<commit_message>
[PHOENIX-6015] modified legacy advertisement feature
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="216">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -682,6 +682,9 @@
   </si>
   <si>
     <t>1016093863</t>
+  </si>
+  <si>
+    <t>1016093877</t>
   </si>
 </sst>
 </file>
@@ -1096,7 +1099,7 @@
         <v>142</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>98765</v>

</xml_diff>

<commit_message>
[PHOENIX-5848] Modified property tax testdata sheet
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="217">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -685,6 +685,9 @@
   </si>
   <si>
     <t>1016093877</t>
+  </si>
+  <si>
+    <t>1016093906</t>
   </si>
 </sst>
 </file>
@@ -1099,7 +1102,7 @@
         <v>142</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>98765</v>

</xml_diff>

<commit_message>
[PHOENIX-6053] completed addition alteration screen of property tax
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="ownerDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,666 +28,637 @@
     <sheet name="dataFromWeb" sheetId="18" state="visible" r:id="rId19"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="217">
-  <si>
-    <t xml:space="preserve">dataName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mobileNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ownerName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">emailAddress</t>
-  </si>
-  <si>
-    <t xml:space="preserve">guardianRelation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">guardian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bimal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bimal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Male</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bimal@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Father</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ram</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reasonForCreation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">extentOfSite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">occupancyCertificateNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">registrationDocNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">registrationDocDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assessmentNewProperty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NEW PROPERTY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">locality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">zoneNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wardNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">blockNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">electionWard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">doorNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pincode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">addressOne</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4th colony</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zone-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Election Ward No. 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12/46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lift</t>
-  </si>
-  <si>
-    <t xml:space="preserve">toilets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">waterTap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">electricity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">attachedBathroom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">waterHarvesting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cableConnection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">all</t>
-  </si>
-  <si>
-    <t xml:space="preserve">floorType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">roofType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wallType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">woodType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">defaultConstructionType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Black Stones</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Absheet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BAMBOO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allmixing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">floorNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">classificationOfBuilding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">natureOfUsage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">firmName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">occupancy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">occupantName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">constructionDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">effectiveFromDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unstructuredLand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">length</t>
-  </si>
-  <si>
-    <t xml:space="preserve">breadth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">buildingPermissionNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">buildingPermissionDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plinthAreaInBuildingPlan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">firstFloor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1st floor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Huts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Residence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Owner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11/22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">approverDepartment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">approverDesignation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">approver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">approverRemarks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">billCollector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REVENUE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bill Collector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D.Khasim ~ REV_Bill Collector_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forward to bill collector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">revenueInspector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UD Revenue Inspector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P.Sadiq Hussain ~ UD RI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forward to revenue insoector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">revenueOfficer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revenue Officer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B.Veeraswamy ~ REV_Revenue Officer_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forward to revenue officer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">commissioner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADMINISTRATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Commissioner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S.Ravindra Babu ~ ADM_Commissioner_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forward to commissioner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">commissioner1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S.Ravindra Babu/ADM_Commissioner_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">engineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENGINEERING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assistant Engineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C.Naresh/ENG_Assistant Engineer_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forward to Engineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">engineer1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A.P.Sreenivasulu/ENG_Assistant Engineer_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">accountOfficer1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACCOUNTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assistant Examiner of Accounts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hanuman Prasad ~ ACC_AEOA_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">accountOfficer2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Examiner of Accounts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D Ramachandra Reddy ~ ACC_EOA_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">accountOfficer3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D Ramachandra Reddy/ACC_EOA_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deputyExecutiveEngineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deputy Executive Engineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S.Nayab Rasool/ENG_Dy. Executive Engineer_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">propertyType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">categoryOfOwnership</t>
-  </si>
-  <si>
-    <t xml:space="preserve">residentialPrivate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Residential</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Private</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assessmentAdditionProperty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editfloorNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editclassificationOfBuilding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editnatureOfUsage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editfirmName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editoccupancy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editoccupantName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editconstructionDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editeffectiveFromDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editunstructuredLand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editlength</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editbreadth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editbuildingPermissionNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editbuildingPermissionDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editplinthAreaInBuildingPlan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">firstFloorAdditionaltaration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2nd Floor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Commercial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sunil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33/22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assessmentNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hscNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">connectionDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">applicantInfo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1016093856</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21/11/2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">applicantInfo1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dataEntryInfo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07/01/2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">additionalConnection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1016047933</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1/2_12.50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">waterSourceType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">connectionType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">usageType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hscPipeSize</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sumpCapacity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">noOfPersons</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reasonForAdditionalConn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">connectionInfo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1016 SURFACE WATER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-metered</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RESIDENTIALS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OYT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">connectionInfo1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New Connection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">changeOfUse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NON-RESIDENTIALS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Change Of Use</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GENERAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DataEntryScreen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">monthlyFees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">donationCharges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">meterCost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">meterName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">meterSINo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">previousReading</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lastReadingDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">currentReading</t>
-  </si>
-  <si>
-    <t xml:space="preserve">feeInfo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abcd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">documentNo1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">documentNo2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">documentNo3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">documentDate1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">documentDate2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">documentDate3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">enclosedInfo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">03/12/16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fromDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">toDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">report1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06/12/2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">material</t>
-  </si>
-  <si>
-    <t xml:space="preserve">quantity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unitOfMeasurement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">existingDistributionPipeline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pipelineToHomeDistance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">estimationCharges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inspectionInfo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">report2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07/12/2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10/12/2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">message1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">actualMessage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">message</t>
-  </si>
-  <si>
-    <t>1016093858</t>
-  </si>
-  <si>
-    <t>1016093859</t>
-  </si>
-  <si>
-    <t>1016093860</t>
-  </si>
-  <si>
-    <t>1016093861</t>
-  </si>
-  <si>
-    <t>1016093862</t>
-  </si>
-  <si>
-    <t>1016093863</t>
-  </si>
-  <si>
-    <t>1016093877</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="209">
+  <si>
+    <t>dataName</t>
+  </si>
+  <si>
+    <t>mobileNumber</t>
+  </si>
+  <si>
+    <t>ownerName</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>emailAddress</t>
+  </si>
+  <si>
+    <t>guardianRelation</t>
+  </si>
+  <si>
+    <t>guardian</t>
+  </si>
+  <si>
+    <t>bimal</t>
+  </si>
+  <si>
+    <t>Bimal</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>bimal@gmail.com</t>
+  </si>
+  <si>
+    <t>Father</t>
+  </si>
+  <si>
+    <t>Ram</t>
+  </si>
+  <si>
+    <t>reasonForCreation</t>
+  </si>
+  <si>
+    <t>extentOfSite</t>
+  </si>
+  <si>
+    <t>occupancyCertificateNumber</t>
+  </si>
+  <si>
+    <t>registrationDocNumber</t>
+  </si>
+  <si>
+    <t>registrationDocDate</t>
+  </si>
+  <si>
+    <t>assessmentNewProperty</t>
+  </si>
+  <si>
+    <t>NEW PROPERTY</t>
+  </si>
+  <si>
+    <t>locality</t>
+  </si>
+  <si>
+    <t>zoneNumber</t>
+  </si>
+  <si>
+    <t>wardNumber</t>
+  </si>
+  <si>
+    <t>blockNumber</t>
+  </si>
+  <si>
+    <t>electionWard</t>
+  </si>
+  <si>
+    <t>doorNumber</t>
+  </si>
+  <si>
+    <t>pincode</t>
+  </si>
+  <si>
+    <t>addressOne</t>
+  </si>
+  <si>
+    <t>4th colony</t>
+  </si>
+  <si>
+    <t>Zone-1</t>
+  </si>
+  <si>
+    <t>Election Ward No. 1</t>
+  </si>
+  <si>
+    <t>12/46</t>
+  </si>
+  <si>
+    <t>lift</t>
+  </si>
+  <si>
+    <t>toilets</t>
+  </si>
+  <si>
+    <t>waterTap</t>
+  </si>
+  <si>
+    <t>electricity</t>
+  </si>
+  <si>
+    <t>attachedBathroom</t>
+  </si>
+  <si>
+    <t>waterHarvesting</t>
+  </si>
+  <si>
+    <t>cableConnection</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>floorType</t>
+  </si>
+  <si>
+    <t>roofType</t>
+  </si>
+  <si>
+    <t>wallType</t>
+  </si>
+  <si>
+    <t>woodType</t>
+  </si>
+  <si>
+    <t>defaultConstructionType</t>
+  </si>
+  <si>
+    <t>Black Stones</t>
+  </si>
+  <si>
+    <t>Absheet</t>
+  </si>
+  <si>
+    <t>BAMBOO</t>
+  </si>
+  <si>
+    <t>Allmixing</t>
+  </si>
+  <si>
+    <t>floorNumber</t>
+  </si>
+  <si>
+    <t>classificationOfBuilding</t>
+  </si>
+  <si>
+    <t>natureOfUsage</t>
+  </si>
+  <si>
+    <t>firmName</t>
+  </si>
+  <si>
+    <t>occupancy</t>
+  </si>
+  <si>
+    <t>occupantName</t>
+  </si>
+  <si>
+    <t>constructionDate</t>
+  </si>
+  <si>
+    <t>effectiveFromDate</t>
+  </si>
+  <si>
+    <t>unstructuredLand</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>breadth</t>
+  </si>
+  <si>
+    <t>buildingPermissionNumber</t>
+  </si>
+  <si>
+    <t>buildingPermissionDate</t>
+  </si>
+  <si>
+    <t>plinthAreaInBuildingPlan</t>
+  </si>
+  <si>
+    <t>firstFloor</t>
+  </si>
+  <si>
+    <t>1st floor</t>
+  </si>
+  <si>
+    <t>Huts</t>
+  </si>
+  <si>
+    <t>Residence</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>11/22</t>
+  </si>
+  <si>
+    <t>approverDepartment</t>
+  </si>
+  <si>
+    <t>approverDesignation</t>
+  </si>
+  <si>
+    <t>approver</t>
+  </si>
+  <si>
+    <t>approverRemarks</t>
+  </si>
+  <si>
+    <t>billCollector</t>
+  </si>
+  <si>
+    <t>REVENUE</t>
+  </si>
+  <si>
+    <t>Bill Collector</t>
+  </si>
+  <si>
+    <t>D.Khasim ~ REV_Bill Collector_1</t>
+  </si>
+  <si>
+    <t>Forward to bill collector</t>
+  </si>
+  <si>
+    <t>revenueInspector</t>
+  </si>
+  <si>
+    <t>UD Revenue Inspector</t>
+  </si>
+  <si>
+    <t>P.Sadiq Hussain ~ UD RI</t>
+  </si>
+  <si>
+    <t>Forward to revenue insoector</t>
+  </si>
+  <si>
+    <t>revenueOfficer</t>
+  </si>
+  <si>
+    <t>Revenue Officer</t>
+  </si>
+  <si>
+    <t>B.Veeraswamy ~ REV_Revenue Officer_3</t>
+  </si>
+  <si>
+    <t>Forward to revenue officer</t>
+  </si>
+  <si>
+    <t>commissioner</t>
+  </si>
+  <si>
+    <t>ADMINISTRATION</t>
+  </si>
+  <si>
+    <t>Commissioner</t>
+  </si>
+  <si>
+    <t>S.Ravindra Babu ~ ADM_Commissioner_1</t>
+  </si>
+  <si>
+    <t>Forward to commissioner</t>
+  </si>
+  <si>
+    <t>commissioner1</t>
+  </si>
+  <si>
+    <t>S.Ravindra Babu/ADM_Commissioner_1</t>
+  </si>
+  <si>
+    <t>engineer</t>
+  </si>
+  <si>
+    <t>ENGINEERING</t>
+  </si>
+  <si>
+    <t>Assistant Engineer</t>
+  </si>
+  <si>
+    <t>C.Naresh/ENG_Assistant Engineer_4</t>
+  </si>
+  <si>
+    <t>Forward to Engineer</t>
+  </si>
+  <si>
+    <t>engineer1</t>
+  </si>
+  <si>
+    <t>A.P.Sreenivasulu/ENG_Assistant Engineer_1</t>
+  </si>
+  <si>
+    <t>accountOfficer1</t>
+  </si>
+  <si>
+    <t>ACCOUNTS</t>
+  </si>
+  <si>
+    <t>Assistant Examiner of Accounts</t>
+  </si>
+  <si>
+    <t>Hanuman Prasad ~ ACC_AEOA_1</t>
+  </si>
+  <si>
+    <t>accountOfficer2</t>
+  </si>
+  <si>
+    <t>Examiner of Accounts</t>
+  </si>
+  <si>
+    <t>D Ramachandra Reddy ~ ACC_EOA_1</t>
+  </si>
+  <si>
+    <t>accountOfficer3</t>
+  </si>
+  <si>
+    <t>D Ramachandra Reddy/ACC_EOA_1</t>
+  </si>
+  <si>
+    <t>deputyExecutiveEngineer</t>
+  </si>
+  <si>
+    <t>Deputy Executive Engineer</t>
+  </si>
+  <si>
+    <t>S.Nayab Rasool/ENG_Dy. Executive Engineer_1</t>
+  </si>
+  <si>
+    <t>propertyType</t>
+  </si>
+  <si>
+    <t>categoryOfOwnership</t>
+  </si>
+  <si>
+    <t>residentialPrivate</t>
+  </si>
+  <si>
+    <t>Residential</t>
+  </si>
+  <si>
+    <t>Private</t>
+  </si>
+  <si>
+    <t>assessmentAdditionProperty</t>
+  </si>
+  <si>
+    <t>editfloorNumber</t>
+  </si>
+  <si>
+    <t>editclassificationOfBuilding</t>
+  </si>
+  <si>
+    <t>editnatureOfUsage</t>
+  </si>
+  <si>
+    <t>editfirmName</t>
+  </si>
+  <si>
+    <t>editoccupancy</t>
+  </si>
+  <si>
+    <t>editoccupantName</t>
+  </si>
+  <si>
+    <t>editconstructionDate</t>
+  </si>
+  <si>
+    <t>editeffectiveFromDate</t>
+  </si>
+  <si>
+    <t>editunstructuredLand</t>
+  </si>
+  <si>
+    <t>editlength</t>
+  </si>
+  <si>
+    <t>editbreadth</t>
+  </si>
+  <si>
+    <t>editbuildingPermissionNumber</t>
+  </si>
+  <si>
+    <t>editbuildingPermissionDate</t>
+  </si>
+  <si>
+    <t>editplinthAreaInBuildingPlan</t>
+  </si>
+  <si>
+    <t>firstFloorAdditionaltaration</t>
+  </si>
+  <si>
+    <t>2nd Floor</t>
+  </si>
+  <si>
+    <t>Commercial</t>
+  </si>
+  <si>
+    <t>Sunil</t>
+  </si>
+  <si>
+    <t>33/22</t>
+  </si>
+  <si>
+    <t>assessmentNumber</t>
+  </si>
+  <si>
+    <t>hscNumber</t>
+  </si>
+  <si>
+    <t>connectionDate</t>
+  </si>
+  <si>
+    <t>applicantInfo</t>
   </si>
   <si>
     <t>1016093906</t>
+  </si>
+  <si>
+    <t>21/11/2016</t>
+  </si>
+  <si>
+    <t>applicantInfo1</t>
+  </si>
+  <si>
+    <t>dataEntryInfo</t>
+  </si>
+  <si>
+    <t>07/01/2017</t>
+  </si>
+  <si>
+    <t>additionalConnection</t>
+  </si>
+  <si>
+    <t>1016047933</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1/2_12.50</t>
+  </si>
+  <si>
+    <t>waterSourceType</t>
+  </si>
+  <si>
+    <t>connectionType</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>usageType</t>
+  </si>
+  <si>
+    <t>hscPipeSize</t>
+  </si>
+  <si>
+    <t>sumpCapacity</t>
+  </si>
+  <si>
+    <t>noOfPersons</t>
+  </si>
+  <si>
+    <t>reasonForAdditionalConn</t>
+  </si>
+  <si>
+    <t>connectionInfo</t>
+  </si>
+  <si>
+    <t>1016 SURFACE WATER</t>
+  </si>
+  <si>
+    <t>Non-metered</t>
+  </si>
+  <si>
+    <t>RESIDENTIALS</t>
+  </si>
+  <si>
+    <t>OYT</t>
+  </si>
+  <si>
+    <t>connectionInfo1</t>
+  </si>
+  <si>
+    <t>New Connection</t>
+  </si>
+  <si>
+    <t>changeOfUse</t>
+  </si>
+  <si>
+    <t>NON-RESIDENTIALS</t>
+  </si>
+  <si>
+    <t>Change Of Use</t>
+  </si>
+  <si>
+    <t>GENERAL</t>
+  </si>
+  <si>
+    <t>DataEntryScreen</t>
+  </si>
+  <si>
+    <t>monthlyFees</t>
+  </si>
+  <si>
+    <t>donationCharges</t>
+  </si>
+  <si>
+    <t>meterCost</t>
+  </si>
+  <si>
+    <t>meterName</t>
+  </si>
+  <si>
+    <t>meterSINo</t>
+  </si>
+  <si>
+    <t>previousReading</t>
+  </si>
+  <si>
+    <t>lastReadingDate</t>
+  </si>
+  <si>
+    <t>currentReading</t>
+  </si>
+  <si>
+    <t>feeInfo</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>documentNo1</t>
+  </si>
+  <si>
+    <t>documentNo2</t>
+  </si>
+  <si>
+    <t>documentNo3</t>
+  </si>
+  <si>
+    <t>documentDate1</t>
+  </si>
+  <si>
+    <t>documentDate2</t>
+  </si>
+  <si>
+    <t>documentDate3</t>
+  </si>
+  <si>
+    <t>enclosedInfo</t>
+  </si>
+  <si>
+    <t>03/12/16</t>
+  </si>
+  <si>
+    <t>fromDate</t>
+  </si>
+  <si>
+    <t>toDate</t>
+  </si>
+  <si>
+    <t>report1</t>
+  </si>
+  <si>
+    <t>06/12/2016</t>
+  </si>
+  <si>
+    <t>material</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>unitOfMeasurement</t>
+  </si>
+  <si>
+    <t>rate</t>
+  </si>
+  <si>
+    <t>existingDistributionPipeline</t>
+  </si>
+  <si>
+    <t>pipelineToHomeDistance</t>
+  </si>
+  <si>
+    <t>estimationCharges</t>
+  </si>
+  <si>
+    <t>inspectionInfo</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>report2</t>
+  </si>
+  <si>
+    <t>07/12/2016</t>
+  </si>
+  <si>
+    <t>10/12/2016</t>
+  </si>
+  <si>
+    <t>message1</t>
+  </si>
+  <si>
+    <t>actualMessage</t>
+  </si>
+  <si>
+    <t>message</t>
   </si>
 </sst>
 </file>
@@ -695,7 +666,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
     <numFmt numFmtId="167" formatCode="0.00"/>
@@ -734,7 +705,7 @@
     <font>
       <sz val="12"/>
       <name val="DejaVu Sans Mono"/>
-      <family val="0"/>
+      <family val="3"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -780,12 +751,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -814,10 +785,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -860,19 +827,18 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="9.6037037037037" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="0" width="24.4" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="0" width="20.1851851851852" collapsed="true"/>
-    <col min="4" max="4" hidden="false" style="0" width="9.6037037037037" collapsed="true"/>
-    <col min="5" max="5" hidden="false" style="1" width="27.9296296296296" collapsed="true"/>
-    <col min="6" max="6" hidden="false" style="0" width="27.9296296296296" collapsed="true"/>
-    <col min="7" max="1025" hidden="false" style="0" width="9.6037037037037" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.4"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.1851851851852"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="27.9296296296296"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -898,12 +864,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>9878976543</v>
+        <v>2299087661</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>8</v>
@@ -923,11 +889,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="Bimal@gmail.com"/>
+    <hyperlink ref="E2" r:id="rId1" display="bimal@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -948,14 +914,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="51.0555555555556" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="0" width="19.2074074074074" collapsed="true"/>
-    <col min="3" max="7" hidden="false" style="0" width="9.9962962962963" collapsed="true"/>
-    <col min="8" max="8" hidden="false" style="0" width="20.1851851851852" collapsed="true"/>
-    <col min="9" max="9" hidden="false" style="0" width="21.6555555555556" collapsed="true"/>
-    <col min="10" max="13" hidden="false" style="0" width="9.9962962962963" collapsed="true"/>
-    <col min="14" max="14" hidden="false" style="0" width="26.262962962963" collapsed="true"/>
-    <col min="15" max="1025" hidden="false" style="0" width="9.9962962962963" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="51.0555555555556"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.2074074074074"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.1851851851852"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="26.262962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1009,7 +975,7 @@
       <c r="A2" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="1" t="s">
         <v>135</v>
       </c>
       <c r="C2" s="0" t="s">
@@ -1036,10 +1002,10 @@
       <c r="J2" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="K2" s="10" t="n">
+      <c r="K2" s="9" t="n">
         <v>10</v>
       </c>
-      <c r="L2" s="10" t="n">
+      <c r="L2" s="9" t="n">
         <v>20</v>
       </c>
       <c r="M2" s="2" t="s">
@@ -1055,7 +1021,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -1070,17 +1036,17 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="29.9851851851852" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="1" width="29.9851851851852" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="1" width="26.262962962963" collapsed="true"/>
-    <col min="4" max="4" hidden="false" style="1" width="35.5703703703704" collapsed="true"/>
-    <col min="5" max="1025" hidden="false" style="0" width="10.1925925925926" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.9851851851852"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="29.9851851851852"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="26.262962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="35.5703703703704"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.1925925925926"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1102,12 +1068,12 @@
         <v>142</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>216</v>
+        <v>143</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>98765</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="1" t="s">
         <v>144</v>
       </c>
     </row>
@@ -1135,7 +1101,7 @@
       <c r="C4" s="1" t="n">
         <v>5626</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="1" t="s">
         <v>147</v>
       </c>
     </row>
@@ -1143,7 +1109,7 @@
       <c r="A5" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="1" t="s">
         <v>149</v>
       </c>
       <c r="C5" s="1" t="n">
@@ -1156,7 +1122,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -1177,16 +1143,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" hidden="false" style="0" width="38.3148148148148" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="0" width="29.3" collapsed="true"/>
-    <col min="4" max="4" hidden="false" style="0" width="23.2259259259259" collapsed="true"/>
-    <col min="5" max="5" hidden="false" style="0" width="22.7333333333333" collapsed="true"/>
-    <col min="6" max="6" hidden="false" style="0" width="18.8148148148148" collapsed="true"/>
-    <col min="7" max="7" hidden="false" style="0" width="21.1666666666667" collapsed="true"/>
-    <col min="8" max="8" hidden="false" style="0" width="23.2259259259259" collapsed="true"/>
-    <col min="9" max="9" hidden="false" style="0" width="24.3037037037037" collapsed="true"/>
-    <col min="10" max="10" hidden="false" style="0" width="38.3148148148148" collapsed="true"/>
-    <col min="11" max="1025" hidden="false" style="0" width="10.1925925925926" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="38.3148148148148"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.3"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.2259259259259"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.7333333333333"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.8148148148148"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.1666666666667"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.2259259259259"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.3037037037037"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="38.3148148148148"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="10.1925925925926"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1240,7 +1206,7 @@
       <c r="F2" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="1" t="s">
         <v>151</v>
       </c>
       <c r="H2" s="0" t="n">
@@ -1343,7 +1309,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -1364,14 +1330,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" hidden="false" style="0" width="21.1666666666667" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="0" width="26.262962962963" collapsed="true"/>
-    <col min="4" max="5" hidden="false" style="0" width="20.6777777777778" collapsed="true"/>
-    <col min="6" max="6" hidden="false" style="0" width="21.1666666666667" collapsed="true"/>
-    <col min="7" max="7" hidden="false" style="0" width="27.3407407407407" collapsed="true"/>
-    <col min="8" max="8" hidden="false" style="0" width="27.537037037037" collapsed="true"/>
-    <col min="9" max="9" hidden="false" style="0" width="28.1259259259259" collapsed="true"/>
-    <col min="10" max="1025" hidden="false" style="0" width="10.1925925925926" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="21.1666666666667"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.262962962963"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.1666666666667"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.3407407407407"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.537037037037"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="28.1259259259259"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.1925925925926"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1425,7 +1391,7 @@
       <c r="G2" s="0" t="n">
         <v>123456</v>
       </c>
-      <c r="H2" s="11" t="n">
+      <c r="H2" s="10" t="n">
         <v>42689</v>
       </c>
       <c r="I2" s="0" t="n">
@@ -1435,7 +1401,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -1456,14 +1422,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="23.7148148148148" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="0" width="24.3037037037037" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="0" width="23.3222222222222" collapsed="true"/>
-    <col min="4" max="4" hidden="false" style="0" width="24.4" collapsed="true"/>
-    <col min="5" max="5" hidden="false" style="0" width="28.6148148148148" collapsed="true"/>
-    <col min="6" max="6" hidden="false" style="0" width="27.537037037037" collapsed="true"/>
-    <col min="7" max="7" hidden="false" style="0" width="26.9481481481481" collapsed="true"/>
-    <col min="8" max="1025" hidden="false" style="0" width="10.1925925925926" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.7148148148148"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.3037037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.3222222222222"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.4"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.6148148148148"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.537037037037"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.9481481481481"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.1925925925926"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1479,13 +1445,13 @@
       <c r="D1" s="0" t="s">
         <v>184</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="1" t="s">
         <v>187</v>
       </c>
     </row>
@@ -1502,20 +1468,20 @@
       <c r="D2" s="0" t="n">
         <v>789</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="1" t="s">
         <v>189</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -1536,20 +1502,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="26.0666666666667" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="0" width="24.8888888888889" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="0" width="25.4777777777778" collapsed="true"/>
-    <col min="4" max="1025" hidden="false" style="0" width="10.1925925925926" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.0666666666667"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.8888888888889"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.4777777777778"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.1925925925926"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="1" t="s">
         <v>191</v>
       </c>
     </row>
@@ -1557,17 +1523,17 @@
       <c r="A2" s="0" t="s">
         <v>192</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="1" t="s">
         <v>193</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -1588,73 +1554,73 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="12" width="21.1666666666667" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="12" width="18.8148148148148" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="12" width="15.2888888888889" collapsed="true"/>
-    <col min="4" max="4" hidden="false" style="12" width="34.0037037037037" collapsed="true"/>
-    <col min="5" max="5" hidden="false" style="12" width="10.3888888888889" collapsed="true"/>
-    <col min="6" max="6" hidden="false" style="12" width="41.2555555555556" collapsed="true"/>
-    <col min="7" max="7" hidden="false" style="12" width="39.1" collapsed="true"/>
-    <col min="8" max="8" hidden="false" style="12" width="32.437037037037" collapsed="true"/>
-    <col min="9" max="1025" hidden="false" style="12" width="14.3074074074074" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="11" width="21.1666666666667"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="11" width="18.8148148148148"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="11" width="34.0037037037037"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="11" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="41.2555555555556"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="11" width="39.1"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="11" width="32.437037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="11" width="14.3074074074074"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="13" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="C2" s="14" t="n">
+      <c r="C2" s="13" t="n">
         <v>10</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="E2" s="14" t="n">
+      <c r="E2" s="13" t="n">
         <v>100</v>
       </c>
-      <c r="F2" s="14" t="n">
+      <c r="F2" s="13" t="n">
         <v>10</v>
       </c>
-      <c r="G2" s="13" t="n">
+      <c r="G2" s="12" t="n">
         <v>1000</v>
       </c>
-      <c r="H2" s="14" t="n">
+      <c r="H2" s="13" t="n">
         <v>1000</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -1675,10 +1641,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="19.2074074074074" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="1" width="20.6777777777778" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="1" width="18.8148148148148" collapsed="true"/>
-    <col min="4" max="1025" hidden="false" style="0" width="9.8" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.2074074074074"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.8148148148148"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1706,7 +1672,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -1727,9 +1693,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="16.5592592592593" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="0" width="17.2481481481481" collapsed="true"/>
-    <col min="3" max="1025" hidden="false" style="0" width="9.9962962962963" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.5592592592593"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1751,7 +1717,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -1772,13 +1738,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="40.2740740740741" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="0" width="29.9851851851852" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="0" width="20.1851851851852" collapsed="true"/>
-    <col min="4" max="4" hidden="false" style="0" width="47.7222222222222" collapsed="true"/>
-    <col min="5" max="5" hidden="false" style="0" width="38.3148148148148" collapsed="true"/>
-    <col min="6" max="6" hidden="false" style="0" width="33.0222222222222" collapsed="true"/>
-    <col min="7" max="1025" hidden="false" style="0" width="9.6037037037037" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.2740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.9851851851852"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.1851851851852"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.7222222222222"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="38.3148148148148"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.0222222222222"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1824,7 +1790,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1845,13 +1811,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="9.6037037037037" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="0" width="17.2481481481481" collapsed="true"/>
-    <col min="3" max="4" hidden="false" style="0" width="21.1666666666667" collapsed="true"/>
-    <col min="5" max="5" hidden="false" style="0" width="22.2444444444444" collapsed="true"/>
-    <col min="6" max="6" hidden="false" style="0" width="32.437037037037" collapsed="true"/>
-    <col min="7" max="7" hidden="false" style="4" width="21.1666666666667" collapsed="true"/>
-    <col min="8" max="1025" hidden="false" style="0" width="9.6037037037037" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="21.1666666666667"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.2444444444444"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.437037037037"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="4" width="21.1666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1903,7 +1869,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1924,7 +1890,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1025" hidden="false" style="0" width="9.6037037037037" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1989,7 +1955,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2010,8 +1976,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="40.2740740740741" collapsed="true"/>
-    <col min="2" max="1025" hidden="false" style="0" width="9.6037037037037" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.2740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2051,7 +2017,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2072,21 +2038,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="9.6037037037037" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="0" width="21.1666666666667" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="0" width="38.2185185185185" collapsed="true"/>
-    <col min="4" max="4" hidden="false" style="0" width="24.4" collapsed="true"/>
-    <col min="5" max="6" hidden="false" style="0" width="9.6037037037037" collapsed="true"/>
-    <col min="7" max="7" hidden="false" style="0" width="24.8888888888889" collapsed="true"/>
-    <col min="8" max="8" hidden="false" style="0" width="28.5148148148148" collapsed="true"/>
-    <col min="9" max="9" hidden="false" style="0" width="30.1814814814815" collapsed="true"/>
-    <col min="10" max="10" hidden="false" style="0" width="29.3" collapsed="true"/>
-    <col min="11" max="11" hidden="false" style="0" width="9.9962962962963" collapsed="true"/>
-    <col min="12" max="12" hidden="false" style="0" width="12.2481481481481" collapsed="true"/>
-    <col min="13" max="13" hidden="false" style="2" width="44.3925925925926" collapsed="true"/>
-    <col min="14" max="14" hidden="false" style="0" width="38.3148148148148" collapsed="true"/>
-    <col min="15" max="15" hidden="false" style="0" width="40.2740740740741" collapsed="true"/>
-    <col min="16" max="1025" hidden="false" style="0" width="9.6037037037037" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1666666666667"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.2185185185185"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.4"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.8888888888889"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.5148148148148"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="30.1814814814815"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="29.3"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.2481481481481"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="44.3925925925926"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="38.3148148148148"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="40.2740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2186,7 +2152,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2207,12 +2173,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="26.9481481481481" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="0" width="34.5925925925926" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="0" width="42.6259259259259" collapsed="true"/>
-    <col min="4" max="4" hidden="false" style="0" width="66.8333333333333" collapsed="true"/>
-    <col min="5" max="5" hidden="false" style="0" width="44.1962962962963" collapsed="true"/>
-    <col min="6" max="1025" hidden="false" style="0" width="9.6037037037037" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.9481481481481"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.5925925925926"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.6259259259259"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="66.8333333333333"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="44.1962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2441,7 +2407,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2462,10 +2428,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="28.6148148148148" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="0" width="22.2444444444444" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="0" width="35.8666666666667" collapsed="true"/>
-    <col min="4" max="1025" hidden="false" style="0" width="9.6037037037037" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.6148148148148"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.2444444444444"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.8666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2493,7 +2459,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2514,10 +2480,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="45.1740740740741" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="0" width="26.9481481481481" collapsed="true"/>
-    <col min="3" max="3" hidden="false" style="0" width="48.9" collapsed="true"/>
-    <col min="4" max="1025" hidden="false" style="0" width="9.9962962962963" collapsed="true"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.1740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.9481481481481"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="48.9"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2545,7 +2511,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
[PHOENIX-5876] refactoring the water charge management module
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="ownerDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,637 +28,648 @@
     <sheet name="dataFromWeb" sheetId="18" state="visible" r:id="rId19"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="209">
-  <si>
-    <t>dataName</t>
-  </si>
-  <si>
-    <t>mobileNumber</t>
-  </si>
-  <si>
-    <t>ownerName</t>
-  </si>
-  <si>
-    <t>gender</t>
-  </si>
-  <si>
-    <t>emailAddress</t>
-  </si>
-  <si>
-    <t>guardianRelation</t>
-  </si>
-  <si>
-    <t>guardian</t>
-  </si>
-  <si>
-    <t>bimal</t>
-  </si>
-  <si>
-    <t>Bimal</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>bimal@gmail.com</t>
-  </si>
-  <si>
-    <t>Father</t>
-  </si>
-  <si>
-    <t>Ram</t>
-  </si>
-  <si>
-    <t>reasonForCreation</t>
-  </si>
-  <si>
-    <t>extentOfSite</t>
-  </si>
-  <si>
-    <t>occupancyCertificateNumber</t>
-  </si>
-  <si>
-    <t>registrationDocNumber</t>
-  </si>
-  <si>
-    <t>registrationDocDate</t>
-  </si>
-  <si>
-    <t>assessmentNewProperty</t>
-  </si>
-  <si>
-    <t>NEW PROPERTY</t>
-  </si>
-  <si>
-    <t>locality</t>
-  </si>
-  <si>
-    <t>zoneNumber</t>
-  </si>
-  <si>
-    <t>wardNumber</t>
-  </si>
-  <si>
-    <t>blockNumber</t>
-  </si>
-  <si>
-    <t>electionWard</t>
-  </si>
-  <si>
-    <t>doorNumber</t>
-  </si>
-  <si>
-    <t>pincode</t>
-  </si>
-  <si>
-    <t>addressOne</t>
-  </si>
-  <si>
-    <t>4th colony</t>
-  </si>
-  <si>
-    <t>Zone-1</t>
-  </si>
-  <si>
-    <t>Election Ward No. 1</t>
-  </si>
-  <si>
-    <t>12/46</t>
-  </si>
-  <si>
-    <t>lift</t>
-  </si>
-  <si>
-    <t>toilets</t>
-  </si>
-  <si>
-    <t>waterTap</t>
-  </si>
-  <si>
-    <t>electricity</t>
-  </si>
-  <si>
-    <t>attachedBathroom</t>
-  </si>
-  <si>
-    <t>waterHarvesting</t>
-  </si>
-  <si>
-    <t>cableConnection</t>
-  </si>
-  <si>
-    <t>all</t>
-  </si>
-  <si>
-    <t>floorType</t>
-  </si>
-  <si>
-    <t>roofType</t>
-  </si>
-  <si>
-    <t>wallType</t>
-  </si>
-  <si>
-    <t>woodType</t>
-  </si>
-  <si>
-    <t>defaultConstructionType</t>
-  </si>
-  <si>
-    <t>Black Stones</t>
-  </si>
-  <si>
-    <t>Absheet</t>
-  </si>
-  <si>
-    <t>BAMBOO</t>
-  </si>
-  <si>
-    <t>Allmixing</t>
-  </si>
-  <si>
-    <t>floorNumber</t>
-  </si>
-  <si>
-    <t>classificationOfBuilding</t>
-  </si>
-  <si>
-    <t>natureOfUsage</t>
-  </si>
-  <si>
-    <t>firmName</t>
-  </si>
-  <si>
-    <t>occupancy</t>
-  </si>
-  <si>
-    <t>occupantName</t>
-  </si>
-  <si>
-    <t>constructionDate</t>
-  </si>
-  <si>
-    <t>effectiveFromDate</t>
-  </si>
-  <si>
-    <t>unstructuredLand</t>
-  </si>
-  <si>
-    <t>length</t>
-  </si>
-  <si>
-    <t>breadth</t>
-  </si>
-  <si>
-    <t>buildingPermissionNumber</t>
-  </si>
-  <si>
-    <t>buildingPermissionDate</t>
-  </si>
-  <si>
-    <t>plinthAreaInBuildingPlan</t>
-  </si>
-  <si>
-    <t>firstFloor</t>
-  </si>
-  <si>
-    <t>1st floor</t>
-  </si>
-  <si>
-    <t>Huts</t>
-  </si>
-  <si>
-    <t>Residence</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>Owner</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>11/22</t>
-  </si>
-  <si>
-    <t>approverDepartment</t>
-  </si>
-  <si>
-    <t>approverDesignation</t>
-  </si>
-  <si>
-    <t>approver</t>
-  </si>
-  <si>
-    <t>approverRemarks</t>
-  </si>
-  <si>
-    <t>billCollector</t>
-  </si>
-  <si>
-    <t>REVENUE</t>
-  </si>
-  <si>
-    <t>Bill Collector</t>
-  </si>
-  <si>
-    <t>D.Khasim ~ REV_Bill Collector_1</t>
-  </si>
-  <si>
-    <t>Forward to bill collector</t>
-  </si>
-  <si>
-    <t>revenueInspector</t>
-  </si>
-  <si>
-    <t>UD Revenue Inspector</t>
-  </si>
-  <si>
-    <t>P.Sadiq Hussain ~ UD RI</t>
-  </si>
-  <si>
-    <t>Forward to revenue insoector</t>
-  </si>
-  <si>
-    <t>revenueOfficer</t>
-  </si>
-  <si>
-    <t>Revenue Officer</t>
-  </si>
-  <si>
-    <t>B.Veeraswamy ~ REV_Revenue Officer_3</t>
-  </si>
-  <si>
-    <t>Forward to revenue officer</t>
-  </si>
-  <si>
-    <t>commissioner</t>
-  </si>
-  <si>
-    <t>ADMINISTRATION</t>
-  </si>
-  <si>
-    <t>Commissioner</t>
-  </si>
-  <si>
-    <t>S.Ravindra Babu ~ ADM_Commissioner_1</t>
-  </si>
-  <si>
-    <t>Forward to commissioner</t>
-  </si>
-  <si>
-    <t>commissioner1</t>
-  </si>
-  <si>
-    <t>S.Ravindra Babu/ADM_Commissioner_1</t>
-  </si>
-  <si>
-    <t>engineer</t>
-  </si>
-  <si>
-    <t>ENGINEERING</t>
-  </si>
-  <si>
-    <t>Assistant Engineer</t>
-  </si>
-  <si>
-    <t>C.Naresh/ENG_Assistant Engineer_4</t>
-  </si>
-  <si>
-    <t>Forward to Engineer</t>
-  </si>
-  <si>
-    <t>engineer1</t>
-  </si>
-  <si>
-    <t>A.P.Sreenivasulu/ENG_Assistant Engineer_1</t>
-  </si>
-  <si>
-    <t>accountOfficer1</t>
-  </si>
-  <si>
-    <t>ACCOUNTS</t>
-  </si>
-  <si>
-    <t>Assistant Examiner of Accounts</t>
-  </si>
-  <si>
-    <t>Hanuman Prasad ~ ACC_AEOA_1</t>
-  </si>
-  <si>
-    <t>accountOfficer2</t>
-  </si>
-  <si>
-    <t>Examiner of Accounts</t>
-  </si>
-  <si>
-    <t>D Ramachandra Reddy ~ ACC_EOA_1</t>
-  </si>
-  <si>
-    <t>accountOfficer3</t>
-  </si>
-  <si>
-    <t>D Ramachandra Reddy/ACC_EOA_1</t>
-  </si>
-  <si>
-    <t>deputyExecutiveEngineer</t>
-  </si>
-  <si>
-    <t>Deputy Executive Engineer</t>
-  </si>
-  <si>
-    <t>S.Nayab Rasool/ENG_Dy. Executive Engineer_1</t>
-  </si>
-  <si>
-    <t>propertyType</t>
-  </si>
-  <si>
-    <t>categoryOfOwnership</t>
-  </si>
-  <si>
-    <t>residentialPrivate</t>
-  </si>
-  <si>
-    <t>Residential</t>
-  </si>
-  <si>
-    <t>Private</t>
-  </si>
-  <si>
-    <t>assessmentAdditionProperty</t>
-  </si>
-  <si>
-    <t>editfloorNumber</t>
-  </si>
-  <si>
-    <t>editclassificationOfBuilding</t>
-  </si>
-  <si>
-    <t>editnatureOfUsage</t>
-  </si>
-  <si>
-    <t>editfirmName</t>
-  </si>
-  <si>
-    <t>editoccupancy</t>
-  </si>
-  <si>
-    <t>editoccupantName</t>
-  </si>
-  <si>
-    <t>editconstructionDate</t>
-  </si>
-  <si>
-    <t>editeffectiveFromDate</t>
-  </si>
-  <si>
-    <t>editunstructuredLand</t>
-  </si>
-  <si>
-    <t>editlength</t>
-  </si>
-  <si>
-    <t>editbreadth</t>
-  </si>
-  <si>
-    <t>editbuildingPermissionNumber</t>
-  </si>
-  <si>
-    <t>editbuildingPermissionDate</t>
-  </si>
-  <si>
-    <t>editplinthAreaInBuildingPlan</t>
-  </si>
-  <si>
-    <t>firstFloorAdditionaltaration</t>
-  </si>
-  <si>
-    <t>2nd Floor</t>
-  </si>
-  <si>
-    <t>Commercial</t>
-  </si>
-  <si>
-    <t>Sunil</t>
-  </si>
-  <si>
-    <t>33/22</t>
-  </si>
-  <si>
-    <t>assessmentNumber</t>
-  </si>
-  <si>
-    <t>hscNumber</t>
-  </si>
-  <si>
-    <t>connectionDate</t>
-  </si>
-  <si>
-    <t>applicantInfo</t>
-  </si>
-  <si>
-    <t>1016093906</t>
-  </si>
-  <si>
-    <t>21/11/2016</t>
-  </si>
-  <si>
-    <t>applicantInfo1</t>
-  </si>
-  <si>
-    <t>dataEntryInfo</t>
-  </si>
-  <si>
-    <t>07/01/2017</t>
-  </si>
-  <si>
-    <t>additionalConnection</t>
-  </si>
-  <si>
-    <t>1016047933</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>1/2_12.50</t>
-  </si>
-  <si>
-    <t>waterSourceType</t>
-  </si>
-  <si>
-    <t>connectionType</t>
-  </si>
-  <si>
-    <t>category</t>
-  </si>
-  <si>
-    <t>usageType</t>
-  </si>
-  <si>
-    <t>hscPipeSize</t>
-  </si>
-  <si>
-    <t>sumpCapacity</t>
-  </si>
-  <si>
-    <t>noOfPersons</t>
-  </si>
-  <si>
-    <t>reasonForAdditionalConn</t>
-  </si>
-  <si>
-    <t>connectionInfo</t>
-  </si>
-  <si>
-    <t>1016 SURFACE WATER</t>
-  </si>
-  <si>
-    <t>Non-metered</t>
-  </si>
-  <si>
-    <t>RESIDENTIALS</t>
-  </si>
-  <si>
-    <t>OYT</t>
-  </si>
-  <si>
-    <t>connectionInfo1</t>
-  </si>
-  <si>
-    <t>New Connection</t>
-  </si>
-  <si>
-    <t>changeOfUse</t>
-  </si>
-  <si>
-    <t>NON-RESIDENTIALS</t>
-  </si>
-  <si>
-    <t>Change Of Use</t>
-  </si>
-  <si>
-    <t>GENERAL</t>
-  </si>
-  <si>
-    <t>DataEntryScreen</t>
-  </si>
-  <si>
-    <t>monthlyFees</t>
-  </si>
-  <si>
-    <t>donationCharges</t>
-  </si>
-  <si>
-    <t>meterCost</t>
-  </si>
-  <si>
-    <t>meterName</t>
-  </si>
-  <si>
-    <t>meterSINo</t>
-  </si>
-  <si>
-    <t>previousReading</t>
-  </si>
-  <si>
-    <t>lastReadingDate</t>
-  </si>
-  <si>
-    <t>currentReading</t>
-  </si>
-  <si>
-    <t>feeInfo</t>
-  </si>
-  <si>
-    <t>abcd</t>
-  </si>
-  <si>
-    <t>documentNo1</t>
-  </si>
-  <si>
-    <t>documentNo2</t>
-  </si>
-  <si>
-    <t>documentNo3</t>
-  </si>
-  <si>
-    <t>documentDate1</t>
-  </si>
-  <si>
-    <t>documentDate2</t>
-  </si>
-  <si>
-    <t>documentDate3</t>
-  </si>
-  <si>
-    <t>enclosedInfo</t>
-  </si>
-  <si>
-    <t>03/12/16</t>
-  </si>
-  <si>
-    <t>fromDate</t>
-  </si>
-  <si>
-    <t>toDate</t>
-  </si>
-  <si>
-    <t>report1</t>
-  </si>
-  <si>
-    <t>06/12/2016</t>
-  </si>
-  <si>
-    <t>material</t>
-  </si>
-  <si>
-    <t>quantity</t>
-  </si>
-  <si>
-    <t>unitOfMeasurement</t>
-  </si>
-  <si>
-    <t>rate</t>
-  </si>
-  <si>
-    <t>existingDistributionPipeline</t>
-  </si>
-  <si>
-    <t>pipelineToHomeDistance</t>
-  </si>
-  <si>
-    <t>estimationCharges</t>
-  </si>
-  <si>
-    <t>inspectionInfo</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>report2</t>
-  </si>
-  <si>
-    <t>07/12/2016</t>
-  </si>
-  <si>
-    <t>10/12/2016</t>
-  </si>
-  <si>
-    <t>message1</t>
-  </si>
-  <si>
-    <t>actualMessage</t>
-  </si>
-  <si>
-    <t>message</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="211">
+  <si>
+    <t xml:space="preserve">dataName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mobileNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ownerName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emailAddress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">guardianRelation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">guardian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bimal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bimal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bimal@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Father</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reasonForCreation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extentOfSite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">occupancyCertificateNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">registrationDocNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">registrationDocDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assessmentNewProperty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEW PROPERTY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">locality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zoneNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wardNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blockNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">electionWard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">doorNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pincode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addressOne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4th colony</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zone-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Election Ward No. 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12/46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lift</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toilets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">waterTap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">electricity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">attachedBathroom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">waterHarvesting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cableConnection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">floorType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">roofType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wallType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">woodType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">defaultConstructionType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Black Stones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAMBOO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allmixing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">floorNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">classificationOfBuilding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">natureOfUsage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">firmName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">occupancy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">occupantName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">constructionDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">effectiveFromDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unstructuredLand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">breadth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buildingPermissionNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buildingPermissionDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plinthAreaInBuildingPlan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">firstFloor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1st floor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Residence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Owner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11/22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">approverDepartment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">approverDesignation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">approver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">approverRemarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">billCollector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REVENUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bill Collector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D.Khasim ~ REV_Bill Collector_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forward to bill collector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">revenueInspector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UD Revenue Inspector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P.Sadiq Hussain ~ UD RI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forward to revenue insoector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">revenueOfficer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revenue Officer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B.Veeraswamy ~ REV_Revenue Officer_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forward to revenue officer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">commissioner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADMINISTRATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commissioner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S.Ravindra Babu ~ ADM_Commissioner_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forward to commissioner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">commissioner1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S.Ravindra Babu/ADM_Commissioner_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENGINEERING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assistant Engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C.Naresh/ENG_Assistant Engineer_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forward to Engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">engineer1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A.P.Sreenivasulu/ENG_Assistant Engineer_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accountOfficer1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACCOUNTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assistant Examiner of Accounts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hanuman Prasad ~ ACC_AEOA_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accountOfficer1a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K.Mohammed Juneed ~ ACC_AEOA_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accountOfficer2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Examiner of Accounts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D Ramachandra Reddy ~ ACC_EOA_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accountOfficer3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D Ramachandra Reddy/ACC_EOA_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deputyExecutiveEngineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deputy Executive Engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S.Nayab Rasool/ENG_Dy. Executive Engineer_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">propertyType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">categoryOfOwnership</t>
+  </si>
+  <si>
+    <t xml:space="preserve">residentialPrivate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Residential</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Private</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assessmentAdditionProperty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editfloorNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editclassificationOfBuilding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editnatureOfUsage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editfirmName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editoccupancy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editoccupantName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editconstructionDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editeffectiveFromDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editunstructuredLand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editlength</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editbreadth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editbuildingPermissionNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editbuildingPermissionDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editplinthAreaInBuildingPlan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">firstFloorAdditionaltaration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2nd Floor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commercial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sunil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33/22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assessmentNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hscNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">connectionDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">applicantInfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1016093906</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21/11/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">applicantInfo1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dataEntryInfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07/01/2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">additionalConnection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1016047933</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/2_12.50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">waterSourceType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">connectionType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">usageType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hscPipeSize</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sumpCapacity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">noOfPersons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reasonForAdditionalConn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">connectionInfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1016 SURFACE WATER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-metered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESIDENTIALS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OYT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">connectionInfo1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Connection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">changeOfUse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NON-RESIDENTIALS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change Of Use</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GENERAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DataEntryScreen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">monthlyFees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">donationCharges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meterCost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meterName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meterSINo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">previousReading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lastReadingDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">currentReading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">feeInfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abcd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">documentNo1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">documentNo2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">documentNo3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">documentDate1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">documentDate2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">documentDate3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enclosedInfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03/12/16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fromDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">report1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06/12/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">material</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unitOfMeasurement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">existingDistributionPipeline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pipelineToHomeDistance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estimationCharges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inspectionInfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">report2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07/12/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10/12/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">message1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">actualMessage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">message</t>
   </si>
 </sst>
 </file>
@@ -666,7 +677,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
     <numFmt numFmtId="167" formatCode="0.00"/>
@@ -827,18 +838,18 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.6037037037037"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.4"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.6037037037037"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="27.9296296296296"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.9888888888889"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="28.6148148148148"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -893,7 +904,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -914,14 +925,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="51.0555555555556"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.2074074074074"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="9.9962962962963"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.6555555555556"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="9.9962962962963"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="26.262962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.4259259259259"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.2444444444444"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="26.9481481481481"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="10.1925925925926"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -929,54 +940,54 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>65</v>
@@ -988,10 +999,10 @@
         <v>67</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="H2" s="3" t="n">
         <v>42319</v>
@@ -1009,7 +1020,7 @@
         <v>20</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="N2" s="3" t="n">
         <v>42358</v>
@@ -1021,7 +1032,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -1042,11 +1053,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.9851851851852"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="29.9851851851852"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="26.262962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="35.5703703703704"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.7703703703704"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="30.7703703703704"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="26.9481481481481"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="36.4555555555556"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.3888888888889"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1054,32 +1065,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>98765</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>1016039599</v>
@@ -1093,7 +1104,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>1016093176</v>
@@ -1102,27 +1113,27 @@
         <v>5626</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -1143,71 +1154,71 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="38.3148148148148"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.3"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.2259259259259"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.7333333333333"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.8148148148148"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.1666666666667"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.2259259259259"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.3037037037037"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="38.3148148148148"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="39.2962962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.9851851851852"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.7148148148148"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.2259259259259"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.2074074074074"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.7148148148148"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.8888888888889"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="39.2962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="10.3888888888889"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>20</v>
@@ -1221,25 +1232,25 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>161</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>163</v>
-      </c>
       <c r="E3" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>25</v>
@@ -1248,21 +1259,21 @@
         <v>4</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>19</v>
@@ -1271,30 +1282,30 @@
         <v>2</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>25</v>
@@ -1303,13 +1314,13 @@
         <v>4</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -1330,14 +1341,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="21.1666666666667"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.262962962963"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="20.6777777777778"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.1666666666667"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.3407407407407"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.537037037037"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="28.1259259259259"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.9481481481481"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="21.1666666666667"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.9296296296296"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.1259259259259"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="28.8111111111111"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.3888888888889"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1345,33 +1356,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1000</v>
@@ -1383,7 +1394,7 @@
         <v>100</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>1234</v>
@@ -1401,7 +1412,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -1422,14 +1433,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.7148148148148"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.3037037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.3222222222222"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.4"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.6148148148148"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.537037037037"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.9481481481481"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.3037037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.8888888888889"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.8111111111111"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.9888888888889"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.3"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.1259259259259"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.537037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.3888888888889"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1437,27 +1448,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>123</v>
@@ -1469,19 +1480,19 @@
         <v>789</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -1502,10 +1513,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.0666666666667"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.8888888888889"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.4777777777778"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.7518518518519"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.4777777777778"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.0666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.3888888888889"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1513,27 +1524,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -1554,15 +1565,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="11" width="21.1666666666667"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="11" width="18.8148148148148"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="11" width="34.0037037037037"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="11" width="10.3888888888889"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="41.2555555555556"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="11" width="39.1"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="11" width="32.437037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="11" width="14.3074074074074"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="11" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="11" width="19.2074074074074"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="11" width="34.7888888888889"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="11" width="10.5851851851852"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="42.3333333333333"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="11" width="40.0777777777778"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="11" width="33.2185185185185"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="11" width="14.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1570,39 +1581,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C2" s="13" t="n">
         <v>10</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="E2" s="13" t="n">
         <v>100</v>
@@ -1620,7 +1631,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -1641,10 +1652,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.2074074074074"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.6777777777778"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.8148148148148"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.6962962962963"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.1666666666667"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.2074074074074"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.9962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1652,27 +1663,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -1693,9 +1704,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.5592592592593"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.9518518518519"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.1925925925926"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1703,21 +1714,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -1738,13 +1749,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.2740740740741"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.9851851851852"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.1851851851852"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.7222222222222"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="38.3148148148148"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.0222222222222"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.2555555555556"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.7703703703704"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.9"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="39.2962962962963"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.8074074074074"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1790,7 +1801,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1811,13 +1822,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.6037037037037"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="21.1666666666667"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.2444444444444"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.437037037037"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="4" width="21.1666666666667"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.7333333333333"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.2185185185185"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="4" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1869,7 +1880,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1890,7 +1901,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1955,7 +1966,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1976,8 +1987,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.2740740740741"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.2555555555556"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2017,7 +2028,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2038,21 +2049,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.6037037037037"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1666666666667"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.2185185185185"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.4"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="9.6037037037037"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.8888888888889"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.5148148148148"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="30.1814814814815"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="29.3"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.9962962962963"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.2481481481481"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="44.3925925925926"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="38.3148148148148"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="40.2740740740741"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.1"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.9888888888889"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="9.8"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.4777777777778"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.2037037037037"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="30.9666666666667"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="29.9851851851852"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.1925925925926"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.4444444444444"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="45.4703703703704"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="39.2962962962963"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="41.2555555555556"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="9.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2152,7 +2163,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2165,20 +2176,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.9481481481481"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.5925925925926"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.6259259259259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="66.8333333333333"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="44.1962962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.537037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.4740740740741"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.7037037037037"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="68.4962962962963"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.2740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2335,25 +2346,25 @@
       <c r="A10" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>103</v>
       </c>
       <c r="C10" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="0" t="s">
         <v>107</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>103</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>110</v>
@@ -2361,53 +2372,67 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>103</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>89</v>
+        <v>111</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>103</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="B14" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B15" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>113</v>
+      <c r="C15" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2428,10 +2453,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.6148148148148"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.2444444444444"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.8666666666667"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.3"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.7333333333333"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.7481481481481"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2439,27 +2464,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2480,10 +2505,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="45.1740740740741"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.9481481481481"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="48.9"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.9962962962963"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.3518518518519"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.537037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.0740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.1925925925926"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2499,7 +2524,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>5000</v>
@@ -2511,7 +2536,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
[PHOENIX-5871] updated transfer of ownership feature
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="ownerDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,650 +26,715 @@
     <sheet name="fieldInseptionDetailsForWaterConnection" sheetId="16" state="visible" r:id="rId17"/>
     <sheet name="ptReport" sheetId="17" state="visible" r:id="rId18"/>
     <sheet name="dataFromWeb" sheetId="18" state="visible" r:id="rId19"/>
+    <sheet name="registrationDetails" sheetId="19" state="visible" r:id="rId20"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="211">
-  <si>
-    <t xml:space="preserve">dataName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mobileNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ownerName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">emailAddress</t>
-  </si>
-  <si>
-    <t xml:space="preserve">guardianRelation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">guardian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bimal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bimal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Male</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bimal@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Father</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ram</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reasonForCreation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">extentOfSite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">occupancyCertificateNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">registrationDocNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">registrationDocDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assessmentNewProperty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NEW PROPERTY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">locality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">zoneNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wardNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">blockNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">electionWard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">doorNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pincode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">addressOne</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4th colony</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zone-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Election Ward No. 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12/46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lift</t>
-  </si>
-  <si>
-    <t xml:space="preserve">toilets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">waterTap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">electricity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">attachedBathroom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">waterHarvesting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cableConnection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">all</t>
-  </si>
-  <si>
-    <t xml:space="preserve">floorType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">roofType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wallType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">woodType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">defaultConstructionType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Black Stones</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Absheet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BAMBOO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allmixing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">floorNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">classificationOfBuilding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">natureOfUsage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">firmName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">occupancy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">occupantName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">constructionDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">effectiveFromDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unstructuredLand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">length</t>
-  </si>
-  <si>
-    <t xml:space="preserve">breadth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">buildingPermissionNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">buildingPermissionDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plinthAreaInBuildingPlan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">firstFloor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1st floor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Huts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Residence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Owner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11/22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">approverDepartment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">approverDesignation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">approver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">approverRemarks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">billCollector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REVENUE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bill Collector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D.Khasim ~ REV_Bill Collector_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forward to bill collector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">revenueInspector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UD Revenue Inspector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P.Sadiq Hussain ~ UD RI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forward to revenue insoector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">revenueOfficer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revenue Officer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B.Veeraswamy ~ REV_Revenue Officer_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forward to revenue officer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">commissioner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADMINISTRATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Commissioner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S.Ravindra Babu ~ ADM_Commissioner_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forward to commissioner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">commissioner1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S.Ravindra Babu/ADM_Commissioner_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">engineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENGINEERING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assistant Engineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C.Naresh/ENG_Assistant Engineer_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forward to Engineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">engineer1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A.P.Sreenivasulu/ENG_Assistant Engineer_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">accountOfficer1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACCOUNTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assistant Examiner of Accounts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hanuman Prasad ~ ACC_AEOA_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">accountOfficer1a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K.Mohammed Juneed ~ ACC_AEOA_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">accountOfficer2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Examiner of Accounts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D Ramachandra Reddy ~ ACC_EOA_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">accountOfficer3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D Ramachandra Reddy/ACC_EOA_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deputyExecutiveEngineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Deputy Executive Engineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S.Nayab Rasool/ENG_Dy. Executive Engineer_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">propertyType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">categoryOfOwnership</t>
-  </si>
-  <si>
-    <t xml:space="preserve">residentialPrivate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Residential</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Private</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assessmentAdditionProperty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editfloorNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editclassificationOfBuilding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editnatureOfUsage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editfirmName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editoccupancy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editoccupantName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editconstructionDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editeffectiveFromDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editunstructuredLand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editlength</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editbreadth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editbuildingPermissionNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editbuildingPermissionDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">editplinthAreaInBuildingPlan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">firstFloorAdditionaltaration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2nd Floor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Commercial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sunil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33/22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">assessmentNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hscNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">connectionDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">applicantInfo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1016093906</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21/11/2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">applicantInfo1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dataEntryInfo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07/01/2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">additionalConnection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1016047933</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1/2_12.50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">waterSourceType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">connectionType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">usageType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hscPipeSize</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sumpCapacity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">noOfPersons</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reasonForAdditionalConn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">connectionInfo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1016 SURFACE WATER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-metered</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RESIDENTIALS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OYT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">connectionInfo1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New Connection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">changeOfUse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NON-RESIDENTIALS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Change Of Use</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GENERAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DataEntryScreen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">monthlyFees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">donationCharges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">meterCost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">meterName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">meterSINo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">previousReading</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lastReadingDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">currentReading</t>
-  </si>
-  <si>
-    <t xml:space="preserve">feeInfo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abcd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">documentNo1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">documentNo2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">documentNo3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">documentDate1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">documentDate2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">documentDate3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">enclosedInfo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">03/12/16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fromDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">toDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">report1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06/12/2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">material</t>
-  </si>
-  <si>
-    <t xml:space="preserve">quantity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unitOfMeasurement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">existingDistributionPipeline</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pipelineToHomeDistance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">estimationCharges</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inspectionInfo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">report2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07/12/2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10/12/2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">message1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">actualMessage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">message</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="234">
+  <si>
+    <t>dataName</t>
+  </si>
+  <si>
+    <t>mobileNumber</t>
+  </si>
+  <si>
+    <t>ownerName</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>emailAddress</t>
+  </si>
+  <si>
+    <t>guardianRelation</t>
+  </si>
+  <si>
+    <t>guardian</t>
+  </si>
+  <si>
+    <t>bimal</t>
+  </si>
+  <si>
+    <t>Bimal</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>bimal@gmail.com</t>
+  </si>
+  <si>
+    <t>Father</t>
+  </si>
+  <si>
+    <t>Ram</t>
+  </si>
+  <si>
+    <t>reasonForCreation</t>
+  </si>
+  <si>
+    <t>extentOfSite</t>
+  </si>
+  <si>
+    <t>occupancyCertificateNumber</t>
+  </si>
+  <si>
+    <t>registrationDocNumber</t>
+  </si>
+  <si>
+    <t>registrationDocDate</t>
+  </si>
+  <si>
+    <t>assessmentNewProperty</t>
+  </si>
+  <si>
+    <t>NEW PROPERTY</t>
+  </si>
+  <si>
+    <t>locality</t>
+  </si>
+  <si>
+    <t>zoneNumber</t>
+  </si>
+  <si>
+    <t>wardNumber</t>
+  </si>
+  <si>
+    <t>blockNumber</t>
+  </si>
+  <si>
+    <t>electionWard</t>
+  </si>
+  <si>
+    <t>doorNumber</t>
+  </si>
+  <si>
+    <t>pincode</t>
+  </si>
+  <si>
+    <t>addressOne</t>
+  </si>
+  <si>
+    <t>4th colony</t>
+  </si>
+  <si>
+    <t>Zone-1</t>
+  </si>
+  <si>
+    <t>Election Ward No. 1</t>
+  </si>
+  <si>
+    <t>12/46</t>
+  </si>
+  <si>
+    <t>lift</t>
+  </si>
+  <si>
+    <t>toilets</t>
+  </si>
+  <si>
+    <t>waterTap</t>
+  </si>
+  <si>
+    <t>electricity</t>
+  </si>
+  <si>
+    <t>attachedBathroom</t>
+  </si>
+  <si>
+    <t>waterHarvesting</t>
+  </si>
+  <si>
+    <t>cableConnection</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>floorType</t>
+  </si>
+  <si>
+    <t>roofType</t>
+  </si>
+  <si>
+    <t>wallType</t>
+  </si>
+  <si>
+    <t>woodType</t>
+  </si>
+  <si>
+    <t>defaultConstructionType</t>
+  </si>
+  <si>
+    <t>Black Stones</t>
+  </si>
+  <si>
+    <t>Absheet</t>
+  </si>
+  <si>
+    <t>BAMBOO</t>
+  </si>
+  <si>
+    <t>Allmixing</t>
+  </si>
+  <si>
+    <t>floorNumber</t>
+  </si>
+  <si>
+    <t>classificationOfBuilding</t>
+  </si>
+  <si>
+    <t>natureOfUsage</t>
+  </si>
+  <si>
+    <t>firmName</t>
+  </si>
+  <si>
+    <t>occupancy</t>
+  </si>
+  <si>
+    <t>occupantName</t>
+  </si>
+  <si>
+    <t>constructionDate</t>
+  </si>
+  <si>
+    <t>effectiveFromDate</t>
+  </si>
+  <si>
+    <t>unstructuredLand</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>breadth</t>
+  </si>
+  <si>
+    <t>buildingPermissionNumber</t>
+  </si>
+  <si>
+    <t>buildingPermissionDate</t>
+  </si>
+  <si>
+    <t>plinthAreaInBuildingPlan</t>
+  </si>
+  <si>
+    <t>firstFloor</t>
+  </si>
+  <si>
+    <t>1st floor</t>
+  </si>
+  <si>
+    <t>Huts</t>
+  </si>
+  <si>
+    <t>Residence</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>11/22</t>
+  </si>
+  <si>
+    <t>approverDepartment</t>
+  </si>
+  <si>
+    <t>approverDesignation</t>
+  </si>
+  <si>
+    <t>approver</t>
+  </si>
+  <si>
+    <t>approverRemarks</t>
+  </si>
+  <si>
+    <t>billCollector</t>
+  </si>
+  <si>
+    <t>REVENUE</t>
+  </si>
+  <si>
+    <t>Bill Collector</t>
+  </si>
+  <si>
+    <t>D.Khasim ~ REV_Bill Collector_1</t>
+  </si>
+  <si>
+    <t>Forward to bill collector</t>
+  </si>
+  <si>
+    <t>revenueInspector</t>
+  </si>
+  <si>
+    <t>UD Revenue Inspector</t>
+  </si>
+  <si>
+    <t>P.Sadiq Hussain ~ UD RI</t>
+  </si>
+  <si>
+    <t>Forward to revenue insoector</t>
+  </si>
+  <si>
+    <t>revenueOfficer</t>
+  </si>
+  <si>
+    <t>Revenue Officer</t>
+  </si>
+  <si>
+    <t>B.Veeraswamy ~ REV_Revenue Officer_3</t>
+  </si>
+  <si>
+    <t>Forward to revenue officer</t>
+  </si>
+  <si>
+    <t>commissioner</t>
+  </si>
+  <si>
+    <t>ADMINISTRATION</t>
+  </si>
+  <si>
+    <t>Commissioner</t>
+  </si>
+  <si>
+    <t>S.Ravindra Babu ~ ADM_Commissioner_1</t>
+  </si>
+  <si>
+    <t>Forward to commissioner</t>
+  </si>
+  <si>
+    <t>commissioner1</t>
+  </si>
+  <si>
+    <t>S.Ravindra Babu/ADM_Commissioner_1</t>
+  </si>
+  <si>
+    <t>engineer</t>
+  </si>
+  <si>
+    <t>ENGINEERING</t>
+  </si>
+  <si>
+    <t>Assistant Engineer</t>
+  </si>
+  <si>
+    <t>C.Naresh/ENG_Assistant Engineer_4</t>
+  </si>
+  <si>
+    <t>Forward to Engineer</t>
+  </si>
+  <si>
+    <t>engineer1</t>
+  </si>
+  <si>
+    <t>A.P.Sreenivasulu/ENG_Assistant Engineer_1</t>
+  </si>
+  <si>
+    <t>accountOfficer1</t>
+  </si>
+  <si>
+    <t>ACCOUNTS</t>
+  </si>
+  <si>
+    <t>Assistant Examiner of Accounts</t>
+  </si>
+  <si>
+    <t>Hanuman Prasad ~ ACC_AEOA_1</t>
+  </si>
+  <si>
+    <t>accountOfficer1a</t>
+  </si>
+  <si>
+    <t>K.Mohammed Juneed ~ ACC_AEOA_1</t>
+  </si>
+  <si>
+    <t>accountOfficer2</t>
+  </si>
+  <si>
+    <t>Examiner of Accounts</t>
+  </si>
+  <si>
+    <t>D Ramachandra Reddy ~ ACC_EOA_1</t>
+  </si>
+  <si>
+    <t>accountOfficer3</t>
+  </si>
+  <si>
+    <t>D Ramachandra Reddy/ACC_EOA_1</t>
+  </si>
+  <si>
+    <t>deputyExecutiveEngineer</t>
+  </si>
+  <si>
+    <t>Deputy Executive Engineer</t>
+  </si>
+  <si>
+    <t>S.Nayab Rasool/ENG_Dy. Executive Engineer_1</t>
+  </si>
+  <si>
+    <t>propertyType</t>
+  </si>
+  <si>
+    <t>categoryOfOwnership</t>
+  </si>
+  <si>
+    <t>residentialPrivate</t>
+  </si>
+  <si>
+    <t>Residential</t>
+  </si>
+  <si>
+    <t>Private</t>
+  </si>
+  <si>
+    <t>assessmentAdditionProperty</t>
+  </si>
+  <si>
+    <t>editfloorNumber</t>
+  </si>
+  <si>
+    <t>editclassificationOfBuilding</t>
+  </si>
+  <si>
+    <t>editnatureOfUsage</t>
+  </si>
+  <si>
+    <t>editfirmName</t>
+  </si>
+  <si>
+    <t>editoccupancy</t>
+  </si>
+  <si>
+    <t>editoccupantName</t>
+  </si>
+  <si>
+    <t>editconstructionDate</t>
+  </si>
+  <si>
+    <t>editeffectiveFromDate</t>
+  </si>
+  <si>
+    <t>editunstructuredLand</t>
+  </si>
+  <si>
+    <t>editlength</t>
+  </si>
+  <si>
+    <t>editbreadth</t>
+  </si>
+  <si>
+    <t>editbuildingPermissionNumber</t>
+  </si>
+  <si>
+    <t>editbuildingPermissionDate</t>
+  </si>
+  <si>
+    <t>editplinthAreaInBuildingPlan</t>
+  </si>
+  <si>
+    <t>firstFloorAdditionaltaration</t>
+  </si>
+  <si>
+    <t>2nd Floor</t>
+  </si>
+  <si>
+    <t>Commercial</t>
+  </si>
+  <si>
+    <t>Sunil</t>
+  </si>
+  <si>
+    <t>33/22</t>
+  </si>
+  <si>
+    <t>assessmentNumber</t>
+  </si>
+  <si>
+    <t>hscNumber</t>
+  </si>
+  <si>
+    <t>connectionDate</t>
+  </si>
+  <si>
+    <t>applicantInfo</t>
+  </si>
+  <si>
+    <t>1016093906</t>
+  </si>
+  <si>
+    <t>21/11/2016</t>
+  </si>
+  <si>
+    <t>applicantInfo1</t>
+  </si>
+  <si>
+    <t>dataEntryInfo</t>
+  </si>
+  <si>
+    <t>07/01/2017</t>
+  </si>
+  <si>
+    <t>additionalConnection</t>
+  </si>
+  <si>
+    <t>1016047933</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1/2_12.50</t>
+  </si>
+  <si>
+    <t>waterSourceType</t>
+  </si>
+  <si>
+    <t>connectionType</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>usageType</t>
+  </si>
+  <si>
+    <t>hscPipeSize</t>
+  </si>
+  <si>
+    <t>sumpCapacity</t>
+  </si>
+  <si>
+    <t>noOfPersons</t>
+  </si>
+  <si>
+    <t>reasonForAdditionalConn</t>
+  </si>
+  <si>
+    <t>connectionInfo</t>
+  </si>
+  <si>
+    <t>1016 SURFACE WATER</t>
+  </si>
+  <si>
+    <t>Non-metered</t>
+  </si>
+  <si>
+    <t>RESIDENTIALS</t>
+  </si>
+  <si>
+    <t>OYT</t>
+  </si>
+  <si>
+    <t>connectionInfo1</t>
+  </si>
+  <si>
+    <t>New Connection</t>
+  </si>
+  <si>
+    <t>changeOfUse</t>
+  </si>
+  <si>
+    <t>NON-RESIDENTIALS</t>
+  </si>
+  <si>
+    <t>Change Of Use</t>
+  </si>
+  <si>
+    <t>GENERAL</t>
+  </si>
+  <si>
+    <t>DataEntryScreen</t>
+  </si>
+  <si>
+    <t>monthlyFees</t>
+  </si>
+  <si>
+    <t>donationCharges</t>
+  </si>
+  <si>
+    <t>meterCost</t>
+  </si>
+  <si>
+    <t>meterName</t>
+  </si>
+  <si>
+    <t>meterSINo</t>
+  </si>
+  <si>
+    <t>previousReading</t>
+  </si>
+  <si>
+    <t>lastReadingDate</t>
+  </si>
+  <si>
+    <t>currentReading</t>
+  </si>
+  <si>
+    <t>feeInfo</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>documentNo1</t>
+  </si>
+  <si>
+    <t>documentNo2</t>
+  </si>
+  <si>
+    <t>documentNo3</t>
+  </si>
+  <si>
+    <t>documentDate1</t>
+  </si>
+  <si>
+    <t>documentDate2</t>
+  </si>
+  <si>
+    <t>documentDate3</t>
+  </si>
+  <si>
+    <t>enclosedInfo</t>
+  </si>
+  <si>
+    <t>03/12/16</t>
+  </si>
+  <si>
+    <t>fromDate</t>
+  </si>
+  <si>
+    <t>toDate</t>
+  </si>
+  <si>
+    <t>report1</t>
+  </si>
+  <si>
+    <t>06/12/2016</t>
+  </si>
+  <si>
+    <t>material</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>unitOfMeasurement</t>
+  </si>
+  <si>
+    <t>rate</t>
+  </si>
+  <si>
+    <t>existingDistributionPipeline</t>
+  </si>
+  <si>
+    <t>pipelineToHomeDistance</t>
+  </si>
+  <si>
+    <t>estimationCharges</t>
+  </si>
+  <si>
+    <t>inspectionInfo</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>report2</t>
+  </si>
+  <si>
+    <t>07/12/2016</t>
+  </si>
+  <si>
+    <t>10/12/2016</t>
+  </si>
+  <si>
+    <t>message1</t>
+  </si>
+  <si>
+    <t>actualMessage</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>sellerExecutantName</t>
+  </si>
+  <si>
+    <t>buyerClaimantName</t>
+  </si>
+  <si>
+    <t>doorNo</t>
+  </si>
+  <si>
+    <t>propertyAddress</t>
+  </si>
+  <si>
+    <t>registeredPlotArea</t>
+  </si>
+  <si>
+    <t>registeredPlinthArea </t>
+  </si>
+  <si>
+    <t>eastBoundary</t>
+  </si>
+  <si>
+    <t>westBoundary</t>
+  </si>
+  <si>
+    <t>northBoundary</t>
+  </si>
+  <si>
+    <t>southBoundary</t>
+  </si>
+  <si>
+    <t>sROName</t>
+  </si>
+  <si>
+    <t>reasonforTransfer</t>
+  </si>
+  <si>
+    <t>registrationDocumentNumber</t>
+  </si>
+  <si>
+    <t>registrationDocumentDate</t>
+  </si>
+  <si>
+    <t>partiesConsiderationValue</t>
+  </si>
+  <si>
+    <t>departmentGuidelinesValue </t>
+  </si>
+  <si>
+    <t>register</t>
+  </si>
+  <si>
+    <t>Nadir</t>
+  </si>
+  <si>
+    <t>Bangalore</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Sro</t>
+  </si>
+  <si>
+    <t>Gift Deed</t>
+  </si>
+  <si>
+    <t>12/12/2016</t>
   </si>
 </sst>
 </file>
@@ -677,7 +742,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
     <numFmt numFmtId="167" formatCode="0.00"/>
@@ -762,7 +827,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -819,6 +884,14 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -839,7 +912,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -904,7 +977,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -920,7 +993,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1032,7 +1105,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -1047,7 +1120,7 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1133,7 +1206,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -1148,8 +1221,8 @@
   </sheetPr>
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1320,7 +1393,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -1412,7 +1485,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -1492,7 +1565,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -1544,7 +1617,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -1631,7 +1704,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -1646,7 +1719,7 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1683,7 +1756,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -1699,7 +1772,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1728,7 +1801,154 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:Q2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3185185185185"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.2962962962963"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.9518518518519"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36296296296296"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.3185185185185"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.737037037037"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.5481481481481"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.4074074074074"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.1"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.0074074074074"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.337037037037"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.3888888888889"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.4296296296296"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="24.7074074074074"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="22.2888888888889"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="21.7814814814815"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="25.1111111111111"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="8.36296296296296"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="N2" s="15" t="n">
+        <v>121</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="P2" s="1" t="n">
+        <v>500000</v>
+      </c>
+      <c r="Q2" s="15" t="n">
+        <v>900000</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -1801,7 +2021,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1880,7 +2100,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1966,7 +2186,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1982,7 +2202,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
@@ -2028,7 +2248,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2163,7 +2383,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2178,8 +2398,8 @@
   </sheetPr>
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16"/>
@@ -2432,7 +2652,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2484,7 +2704,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2499,8 +2719,8 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2536,7 +2756,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
[PHOENIX-6060] updated create revision petition
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="19"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="ownerDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,13 +28,14 @@
     <sheet name="dataFromWeb" sheetId="18" state="visible" r:id="rId19"/>
     <sheet name="registrationDetails" sheetId="19" state="visible" r:id="rId20"/>
     <sheet name="searchDetails" sheetId="20" state="visible" r:id="rId21"/>
+    <sheet name="revisionPetitionDetails" sheetId="21" state="visible" r:id="rId22"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="253">
   <si>
     <t>dataName</t>
   </si>
@@ -784,6 +785,15 @@
   </si>
   <si>
     <t>Revenue Ward No 87</t>
+  </si>
+  <si>
+    <t>revisionPetitionDetails</t>
+  </si>
+  <si>
+    <t>revisionpetitionBlock</t>
+  </si>
+  <si>
+    <t>Revision Started</t>
   </si>
 </sst>
 </file>
@@ -802,6 +812,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -843,6 +854,7 @@
       <sz val="9"/>
       <name val="Courier New"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -891,7 +903,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -952,11 +964,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -968,8 +976,16 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1423,9 +1439,12 @@
       <c r="A4" s="1" t="s">
         <v>174</v>
       </c>
+      <c r="B4" s="0"/>
+      <c r="C4" s="0"/>
       <c r="D4" s="1" t="s">
         <v>175</v>
       </c>
+      <c r="E4" s="0"/>
       <c r="F4" s="1" t="s">
         <v>124</v>
       </c>
@@ -1734,6 +1753,7 @@
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="43.9642857142857"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="36.4387755102041"/>
     <col collapsed="false" hidden="false" max="257" min="9" style="1" width="16.0204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2128,29 +2148,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="15" width="28.0612244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="16" width="20.0051020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.0612244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="15" width="20.0051020408163"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="18" t="s">
         <v>241</v>
       </c>
       <c r="B2" s="19" t="n">
@@ -2158,41 +2178,87 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="18" t="s">
         <v>242</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="19" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="18" t="s">
         <v>244</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="19" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="18" t="s">
         <v>246</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="19" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="18" t="s">
         <v>248</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="19" t="s">
         <v>249</v>
       </c>
     </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.1989795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="18.8877551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>252</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2435,10 +2501,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2555,6 +2621,7 @@
         <v>30</v>
       </c>
     </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2737,6 +2804,7 @@
       <c r="D9" s="1" t="s">
         <v>105</v>
       </c>
+      <c r="E9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
@@ -2751,6 +2819,7 @@
       <c r="D10" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="E10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
@@ -2765,6 +2834,7 @@
       <c r="D11" s="1" t="s">
         <v>110</v>
       </c>
+      <c r="E11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
@@ -2779,6 +2849,7 @@
       <c r="D12" s="1" t="s">
         <v>112</v>
       </c>
+      <c r="E12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
@@ -2793,6 +2864,7 @@
       <c r="D13" s="1" t="s">
         <v>112</v>
       </c>
+      <c r="E13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
@@ -2824,6 +2896,7 @@
       <c r="D15" s="1" t="s">
         <v>115</v>
       </c>
+      <c r="E15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">

</xml_diff>

<commit_message>
[PHOENIX-6108] Completed the Bank to Bank payment transfer scenario
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="21"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="ownerDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,787 +32,795 @@
     <sheet name="hearingDetails" sheetId="22" state="visible" r:id="rId23"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="259">
-  <si>
-    <t>dataName</t>
-  </si>
-  <si>
-    <t>mobileNumber</t>
-  </si>
-  <si>
-    <t>ownerName</t>
-  </si>
-  <si>
-    <t>gender</t>
-  </si>
-  <si>
-    <t>emailAddress</t>
-  </si>
-  <si>
-    <t>guardianRelation</t>
-  </si>
-  <si>
-    <t>guardian</t>
-  </si>
-  <si>
-    <t>bimal</t>
-  </si>
-  <si>
-    <t>Bimal</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>bimal@gmail.com</t>
-  </si>
-  <si>
-    <t>Father</t>
-  </si>
-  <si>
-    <t>Ram</t>
-  </si>
-  <si>
-    <t>reasonForCreation</t>
-  </si>
-  <si>
-    <t>extentOfSite</t>
-  </si>
-  <si>
-    <t>occupancyCertificateNumber</t>
-  </si>
-  <si>
-    <t>registrationDocNumber</t>
-  </si>
-  <si>
-    <t>registrationDocDate</t>
-  </si>
-  <si>
-    <t>assessmentNewProperty</t>
-  </si>
-  <si>
-    <t>NEW PROPERTY</t>
-  </si>
-  <si>
-    <t>locality</t>
-  </si>
-  <si>
-    <t>zoneNumber</t>
-  </si>
-  <si>
-    <t>wardNumber</t>
-  </si>
-  <si>
-    <t>blockNumber</t>
-  </si>
-  <si>
-    <t>electionWard</t>
-  </si>
-  <si>
-    <t>doorNumber</t>
-  </si>
-  <si>
-    <t>pincode</t>
-  </si>
-  <si>
-    <t>addressOne</t>
-  </si>
-  <si>
-    <t>4th colony</t>
-  </si>
-  <si>
-    <t>Zone-1</t>
-  </si>
-  <si>
-    <t>Election Ward No. 1</t>
-  </si>
-  <si>
-    <t>12/46</t>
-  </si>
-  <si>
-    <t>lift</t>
-  </si>
-  <si>
-    <t>toilets</t>
-  </si>
-  <si>
-    <t>waterTap</t>
-  </si>
-  <si>
-    <t>electricity</t>
-  </si>
-  <si>
-    <t>attachedBathroom</t>
-  </si>
-  <si>
-    <t>waterHarvesting</t>
-  </si>
-  <si>
-    <t>cableConnection</t>
-  </si>
-  <si>
-    <t>all</t>
-  </si>
-  <si>
-    <t>floorType</t>
-  </si>
-  <si>
-    <t>roofType</t>
-  </si>
-  <si>
-    <t>wallType</t>
-  </si>
-  <si>
-    <t>woodType</t>
-  </si>
-  <si>
-    <t>defaultConstructionType</t>
-  </si>
-  <si>
-    <t>Black Stones</t>
-  </si>
-  <si>
-    <t>Absheet</t>
-  </si>
-  <si>
-    <t>BAMBOO</t>
-  </si>
-  <si>
-    <t>Allmixing</t>
-  </si>
-  <si>
-    <t>floorNumber</t>
-  </si>
-  <si>
-    <t>classificationOfBuilding</t>
-  </si>
-  <si>
-    <t>natureOfUsage</t>
-  </si>
-  <si>
-    <t>firmName</t>
-  </si>
-  <si>
-    <t>occupancy</t>
-  </si>
-  <si>
-    <t>occupantName</t>
-  </si>
-  <si>
-    <t>constructionDate</t>
-  </si>
-  <si>
-    <t>effectiveFromDate</t>
-  </si>
-  <si>
-    <t>unstructuredLand</t>
-  </si>
-  <si>
-    <t>length</t>
-  </si>
-  <si>
-    <t>breadth</t>
-  </si>
-  <si>
-    <t>buildingPermissionNumber</t>
-  </si>
-  <si>
-    <t>buildingPermissionDate</t>
-  </si>
-  <si>
-    <t>plinthAreaInBuildingPlan</t>
-  </si>
-  <si>
-    <t>firstFloor</t>
-  </si>
-  <si>
-    <t>1st floor</t>
-  </si>
-  <si>
-    <t>Huts</t>
-  </si>
-  <si>
-    <t>Residence</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>Owner</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>11/22</t>
-  </si>
-  <si>
-    <t>approverDepartment</t>
-  </si>
-  <si>
-    <t>approverDesignation</t>
-  </si>
-  <si>
-    <t>approver</t>
-  </si>
-  <si>
-    <t>approverRemarks</t>
-  </si>
-  <si>
-    <t>billCollector</t>
-  </si>
-  <si>
-    <t>REVENUE</t>
-  </si>
-  <si>
-    <t>Bill Collector</t>
-  </si>
-  <si>
-    <t>D.Khasim ~ REV_Bill Collector_1</t>
-  </si>
-  <si>
-    <t>Forward to bill collector</t>
-  </si>
-  <si>
-    <t>revenueInspector</t>
-  </si>
-  <si>
-    <t>UD Revenue Inspector</t>
-  </si>
-  <si>
-    <t>P.Sadiq Hussain ~ UD RI</t>
-  </si>
-  <si>
-    <t>Forward to revenue insoector</t>
-  </si>
-  <si>
-    <t>revenueOfficer</t>
-  </si>
-  <si>
-    <t>Revenue Officer</t>
-  </si>
-  <si>
-    <t>B.Veeraswamy ~ REV_Revenue Officer_3</t>
-  </si>
-  <si>
-    <t>Forward to revenue officer</t>
-  </si>
-  <si>
-    <t>commissioner</t>
-  </si>
-  <si>
-    <t>ADMINISTRATION</t>
-  </si>
-  <si>
-    <t>Commissioner</t>
-  </si>
-  <si>
-    <t>S.Ravindra Babu ~ ADM_Commissioner_1</t>
-  </si>
-  <si>
-    <t>Forward to commissioner</t>
-  </si>
-  <si>
-    <t>commissioner1</t>
-  </si>
-  <si>
-    <t>S.Ravindra Babu/ADM_Commissioner_1</t>
-  </si>
-  <si>
-    <t>engineer</t>
-  </si>
-  <si>
-    <t>ENGINEERING</t>
-  </si>
-  <si>
-    <t>Assistant Engineer</t>
-  </si>
-  <si>
-    <t>C.Naresh/ENG_Assistant Engineer_4</t>
-  </si>
-  <si>
-    <t>Forward to Engineer</t>
-  </si>
-  <si>
-    <t>engineer1</t>
-  </si>
-  <si>
-    <t>A.P.Sreenivasulu/ENG_Assistant Engineer_1</t>
-  </si>
-  <si>
-    <t>accountOfficer1</t>
-  </si>
-  <si>
-    <t>ACCOUNTS</t>
-  </si>
-  <si>
-    <t>Assistant Examiner of Accounts</t>
-  </si>
-  <si>
-    <t>Hanuman Prasad ~ ACC_AEOA_1</t>
-  </si>
-  <si>
-    <t>accountOfficer1a</t>
-  </si>
-  <si>
-    <t>K.Mohammed Juneed ~ ACC_AEOA_1</t>
-  </si>
-  <si>
-    <t>accountOfficer2</t>
-  </si>
-  <si>
-    <t>Examiner of Accounts</t>
-  </si>
-  <si>
-    <t>D Ramachandra Reddy ~ ACC_EOA_1</t>
-  </si>
-  <si>
-    <t>accountOfficer3</t>
-  </si>
-  <si>
-    <t>D Ramachandra Reddy/ACC_EOA_1</t>
-  </si>
-  <si>
-    <t>deputyExecutiveEngineer</t>
-  </si>
-  <si>
-    <t>Deputy Executive Engineer</t>
-  </si>
-  <si>
-    <t>S.Nayab Rasool/ENG_Dy. Executive Engineer_1</t>
-  </si>
-  <si>
-    <t>sanitaryInspector</t>
-  </si>
-  <si>
-    <t>PUBLIC HEALTH AND SANITATION</t>
-  </si>
-  <si>
-    <t>Sanitary Inspector</t>
-  </si>
-  <si>
-    <t>Chandragiri Murali Krishna ~ PHS_Sanitary Inspector_1</t>
-  </si>
-  <si>
-    <t>Forward to Sanitary Inspector</t>
-  </si>
-  <si>
-    <t>propertyType</t>
-  </si>
-  <si>
-    <t>categoryOfOwnership</t>
-  </si>
-  <si>
-    <t>residentialPrivate</t>
-  </si>
-  <si>
-    <t>Residential</t>
-  </si>
-  <si>
-    <t>Private</t>
-  </si>
-  <si>
-    <t>assessmentAdditionProperty</t>
-  </si>
-  <si>
-    <t>editfloorNumber</t>
-  </si>
-  <si>
-    <t>editclassificationOfBuilding</t>
-  </si>
-  <si>
-    <t>editnatureOfUsage</t>
-  </si>
-  <si>
-    <t>editfirmName</t>
-  </si>
-  <si>
-    <t>editoccupancy</t>
-  </si>
-  <si>
-    <t>editoccupantName</t>
-  </si>
-  <si>
-    <t>editconstructionDate</t>
-  </si>
-  <si>
-    <t>editeffectiveFromDate</t>
-  </si>
-  <si>
-    <t>editunstructuredLand</t>
-  </si>
-  <si>
-    <t>editlength</t>
-  </si>
-  <si>
-    <t>editbreadth</t>
-  </si>
-  <si>
-    <t>editbuildingPermissionNumber</t>
-  </si>
-  <si>
-    <t>editbuildingPermissionDate</t>
-  </si>
-  <si>
-    <t>editplinthAreaInBuildingPlan</t>
-  </si>
-  <si>
-    <t>firstFloorAdditionaltaration</t>
-  </si>
-  <si>
-    <t>2nd Floor</t>
-  </si>
-  <si>
-    <t>Commercial</t>
-  </si>
-  <si>
-    <t>Sunil</t>
-  </si>
-  <si>
-    <t>33/22</t>
-  </si>
-  <si>
-    <t>assessmentNumber</t>
-  </si>
-  <si>
-    <t>hscNumber</t>
-  </si>
-  <si>
-    <t>connectionDate</t>
-  </si>
-  <si>
-    <t>applicantInfo</t>
-  </si>
-  <si>
-    <t>1016093906</t>
-  </si>
-  <si>
-    <t>21/11/2016</t>
-  </si>
-  <si>
-    <t>applicantInfo1</t>
-  </si>
-  <si>
-    <t>dataEntryInfo</t>
-  </si>
-  <si>
-    <t>07/01/2017</t>
-  </si>
-  <si>
-    <t>additionalConnection</t>
-  </si>
-  <si>
-    <t>1016047933</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>1/2_12.50</t>
-  </si>
-  <si>
-    <t>waterSourceType</t>
-  </si>
-  <si>
-    <t>connectionType</t>
-  </si>
-  <si>
-    <t>category</t>
-  </si>
-  <si>
-    <t>usageType</t>
-  </si>
-  <si>
-    <t>hscPipeSize</t>
-  </si>
-  <si>
-    <t>sumpCapacity</t>
-  </si>
-  <si>
-    <t>noOfPersons</t>
-  </si>
-  <si>
-    <t>reasonForAdditionalConn</t>
-  </si>
-  <si>
-    <t>connectionInfo</t>
-  </si>
-  <si>
-    <t>1016 SURFACE WATER</t>
-  </si>
-  <si>
-    <t>Non-metered</t>
-  </si>
-  <si>
-    <t>RESIDENTIALS</t>
-  </si>
-  <si>
-    <t>OYT</t>
-  </si>
-  <si>
-    <t>connectionInfo1</t>
-  </si>
-  <si>
-    <t>New Connection</t>
-  </si>
-  <si>
-    <t>changeOfUse</t>
-  </si>
-  <si>
-    <t>NON-RESIDENTIALS</t>
-  </si>
-  <si>
-    <t>Change Of Use</t>
-  </si>
-  <si>
-    <t>GENERAL</t>
-  </si>
-  <si>
-    <t>DataEntryScreen</t>
-  </si>
-  <si>
-    <t>monthlyFees</t>
-  </si>
-  <si>
-    <t>donationCharges</t>
-  </si>
-  <si>
-    <t>meterCost</t>
-  </si>
-  <si>
-    <t>meterName</t>
-  </si>
-  <si>
-    <t>meterSINo</t>
-  </si>
-  <si>
-    <t>previousReading</t>
-  </si>
-  <si>
-    <t>lastReadingDate</t>
-  </si>
-  <si>
-    <t>currentReading</t>
-  </si>
-  <si>
-    <t>feeInfo</t>
-  </si>
-  <si>
-    <t>abcd</t>
-  </si>
-  <si>
-    <t>documentNo1</t>
-  </si>
-  <si>
-    <t>documentNo2</t>
-  </si>
-  <si>
-    <t>documentNo3</t>
-  </si>
-  <si>
-    <t>documentDate1</t>
-  </si>
-  <si>
-    <t>documentDate2</t>
-  </si>
-  <si>
-    <t>documentDate3</t>
-  </si>
-  <si>
-    <t>enclosedInfo</t>
-  </si>
-  <si>
-    <t>03/12/16</t>
-  </si>
-  <si>
-    <t>fromDate</t>
-  </si>
-  <si>
-    <t>toDate</t>
-  </si>
-  <si>
-    <t>report1</t>
-  </si>
-  <si>
-    <t>06/12/2016</t>
-  </si>
-  <si>
-    <t>material</t>
-  </si>
-  <si>
-    <t>quantity</t>
-  </si>
-  <si>
-    <t>unitOfMeasurement</t>
-  </si>
-  <si>
-    <t>rate</t>
-  </si>
-  <si>
-    <t>existingDistributionPipeline</t>
-  </si>
-  <si>
-    <t>pipelineToHomeDistance</t>
-  </si>
-  <si>
-    <t>estimationCharges</t>
-  </si>
-  <si>
-    <t>inspectionInfo</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>report2</t>
-  </si>
-  <si>
-    <t>07/12/2016</t>
-  </si>
-  <si>
-    <t>10/12/2016</t>
-  </si>
-  <si>
-    <t>message1</t>
-  </si>
-  <si>
-    <t>actualMessage</t>
-  </si>
-  <si>
-    <t>message</t>
-  </si>
-  <si>
-    <t>sellerExecutantName</t>
-  </si>
-  <si>
-    <t>buyerClaimantName</t>
-  </si>
-  <si>
-    <t>doorNo</t>
-  </si>
-  <si>
-    <t>propertyAddress</t>
-  </si>
-  <si>
-    <t>registeredPlotArea</t>
-  </si>
-  <si>
-    <t>registerPlinthArea</t>
-  </si>
-  <si>
-    <t>eastBoundary</t>
-  </si>
-  <si>
-    <t>westBoundary</t>
-  </si>
-  <si>
-    <t>northBoundary</t>
-  </si>
-  <si>
-    <t>southBoundary</t>
-  </si>
-  <si>
-    <t>sroName</t>
-  </si>
-  <si>
-    <t>reasonForChange</t>
-  </si>
-  <si>
-    <t>registrationDocumentNumber</t>
-  </si>
-  <si>
-    <t>registrationDocumentDate</t>
-  </si>
-  <si>
-    <t>partiesConsiderationValue</t>
-  </si>
-  <si>
-    <t>departmentGuide</t>
-  </si>
-  <si>
-    <t>register</t>
-  </si>
-  <si>
-    <t>Nadir</t>
-  </si>
-  <si>
-    <t>Bangalore</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>Sro</t>
-  </si>
-  <si>
-    <t>Gift Deed</t>
-  </si>
-  <si>
-    <t>12/12/2016</t>
-  </si>
-  <si>
-    <t>dataRow</t>
-  </si>
-  <si>
-    <t>searchValue</t>
-  </si>
-  <si>
-    <t>searchWithAssessmentNumber</t>
-  </si>
-  <si>
-    <t>searchWithMobileNumber</t>
-  </si>
-  <si>
-    <t>0000161311</t>
-  </si>
-  <si>
-    <t>searchWithDoorNumber</t>
-  </si>
-  <si>
-    <t>87/1110-9-c</t>
-  </si>
-  <si>
-    <t>searchWithZoneNumber</t>
-  </si>
-  <si>
-    <t>Zone-15</t>
-  </si>
-  <si>
-    <t>searchWithWardNumber</t>
-  </si>
-  <si>
-    <t>Revenue Ward No 87</t>
-  </si>
-  <si>
-    <t>revisionPetitionDetails</t>
-  </si>
-  <si>
-    <t>revisionpetitionBlock</t>
-  </si>
-  <si>
-    <t>Revision Started</t>
-  </si>
-  <si>
-    <t>hearingDate</t>
-  </si>
-  <si>
-    <t>hearingTime</t>
-  </si>
-  <si>
-    <t>venue</t>
-  </si>
-  <si>
-    <t>hearingBlock</t>
-  </si>
-  <si>
-    <t>28/06/2017</t>
-  </si>
-  <si>
-    <t>9.30 AM</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="260">
+  <si>
+    <t xml:space="preserve">dataName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mobileNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ownerName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emailAddress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">guardianRelation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">guardian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bimal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bimal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bimal@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Father</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reasonForCreation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extentOfSite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">occupancyCertificateNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">registrationDocNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">registrationDocDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assessmentNewProperty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NEW PROPERTY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">locality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zoneNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wardNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blockNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">electionWard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">doorNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pincode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addressOne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4th colony</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zone-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Election Ward No. 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12/46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lift</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toilets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">waterTap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">electricity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">attachedBathroom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">waterHarvesting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cableConnection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">floorType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">roofType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wallType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">woodType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">defaultConstructionType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Black Stones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Absheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAMBOO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allmixing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">floorNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">classificationOfBuilding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">natureOfUsage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">firmName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">occupancy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">occupantName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">constructionDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">effectiveFromDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unstructuredLand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">breadth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buildingPermissionNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buildingPermissionDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plinthAreaInBuildingPlan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">firstFloor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1st floor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Residence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Owner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11/22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">approverDepartment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">approverDesignation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">approver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">approverRemarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">billCollector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REVENUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bill Collector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D.Khasim ~ REV_Bill Collector_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forward to bill collector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">revenueInspector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UD Revenue Inspector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P.Sadiq Hussain ~ UD RI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forward to revenue insoector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">revenueOfficer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revenue Officer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B.Veeraswamy ~ REV_Revenue Officer_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forward to revenue officer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">commissioner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADMINISTRATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commissioner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S.Ravindra Babu ~ ADM_Commissioner_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forward to commissioner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">commissioner1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S.Ravindra Babu/ADM_Commissioner_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENGINEERING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assistant Engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C.Naresh/ENG_Assistant Engineer_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forward to Engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">engineer1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A.P.Sreenivasulu/ENG_Assistant Engineer_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accountOfficer1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACCOUNTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assistant Examiner of Accounts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hanuman Prasad ~ ACC_AEOA_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accountOfficer1a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K.Mohammed Juneed ~ ACC_AEOA_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accountOfficer2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Examiner of Accounts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D Ramachandra Reddy ~ ACC_EOA_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accountOfficer3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D Ramachandra Reddy/ACC_EOA_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deputyExecutiveEngineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deputy Executive Engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S.Nayab Rasool/ENG_Dy. Executive Engineer_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sanitaryInspector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUBLIC HEALTH AND SANITATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sanitary Inspector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chandragiri Murali Krishna ~ PHS_Sanitary Inspector_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forward to Sanitary Inspector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">propertyType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">categoryOfOwnership</t>
+  </si>
+  <si>
+    <t xml:space="preserve">residentialPrivate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Residential</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Private</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assessmentAdditionProperty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editfloorNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editclassificationOfBuilding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editnatureOfUsage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editfirmName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editoccupancy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editoccupantName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editconstructionDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editeffectiveFromDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editunstructuredLand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editlength</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editbreadth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editbuildingPermissionNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editbuildingPermissionDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editplinthAreaInBuildingPlan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">firstFloorAdditionaltaration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2nd Floor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commercial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sunil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33/22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assessmentNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hscNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">connectionDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">applicantInfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1016093906</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21/11/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">applicantInfo1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dataEntryInfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07/01/2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">additionalConnection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1016047933</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/2_12.50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">waterSourceType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">connectionType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">usageType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hscPipeSize</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sumpCapacity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">noOfPersons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reasonForAdditionalConn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">connectionInfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1016 SURFACE WATER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-metered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESIDENTIALS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OYT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RESIDENTIAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">connectionInfo1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Connection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">changeOfUse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NON-RESIDENTIALS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change Of Use</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GENERAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DataEntryScreen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">monthlyFees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">donationCharges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meterCost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meterName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meterSINo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">previousReading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lastReadingDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">currentReading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">feeInfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abcd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">documentNo1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">documentNo2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">documentNo3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">documentDate1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">documentDate2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">documentDate3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enclosedInfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03/12/16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fromDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">report1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06/12/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">material</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unitOfMeasurement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">existingDistributionPipeline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pipelineToHomeDistance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">estimationCharges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inspectionInfo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">report2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07/12/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10/12/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">message1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">actualMessage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sellerExecutantName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buyerClaimantName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">doorNo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">propertyAddress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">registeredPlotArea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">registerPlinthArea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eastBoundary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">westBoundary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">northBoundary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">southBoundary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sroName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reasonForChange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">registrationDocumentNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">registrationDocumentDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">partiesConsiderationValue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">departmentGuide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">register</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nadir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bangalore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gift Deed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12/12/2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dataRow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">searchValue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">searchWithAssessmentNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">searchWithMobileNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000161311</t>
+  </si>
+  <si>
+    <t xml:space="preserve">searchWithDoorNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87/1110-9-c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">searchWithZoneNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zone-15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">searchWithWardNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revenue Ward No 87</t>
+  </si>
+  <si>
+    <t xml:space="preserve">revisionPetitionDetails</t>
+  </si>
+  <si>
+    <t xml:space="preserve">revisionpetitionBlock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revision Started</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hearingDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hearingTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">venue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hearingBlock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28/06/2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.30 AM</t>
   </si>
 </sst>
 </file>
@@ -820,14 +828,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YYYY"/>
     <numFmt numFmtId="167" formatCode="0.00"/>
     <numFmt numFmtId="168" formatCode="DD/MM/YY"/>
     <numFmt numFmtId="169" formatCode="HH:MM\ AM/PM"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -868,6 +876,12 @@
       <name val="DejaVu Sans Mono"/>
       <family val="3"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -923,7 +937,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -964,6 +978,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -988,11 +1006,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1042,13 +1060,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.7551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.4132653061224"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.6887755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.7551020408163"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="31.3877551020408"/>
-    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="10.7551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.7551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.1326530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="31.0459183673469"/>
+    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1103,7 +1121,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1124,15 +1142,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="57.5051020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.6071428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="11.1785714285714"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="22.6887755102041"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="24.4081632653061"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="1" width="11.1785714285714"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="29.5612244897959"/>
-    <col collapsed="false" hidden="false" max="257" min="15" style="1" width="11.1785714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="11.1785714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="56.8316326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="1" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="29.1581632653061"/>
+    <col collapsed="false" hidden="false" max="257" min="15" style="1" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.9336734693878"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1232,7 +1250,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1253,11 +1271,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="33.7551020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="29.5612244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="39.9948979591837"/>
-    <col collapsed="false" hidden="false" max="257" min="5" style="1" width="11.4030612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="11.4030612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="33.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="29.1581632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="39.5510204081633"/>
+    <col collapsed="false" hidden="false" max="257" min="5" style="1" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="11.2040816326531"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1333,7 +1351,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1348,23 +1366,23 @@
   </sheetPr>
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q24" activeCellId="0" sqref="Q24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="43.1071428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="32.8928571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="26.015306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="25.4795918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="21.0663265306122"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="26.015306122449"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="27.3061224489796"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="43.1071428571429"/>
-    <col collapsed="false" hidden="false" max="257" min="11" style="1" width="11.4030612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="11.4030612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="42.6581632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="32.3979591836735"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="42.6581632653061"/>
+    <col collapsed="false" hidden="false" max="257" min="11" style="1" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="11.2040816326531"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1415,8 +1433,8 @@
       <c r="E2" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>124</v>
+      <c r="F2" s="10" t="s">
+        <v>172</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>158</v>
@@ -1431,9 +1449,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="17.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>168</v>
@@ -1448,7 +1466,7 @@
         <v>171</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>124</v>
+        <v>172</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>158</v>
@@ -1460,21 +1478,21 @@
         <v>4</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B4" s="0"/>
       <c r="C4" s="0"/>
       <c r="D4" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E4" s="0"/>
       <c r="F4" s="1" t="s">
-        <v>124</v>
+        <v>172</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>158</v>
@@ -1486,10 +1504,10 @@
         <v>2</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>153</v>
       </c>
@@ -1500,13 +1518,13 @@
         <v>169</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>124</v>
+        <v>172</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>158</v>
@@ -1518,13 +1536,13 @@
         <v>4</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1545,15 +1563,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="29.5612244897959"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="23.219387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="30.6326530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="30.8520408163265"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="31.6071428571429"/>
-    <col collapsed="false" hidden="false" max="257" min="10" style="1" width="11.4030612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="11.4030612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="29.1581632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="30.5102040816327"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="31.1836734693878"/>
+    <col collapsed="false" hidden="false" max="257" min="10" style="1" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="11.2040816326531"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1561,33 +1579,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>1000</v>
@@ -1599,7 +1617,7 @@
         <v>100</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>1234</v>
@@ -1607,7 +1625,7 @@
       <c r="G2" s="1" t="n">
         <v>123456</v>
       </c>
-      <c r="H2" s="10" t="n">
+      <c r="H2" s="11" t="n">
         <v>42689</v>
       </c>
       <c r="I2" s="1" t="n">
@@ -1617,7 +1635,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1638,15 +1656,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.6581632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.3061224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="26.1173469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="27.4132653061224"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="32.1479591836735"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="30.8520408163265"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="30.2040816326531"/>
-    <col collapsed="false" hidden="false" max="257" min="8" style="1" width="11.4030612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="11.4030612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.3214285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="25.7857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="27.1326530612245"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="31.7244897959184"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="30.5102040816327"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="29.6989795918367"/>
+    <col collapsed="false" hidden="false" max="257" min="8" style="1" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="11.2040816326531"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1654,27 +1672,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>123</v>
@@ -1686,19 +1704,19 @@
         <v>789</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1719,11 +1737,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="29.3469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.9540816326531"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="28.5918367346939"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="11.4030612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="11.4030612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.6734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="28.2142857142857"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="11.2040816326531"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1731,27 +1749,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1772,74 +1790,74 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.0663265306122"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.1989795918367"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="38.1683673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="46.4387755102041"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="43.9642857142857"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="36.4387755102041"/>
-    <col collapsed="false" hidden="false" max="257" min="9" style="1" width="16.0204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="37.6632653061224"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="45.8979591836735"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="43.469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="35.9081632653061"/>
+    <col collapsed="false" hidden="false" max="257" min="9" style="1" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="C1" s="12" t="s">
+      <c r="B1" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="C1" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="D1" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="E1" s="13" t="s">
         <v>205</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="F1" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="G1" s="13" t="s">
         <v>207</v>
       </c>
+      <c r="H1" s="13" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>188</v>
-      </c>
-      <c r="C2" s="12" t="n">
+      <c r="A2" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="C2" s="13" t="n">
         <v>10</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>209</v>
-      </c>
-      <c r="E2" s="12" t="n">
+      <c r="D2" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="E2" s="13" t="n">
         <v>100</v>
       </c>
-      <c r="F2" s="12" t="n">
+      <c r="F2" s="13" t="n">
         <v>10</v>
       </c>
-      <c r="G2" s="11" t="n">
+      <c r="G2" s="12" t="n">
         <v>1000</v>
       </c>
-      <c r="H2" s="12" t="n">
+      <c r="H2" s="13" t="n">
         <v>1000</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1860,11 +1878,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.6071428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.219387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.0663265306122"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="10.9591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.9591836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1872,27 +1890,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1913,10 +1931,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.5918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.3469387755102"/>
-    <col collapsed="false" hidden="false" max="257" min="3" style="1" width="11.1785714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="11.1785714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="257" min="3" style="1" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.9336734693878"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1924,21 +1942,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1959,137 +1977,136 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.7040816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.5561224489796"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.6887755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.16836734693878"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.7040816326531"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.25"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.6173469387755"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="13.2755102040816"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="14.2755102040816"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="17.9183673469388"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="11.4030612244898"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="16.9285714285714"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="27.1071428571429"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="24.4489795918367"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="27.5459183673469"/>
-    <col collapsed="false" hidden="false" max="257" min="18" style="1" width="9.16836734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="9.16836734693878"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="26.7295918367347"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="257" min="18" style="1" width="9.04591836734694"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>216</v>
-      </c>
-      <c r="C1" s="13" t="s">
+      <c r="B1" s="14" t="s">
         <v>217</v>
       </c>
+      <c r="C1" s="14" t="s">
+        <v>218</v>
+      </c>
       <c r="D1" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="L1" s="13" t="s">
         <v>226</v>
       </c>
+      <c r="L1" s="14" t="s">
+        <v>227</v>
+      </c>
       <c r="M1" s="2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="F2" s="12" t="n">
+        <v>235</v>
+      </c>
+      <c r="F2" s="13" t="n">
         <v>30</v>
       </c>
-      <c r="G2" s="12" t="n">
+      <c r="G2" s="13" t="n">
         <v>20</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="N2" s="14" t="n">
+        <v>238</v>
+      </c>
+      <c r="N2" s="15" t="n">
         <v>121</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="P2" s="12" t="n">
+        <v>239</v>
+      </c>
+      <c r="P2" s="13" t="n">
         <v>500000</v>
       </c>
-      <c r="Q2" s="14" t="n">
+      <c r="Q2" s="15" t="n">
         <v>900000</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2110,14 +2127,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="45.2602040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="33.7551020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.6887755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="53.6479591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="43.1071428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="37.0867346938776"/>
-    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="10.7551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.7551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="44.6836734693878"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="33.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="53.0510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="42.6581632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2163,7 +2180,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2184,64 +2201,64 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.0612244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="15" width="20.0051020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.6734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="16" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16" t="s">
-        <v>239</v>
-      </c>
-      <c r="B1" s="17" t="s">
+      <c r="A1" s="17" t="s">
         <v>240</v>
       </c>
+      <c r="B1" s="18" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="18" t="s">
-        <v>241</v>
-      </c>
-      <c r="B2" s="19" t="n">
+      <c r="A2" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="B2" s="20" t="n">
         <v>1016063818</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="18" t="s">
-        <v>242</v>
-      </c>
-      <c r="B3" s="19" t="s">
+      <c r="A3" s="19" t="s">
         <v>243</v>
       </c>
+      <c r="B3" s="20" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="18" t="s">
-        <v>244</v>
-      </c>
-      <c r="B4" s="19" t="s">
+      <c r="A4" s="19" t="s">
         <v>245</v>
       </c>
+      <c r="B4" s="20" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="B5" s="19" t="s">
+      <c r="A5" s="19" t="s">
         <v>247</v>
       </c>
+      <c r="B5" s="20" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="18" t="s">
-        <v>248</v>
-      </c>
-      <c r="B6" s="19" t="s">
+      <c r="A6" s="19" t="s">
         <v>249</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2262,31 +2279,31 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.1989795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8877551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>239</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>250</v>
+        <v>240</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>251</v>
-      </c>
-      <c r="B2" s="18" t="s">
         <v>252</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>253</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2301,47 +2318,47 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>239</v>
-      </c>
-      <c r="B1" s="20" t="s">
-        <v>253</v>
+        <v>240</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>254</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>256</v>
-      </c>
-      <c r="B2" s="21" t="s">
         <v>257</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="B2" s="22" t="s">
         <v>258</v>
       </c>
+      <c r="C2" s="23" t="s">
+        <v>259</v>
+      </c>
       <c r="D2" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2362,14 +2379,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.7551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.3469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="24.9387755102041"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="36.4387755102041"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="257" min="8" style="1" width="10.7551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.7551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="35.9081632653061"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="257" min="8" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2421,7 +2438,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2442,8 +2459,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="10.7551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.7551020408163"/>
+    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2508,7 +2525,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2529,9 +2546,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="45.2602040816327"/>
-    <col collapsed="false" hidden="false" max="257" min="2" style="1" width="10.7551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.7551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="44.6836734693878"/>
+    <col collapsed="false" hidden="false" max="257" min="2" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2571,7 +2588,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2592,22 +2609,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.7551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="42.8928571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="27.4132653061224"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="10.7551020408163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="27.9540816326531"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="32.0357142857143"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="33.9744897959184"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="32.8928571428571"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="11.1785714285714"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.6530612244898"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="49.8724489795918"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="43.1071428571429"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="45.2602040816327"/>
-    <col collapsed="false" hidden="false" max="257" min="16" style="1" width="10.7551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.7551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="42.3877551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="27.1326530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="27.6734693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="31.5867346938776"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="33.6122448979592"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="32.3979591836735"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="49.2704081632653"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="42.6581632653061"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="44.6836734693878"/>
+    <col collapsed="false" hidden="false" max="257" min="16" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2708,7 +2725,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2729,13 +2746,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="30.2040816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="38.9132653061224"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="47.9387755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="75.1377551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="49.6581632653061"/>
-    <col collapsed="false" hidden="false" max="257" min="6" style="1" width="10.7551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.7551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="29.6989795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="38.3367346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="47.3826530612245"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="74.2448979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="49.1377551020408"/>
+    <col collapsed="false" hidden="false" max="257" min="6" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3001,7 +3018,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3022,11 +3039,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="32.1479591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.9387755102041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="40.3061224489796"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="10.7551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.7551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="31.7244897959184"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="39.8214285714286"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3054,7 +3071,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3075,11 +3092,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="50.8469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="30.2040816326531"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="54.9336734693878"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="11.1785714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="11.1785714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="50.219387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="29.6989795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="54.4030612244898"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.9336734693878"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3107,7 +3124,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
[PHOENIX-6058] Completed the search property scenario
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="ownerDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="265">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -769,9 +769,15 @@
     <t xml:space="preserve">searchValue</t>
   </si>
   <si>
+    <t xml:space="preserve">searchValue2</t>
+  </si>
+  <si>
     <t xml:space="preserve">searchWithAssessmentNumber</t>
   </si>
   <si>
+    <t xml:space="preserve">null</t>
+  </si>
+  <si>
     <t xml:space="preserve">searchWithMobileNumber</t>
   </si>
   <si>
@@ -784,16 +790,25 @@
     <t xml:space="preserve">87/1110-9-c</t>
   </si>
   <si>
-    <t xml:space="preserve">searchWithZoneNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zone-15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">searchWithWardNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revenue Ward No 87</t>
+    <t xml:space="preserve">searchWithZoneAndWardNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zone-15;Revenue Ward No  87</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87/1110-9-c;C. Naga Sailaja W/o R. Satish Kumar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">searchWithOwnerName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">revenue colony;C. Naga Sailaja W/o R. Satish Kumar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">searchByDemand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">500;501</t>
   </si>
   <si>
     <t xml:space="preserve">revisionPetitionDetails</t>
@@ -878,16 +893,17 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="9"/>
       <name val="Courier New"/>
       <family val="3"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -978,10 +994,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1006,12 +1018,16 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1060,13 +1076,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.1326530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="31.0459183673469"/>
-    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.9183673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1142,15 +1158,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="56.8316326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="1" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="29.1581632653061"/>
-    <col collapsed="false" hidden="false" max="257" min="15" style="1" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="54.8061224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="27.9438775510204"/>
+    <col collapsed="false" hidden="false" max="257" min="15" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1271,11 +1287,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="33.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="29.1581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="39.5510204081633"/>
-    <col collapsed="false" hidden="false" max="257" min="5" style="1" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="31.9948979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="27.9438775510204"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="38.0663265306122"/>
+    <col collapsed="false" hidden="false" max="257" min="5" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1366,23 +1382,23 @@
   </sheetPr>
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="42.6581632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="32.3979591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="42.6581632653061"/>
-    <col collapsed="false" hidden="false" max="257" min="11" style="1" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="41.1734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="31.1836734693878"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="41.1734693877551"/>
+    <col collapsed="false" hidden="false" max="257" min="11" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1433,7 +1449,7 @@
       <c r="E2" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="8" t="s">
         <v>172</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -1563,15 +1579,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="29.1581632653061"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="30.2397959183673"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="30.5102040816327"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="31.1836734693878"/>
-    <col collapsed="false" hidden="false" max="257" min="10" style="1" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="27.9438775510204"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="30.1020408163265"/>
+    <col collapsed="false" hidden="false" max="257" min="10" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1625,7 +1641,7 @@
       <c r="G2" s="1" t="n">
         <v>123456</v>
       </c>
-      <c r="H2" s="11" t="n">
+      <c r="H2" s="10" t="n">
         <v>42689</v>
       </c>
       <c r="I2" s="1" t="n">
@@ -1656,15 +1672,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.3214285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="25.7857142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="27.1326530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="31.7244897959184"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="30.5102040816327"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="29.6989795918367"/>
-    <col collapsed="false" hidden="false" max="257" min="8" style="1" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="25.9183673469388"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="30.5102040816327"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="257" min="8" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1737,11 +1753,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="28.8877551020408"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.6734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.7295918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1790,67 +1806,66 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="37.6632653061224"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="45.8979591836735"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="43.469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="35.9081632653061"/>
-    <col collapsed="false" hidden="false" max="257" min="9" style="1" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="36.4489795918367"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="44.1428571428571"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="41.8469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="34.5561224489796"/>
+    <col collapsed="false" hidden="false" max="257" min="9" style="1" width="15.3877551020408"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="12" t="s">
         <v>207</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="12" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>189</v>
       </c>
-      <c r="C2" s="13" t="n">
+      <c r="C2" s="12" t="n">
         <v>10</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="12" t="s">
         <v>210</v>
       </c>
-      <c r="E2" s="13" t="n">
+      <c r="E2" s="12" t="n">
         <v>100</v>
       </c>
-      <c r="F2" s="13" t="n">
+      <c r="F2" s="12" t="n">
         <v>10</v>
       </c>
-      <c r="G2" s="12" t="n">
+      <c r="G2" s="11" t="n">
         <v>1000</v>
       </c>
-      <c r="H2" s="13" t="n">
+      <c r="H2" s="12" t="n">
         <v>1000</v>
       </c>
     </row>
@@ -1878,11 +1893,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1931,10 +1946,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="257" min="3" style="1" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="257" min="3" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1977,34 +1992,35 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="26.7295918367347"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="257" min="18" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="25.515306122449"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="257" min="18" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>218</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -2031,7 +2047,7 @@
       <c r="K1" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="13" t="s">
         <v>227</v>
       </c>
       <c r="M1" s="2" t="s">
@@ -2066,10 +2082,10 @@
       <c r="E2" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="F2" s="13" t="n">
+      <c r="F2" s="12" t="n">
         <v>30</v>
       </c>
-      <c r="G2" s="13" t="n">
+      <c r="G2" s="12" t="n">
         <v>20</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -2090,16 +2106,16 @@
       <c r="M2" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="N2" s="15" t="n">
+      <c r="N2" s="14" t="n">
         <v>121</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="P2" s="13" t="n">
+      <c r="P2" s="12" t="n">
         <v>500000</v>
       </c>
-      <c r="Q2" s="15" t="n">
+      <c r="Q2" s="14" t="n">
         <v>900000</v>
       </c>
     </row>
@@ -2127,14 +2143,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="44.6836734693878"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="33.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="53.0510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="42.6581632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="36.719387755102"/>
-    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="43.0612244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="31.9948979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="51.2959183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="41.1734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="35.234693877551"/>
+    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2193,68 +2209,93 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.6734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="16" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.7295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="15" width="43.3316326530612"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.0918367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="16" t="s">
         <v>240</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>241</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="19" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B2" s="20" t="n">
         <v>1016063818</v>
       </c>
+      <c r="C2" s="0" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B3" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>246</v>
+        <v>248</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="19" t="s">
-        <v>249</v>
-      </c>
-      <c r="B6" s="20" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="C5" s="0" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2279,9 +2320,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2289,15 +2330,15 @@
         <v>240</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -2324,7 +2365,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2332,24 +2373,24 @@
         <v>240</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>235</v>
@@ -2379,14 +2420,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="24.7040816326531"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="35.9081632653061"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="257" min="8" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="34.5561224489796"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="257" min="8" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2459,8 +2500,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2546,9 +2587,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="44.6836734693878"/>
-    <col collapsed="false" hidden="false" max="257" min="2" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="43.0612244897959"/>
+    <col collapsed="false" hidden="false" max="257" min="2" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2609,22 +2650,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="42.3877551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="27.1326530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="27.6734693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="31.5867346938776"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="33.6122448979592"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="32.3979591836735"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.5"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="49.2704081632653"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="42.6581632653061"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="44.6836734693878"/>
-    <col collapsed="false" hidden="false" max="257" min="16" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="40.765306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="25.9183673469388"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="26.7295918367347"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="30.3724489795918"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="31.1836734693878"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="47.515306122449"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="41.1734693877551"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="43.0612244897959"/>
+    <col collapsed="false" hidden="false" max="257" min="16" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2746,13 +2787,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="29.6989795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="38.3367346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="47.3826530612245"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="74.2448979591837"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="49.1377551020408"/>
-    <col collapsed="false" hidden="false" max="257" min="6" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="36.9897959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="45.7602040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="71.6785714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="47.2448979591837"/>
+    <col collapsed="false" hidden="false" max="257" min="6" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3039,11 +3080,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="31.7244897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.7040816326531"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="39.8214285714286"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="30.5102040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="38.3367346938776"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3092,11 +3133,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="50.219387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="29.6989795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="54.4030612244898"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="48.5969387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="52.3775510204082"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[PHOENIX-6004] Completed the Legal Case Management Services
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="19"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="ownerDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="265">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -325,7 +325,7 @@
     <t xml:space="preserve">commissioner1</t>
   </si>
   <si>
-    <t xml:space="preserve">S.Ravindra Babu/ADM_Commissioner_1</t>
+    <t xml:space="preserve">Ravindra Babu/ADM_Commissioner_2</t>
   </si>
   <si>
     <t xml:space="preserve">engineer</t>
@@ -1076,13 +1076,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.9183673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="28.6173469387755"/>
+    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1158,15 +1158,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="54.8061224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="27.9438775510204"/>
-    <col collapsed="false" hidden="false" max="257" min="15" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="52.9183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="7" min="3" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="27.1326530612245"/>
+    <col collapsed="false" hidden="false" max="257" min="15" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1287,11 +1287,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="31.9948979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="27.9438775510204"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="38.0663265306122"/>
-    <col collapsed="false" hidden="false" max="257" min="5" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="27.1326530612245"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="257" min="5" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.2602040816327"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1388,17 +1388,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="41.1734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="31.1836734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="41.1734693877551"/>
-    <col collapsed="false" hidden="false" max="257" min="11" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="30.1020408163265"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="257" min="11" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.2602040816327"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1579,15 +1579,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="27.9438775510204"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="29.0255102040816"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="30.1020408163265"/>
-    <col collapsed="false" hidden="false" max="257" min="10" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="27.1326530612245"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="28.2142857142857"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="257" min="10" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.2602040816327"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1672,15 +1672,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="25.9183673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="30.5102040816327"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="28.484693877551"/>
-    <col collapsed="false" hidden="false" max="257" min="8" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="28.2142857142857"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="257" min="8" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.2602040816327"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1753,11 +1753,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.7295918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.515306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.2602040816327"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1806,15 +1806,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="36.4489795918367"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="44.1428571428571"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="41.8469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="34.5561224489796"/>
-    <col collapsed="false" hidden="false" max="257" min="9" style="1" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="34.9642857142857"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="42.5204081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="40.2295918367347"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="33.3418367346939"/>
+    <col collapsed="false" hidden="false" max="257" min="9" style="1" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1893,11 +1894,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1946,10 +1946,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="257" min="3" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="257" min="3" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1992,25 +1992,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="25.515306122449"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="257" min="18" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="257" min="18" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2143,14 +2143,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="43.0612244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="31.9948979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="51.2959183673469"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="41.1734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="35.234693877551"/>
-    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="41.5765306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="49.4081632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="34.0204081632653"/>
+    <col collapsed="false" hidden="false" max="257" min="7" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2211,16 +2211,16 @@
   </sheetPr>
   <dimension ref="A1:C65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.7295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="15" width="43.3316326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.0918367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.515306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="15" width="41.8469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.7448979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2320,9 +2320,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2365,7 +2365,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2420,14 +2420,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="34.5561224489796"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="257" min="8" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="33.3418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="257" min="8" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2500,8 +2500,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2587,9 +2587,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="43.0612244897959"/>
-    <col collapsed="false" hidden="false" max="257" min="2" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="41.5765306122449"/>
+    <col collapsed="false" hidden="false" max="257" min="2" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2650,22 +2650,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="40.765306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="25.9183673469388"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="26.7295918367347"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="30.3724489795918"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="32.265306122449"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="31.1836734693878"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="47.515306122449"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="41.1734693877551"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="43.0612244897959"/>
-    <col collapsed="false" hidden="false" max="257" min="16" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="39.4183673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="25.515306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="29.2908163265306"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="31.0459183673469"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="30.1020408163265"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="45.8979591836735"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="41.5765306122449"/>
+    <col collapsed="false" hidden="false" max="257" min="16" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2779,21 +2779,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="28.484693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="36.9897959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="45.7602040816327"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="71.6785714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="47.2448979591837"/>
-    <col collapsed="false" hidden="false" max="257" min="6" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="35.6377551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="44.1428571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="69.25"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="45.6275510204082"/>
+    <col collapsed="false" hidden="false" max="257" min="6" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3009,50 +3009,33 @@
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>90</v>
+        <v>96</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>114</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>92</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="E14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>114</v>
+        <v>117</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>118</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E15" s="0"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D16" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>120</v>
       </c>
     </row>
@@ -3080,11 +3063,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="30.5102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="38.3367346938776"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="36.9897959183673"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3133,11 +3116,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="48.5969387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="28.484693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="52.3775510204082"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="46.7091836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="50.6224489795918"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
[PHOENIX-5847] updated field level changes in property detail page
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/PTISTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ownerDetails" sheetId="1" state="visible" r:id="rId2"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="269">
   <si>
     <t>dataName</t>
   </si>
@@ -168,13 +168,10 @@
     <t>defaultConstructionType</t>
   </si>
   <si>
-    <t>Black Stones</t>
+    <t>BAMBOO</t>
   </si>
   <si>
     <t>Absheet</t>
-  </si>
-  <si>
-    <t>BAMBOO</t>
   </si>
   <si>
     <t>Allmixing</t>
@@ -1189,7 +1186,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>5000</v>
@@ -1238,69 +1235,69 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="H2" s="5" t="n">
         <v>42319</v>
@@ -1309,7 +1306,7 @@
         <v>42327</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K2" s="10" t="n">
         <v>10</v>
@@ -1318,7 +1315,7 @@
         <v>20</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="N2" s="5" t="n">
         <v>42358</v>
@@ -1363,32 +1360,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>155</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>98765</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>1016039599</v>
@@ -1402,7 +1399,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>1016093176</v>
@@ -1411,21 +1408,21 @@
         <v>5626</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>161</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -1467,57 +1464,57 @@
   <sheetData>
     <row r="1" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="20.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="D2" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="F2" s="9" t="s">
-        <v>177</v>
-      </c>
       <c r="G2" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H2" s="1" t="n">
         <v>20</v>
@@ -1531,25 +1528,25 @@
     </row>
     <row r="3" customFormat="false" ht="17.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H3" s="1" t="n">
         <v>25</v>
@@ -1558,24 +1555,24 @@
         <v>4</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B4" s="0"/>
       <c r="C4" s="0"/>
       <c r="D4" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E4" s="0"/>
       <c r="F4" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>19</v>
@@ -1584,30 +1581,30 @@
         <v>2</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>174</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H5" s="1" t="n">
         <v>25</v>
@@ -1616,7 +1613,7 @@
         <v>4</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -1659,33 +1656,33 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>1000</v>
@@ -1697,7 +1694,7 @@
         <v>100</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>1234</v>
@@ -1752,27 +1749,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>199</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>123</v>
@@ -1784,13 +1781,13 @@
         <v>789</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -1829,21 +1826,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>203</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>206</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -1887,39 +1884,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>212</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C2" s="6" t="n">
         <v>10</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E2" s="6" t="n">
         <v>100</v>
@@ -1970,21 +1967,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>203</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>217</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -2022,15 +2019,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -2146,69 +2143,69 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="13" t="s">
         <v>231</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="M1" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>236</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F2" s="6" t="n">
         <v>30</v>
@@ -2217,28 +2214,28 @@
         <v>20</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>242</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>243</v>
       </c>
       <c r="N2" s="6" t="n">
         <v>121</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="P2" s="6" t="n">
         <v>500000</v>
@@ -2279,73 +2276,73 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="C1" s="17" t="s">
         <v>246</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B2" s="19" t="n">
         <v>1016063818</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="B3" s="19" t="s">
         <v>250</v>
       </c>
-      <c r="B3" s="19" t="s">
-        <v>251</v>
-      </c>
       <c r="C3" s="0" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="B4" s="19" t="s">
         <v>252</v>
       </c>
-      <c r="B4" s="19" t="s">
-        <v>253</v>
-      </c>
       <c r="C4" s="0" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="18" t="s">
+        <v>253</v>
+      </c>
+      <c r="B5" s="19" t="s">
         <v>254</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="C5" s="0" t="s">
         <v>255</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="B6" s="20" t="s">
         <v>257</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="B7" s="20" t="s">
         <v>259</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2381,18 +2378,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>262</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -2424,30 +2421,30 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B1" s="21" t="s">
+        <v>263</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>264</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>265</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>267</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="C2" s="23" t="s">
         <v>268</v>
       </c>
-      <c r="C2" s="23" t="s">
-        <v>269</v>
-      </c>
       <c r="D2" s="0" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -2635,8 +2632,8 @@
   </sheetPr>
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2674,10 +2671,10 @@
         <v>44</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2732,66 +2729,66 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>8</v>
@@ -2803,7 +2800,7 @@
         <v>42654</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K2" s="1" t="n">
         <v>10</v>
@@ -2812,7 +2809,7 @@
         <v>20</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N2" s="5" t="n">
         <v>42358</v>
@@ -2839,7 +2836,7 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2857,27 +2854,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>74</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -2918,242 +2915,242 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="E8" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="C9" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="E9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="E10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>114</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>115</v>
       </c>
       <c r="E11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="E12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="E13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C14" s="9" t="s">
+      <c r="D14" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>120</v>
       </c>
       <c r="E14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3193,21 +3190,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>